<commit_message>
test-23: hybrid model (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>RF-100 (superdataset-24-f 2Y.csv + extrapol)</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
+  </si>
+  <si>
+    <t>RF-100 (superdataset-24-f 2Ysum.csv + extrapol)</t>
   </si>
 </sst>
 </file>
@@ -388,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:T57"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X48" sqref="X48"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,12 +2160,1771 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C3:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="X51" sqref="X51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7823.1866903658247</v>
+      </c>
+      <c r="E5" s="3">
+        <v>52710.215953496809</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>19988.180811262479</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>34502.219893551322</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3">
+        <v>21663.98982334241</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7660.0111798909347</v>
+      </c>
+      <c r="E6" s="3">
+        <v>55518.847043415073</v>
+      </c>
+      <c r="H6" s="2">
+        <f>H5+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>25762.852665213439</v>
+      </c>
+      <c r="M6" s="2">
+        <f>M5+1</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="3">
+        <v>25575.293685376921</v>
+      </c>
+      <c r="S6" s="2">
+        <f>S5+1</f>
+        <v>2</v>
+      </c>
+      <c r="T6" s="3">
+        <v>18599.50895286103</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7711.5818334242222</v>
+      </c>
+      <c r="E7" s="3">
+        <v>49560.706226975468</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H54" si="1">H6+1</f>
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>25352.916455949129</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:M54" si="2">M6+1</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="3">
+        <v>27527.12490572207</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" ref="S7:S54" si="3">S6+1</f>
+        <v>3</v>
+      </c>
+      <c r="T7" s="3">
+        <v>18386.542879927329</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>7762.1150897296066</v>
+      </c>
+      <c r="E8" s="3">
+        <v>52971.517823614893</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>24894.749163669389</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>21384.566414532241</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="T8" s="3">
+        <v>17922.602198092642</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7544.6509077482378</v>
+      </c>
+      <c r="E9" s="3">
+        <v>53749.129033424157</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>26957.038760762938</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N9" s="3">
+        <v>27085.683077565842</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="T9" s="3">
+        <v>19444.21708083561</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7898.2810496478069</v>
+      </c>
+      <c r="E10" s="3">
+        <v>47687.253339600356</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <v>24830.75390735695</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N10" s="3">
+        <v>28476.734489373299</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="T10" s="3">
+        <v>18654.721078383289</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7450.3752128152692</v>
+      </c>
+      <c r="E11" s="3">
+        <v>58094.200009355132</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="3">
+        <v>24969.679909173479</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N11" s="3">
+        <v>27077.582967484101</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="T11" s="3">
+        <v>23943.555937420519</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7507.2787979777322</v>
+      </c>
+      <c r="E12" s="3">
+        <v>55329.209005722063</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I12" s="3">
+        <v>22185.101828156221</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N12" s="3">
+        <v>26628.425764577649</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="T12" s="3">
+        <v>17582.05317674841</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7588.7223692797088</v>
+      </c>
+      <c r="E13" s="3">
+        <v>57686.881398455938</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="3">
+        <v>31867.699928792001</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N13" s="3">
+        <v>29405.42495404177</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="T13" s="3">
+        <v>22379.753733878289</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>7570.3558720745277</v>
+      </c>
+      <c r="E14" s="3">
+        <v>51072.729917257027</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I14" s="3">
+        <v>21240.903485921881</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N14" s="3">
+        <v>28703.283207266111</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="T14" s="3">
+        <v>17194.889912715709</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7802.6547137695979</v>
+      </c>
+      <c r="E15" s="3">
+        <v>48057.7256342416</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I15" s="3">
+        <v>21795.601074659389</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N15" s="3">
+        <v>22092.301140781099</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="T15" s="3">
+        <v>22304.639723433229</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7631.4438752329024</v>
+      </c>
+      <c r="E16" s="3">
+        <v>50594.544134786542</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="3">
+        <v>22037.024806176199</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N16" s="3">
+        <v>25953.812155131691</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="T16" s="3">
+        <v>27248.285171480471</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="3">
+        <v>7440.5710242444911</v>
+      </c>
+      <c r="E17" s="3">
+        <v>54321.468932788368</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I17" s="3">
+        <v>26236.623352225241</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N17" s="3">
+        <v>27821.480453769302</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="T17" s="3">
+        <v>19862.88902397819</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>7354.9719687116567</v>
+      </c>
+      <c r="E18" s="3">
+        <v>55850.850886103537</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I18" s="3">
+        <v>27147.73105467757</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N18" s="3">
+        <v>27838.79081525885</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="T18" s="3">
+        <v>20928.38678855585</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <v>7398.8778024539897</v>
+      </c>
+      <c r="E19" s="3">
+        <v>57232.675819164389</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I19" s="3">
+        <v>20544.2572544959</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N19" s="3">
+        <v>25870.22933914623</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="T19" s="3">
+        <v>21287.515517257041</v>
+      </c>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>7710.6561312428967</v>
+      </c>
+      <c r="E20" s="3">
+        <v>51584.592219436861</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I20" s="3">
+        <v>19110.42362470481</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N20" s="3">
+        <v>24846.992360762939</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="T20" s="3">
+        <v>19211.921113987279</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3">
+        <v>7689.9652432174516</v>
+      </c>
+      <c r="E21" s="3">
+        <v>58188.184075386009</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I21" s="3">
+        <v>25860.425137874648</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="N21" s="3">
+        <v>23736.14106557675</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="T21" s="3">
+        <v>23136.30079128065</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3">
+        <v>7519.277775664621</v>
+      </c>
+      <c r="E22" s="3">
+        <v>56606.090532970033</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I22" s="3">
+        <v>27472.0514990009</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N22" s="3">
+        <v>26362.956930790191</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="T22" s="3">
+        <v>21145.99625912806</v>
+      </c>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>7782.7081836173611</v>
+      </c>
+      <c r="E23" s="3">
+        <v>51142.05237166211</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I23" s="3">
+        <v>27885.479411080829</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="N23" s="3">
+        <v>27480.216748047231</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="T23" s="3">
+        <v>23775.2739065395</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="3">
+        <v>7807.0051742331298</v>
+      </c>
+      <c r="E24" s="3">
+        <v>49307.501654132597</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I24" s="3">
+        <v>22540.642134423251</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="N24" s="3">
+        <v>24043.32874586738</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="T24" s="3">
+        <v>22588.26661562216</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="3">
+        <v>7769.362968370825</v>
+      </c>
+      <c r="E25" s="3">
+        <v>45691.652806721147</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="3">
+        <v>29237.82799527701</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="N25" s="3">
+        <v>28385.239127702091</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="T25" s="3">
+        <v>27922.982265031791</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="3">
+        <v>7853.8772735741886</v>
+      </c>
+      <c r="E26" s="3">
+        <v>56604.223211444143</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I26" s="3">
+        <v>23716.743336603078</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="N26" s="3">
+        <v>20175.915136784741</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="T26" s="3">
+        <v>22856.326849591271</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="3">
+        <v>7699.6338483980926</v>
+      </c>
+      <c r="E27" s="3">
+        <v>52656.326339055391</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I27" s="3">
+        <v>29189.776946775652</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="N27" s="3">
+        <v>27921.91306158037</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="T27" s="3">
+        <v>22432.51333178928</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="3">
+        <v>7521.6410705294275</v>
+      </c>
+      <c r="E28" s="3">
+        <v>50762.124475749311</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="3">
+        <v>24353.516116621238</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="N28" s="3">
+        <v>27791.54312588555</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="T28" s="3">
+        <v>17730.622855222518</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>7451.2328930924796</v>
+      </c>
+      <c r="E29" s="3">
+        <v>58152.843750499538</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="3">
+        <v>23709.83611952771</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="N29" s="3">
+        <v>21539.069658128981</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="T29" s="3">
+        <v>18720.238376566751</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="3">
+        <v>7681.3967379004771</v>
+      </c>
+      <c r="E30" s="3">
+        <v>52709.304436421422</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I30" s="3">
+        <v>18306.851416167119</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="N30" s="3">
+        <v>33628.939120799267</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="T30" s="3">
+        <v>20426.31913342416</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3">
+        <v>7480.9009831856411</v>
+      </c>
+      <c r="E31" s="3">
+        <v>54041.1170181653</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="3">
+        <v>29864.813650862841</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N31" s="3">
+        <v>31318.72610426883</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="T31" s="3">
+        <v>22420.379969936421</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="3">
+        <v>7707.2291962054069</v>
+      </c>
+      <c r="E32" s="3">
+        <v>51117.340942870112</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I32" s="3">
+        <v>25500.028851952771</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N32" s="3">
+        <v>27313.788173297002</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="T32" s="3">
+        <v>24989.127697366031</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="3">
+        <v>7492.9524796182704</v>
+      </c>
+      <c r="E33" s="3">
+        <v>54472.262249318803</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I33" s="3">
+        <v>27626.105386012721</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="N33" s="3">
+        <v>26192.68274296094</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="T33" s="3">
+        <v>19748.76884632152</v>
+      </c>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="3">
+        <v>7694.3423088389</v>
+      </c>
+      <c r="E34" s="3">
+        <v>46423.384147229794</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I34" s="3">
+        <v>29556.621621435061</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="N34" s="3">
+        <v>22778.67878328792</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="T34" s="3">
+        <v>21015.266439327879</v>
+      </c>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="3">
+        <v>7399.6571902976602</v>
+      </c>
+      <c r="E35" s="3">
+        <v>60090.636205086281</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I35" s="3">
+        <v>29468.62768937329</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="N35" s="3">
+        <v>28720.51647956403</v>
+      </c>
+      <c r="S35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="T35" s="3">
+        <v>18538.354909173471</v>
+      </c>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="3">
+        <v>7778.3690815042046</v>
+      </c>
+      <c r="E36" s="3">
+        <v>51204.762465122607</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I36" s="3">
+        <v>26302.726810535871</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N36" s="3">
+        <v>25526.191755858312</v>
+      </c>
+      <c r="S36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="T36" s="3">
+        <v>18735.437490917349</v>
+      </c>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="3">
+        <v>7364.594412519883</v>
+      </c>
+      <c r="E37" s="3">
+        <v>61698.750824069022</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I37" s="3">
+        <v>23987.593416893731</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="N37" s="3">
+        <v>27571.763638147131</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="T37" s="3">
+        <v>22397.248349137149</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="3">
+        <v>7946.5256880027273</v>
+      </c>
+      <c r="E38" s="3">
+        <v>49725.176980381468</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I38" s="3">
+        <v>22007.317797275209</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="N38" s="3">
+        <v>30256.78878801089</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="T38" s="3">
+        <v>24820.39397874659</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="3">
+        <v>8187.0029045898664</v>
+      </c>
+      <c r="E39" s="3">
+        <v>46272.614880108988</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I39" s="3">
+        <v>33985.91971335149</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="N39" s="3">
+        <v>24169.101326067201</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="T39" s="3">
+        <v>18504.760334150771</v>
+      </c>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="3">
+        <v>7238.5136854124066</v>
+      </c>
+      <c r="E40" s="3">
+        <v>61604.841711353307</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I40" s="3">
+        <v>30214.322368392379</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N40" s="3">
+        <v>23871.78472043596</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="T40" s="3">
+        <v>21995.620856039961</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="3">
+        <v>7751.791144126335</v>
+      </c>
+      <c r="E41" s="3">
+        <v>56188.949595367827</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I41" s="3">
+        <v>26575.209826339691</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="N41" s="3">
+        <v>29646.2960959128</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="T41" s="3">
+        <v>24134.164480926422</v>
+      </c>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="3">
+        <v>7772.6786802772094</v>
+      </c>
+      <c r="E42" s="3">
+        <v>50070.648766939143</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I42" s="3">
+        <v>29032.851417257039</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="N42" s="3">
+        <v>28792.718485013618</v>
+      </c>
+      <c r="S42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="T42" s="3">
+        <v>18026.155254405079</v>
+      </c>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="3">
+        <v>7500.7386740286311</v>
+      </c>
+      <c r="E43" s="3">
+        <v>53672.770570663022</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I43" s="3">
+        <v>22909.176117711158</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="N43" s="3">
+        <v>25922.16662270662</v>
+      </c>
+      <c r="S43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="T43" s="3">
+        <v>23064.1741421435</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>7386.9451976141781</v>
+      </c>
+      <c r="E44" s="3">
+        <v>58701.652054314247</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I44" s="3">
+        <v>29475.973014713891</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="N44" s="3">
+        <v>28710.912568210711</v>
+      </c>
+      <c r="S44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="T44" s="3">
+        <v>17387.668342688459</v>
+      </c>
+    </row>
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="3">
+        <v>7799.2555106793943</v>
+      </c>
+      <c r="E45" s="3">
+        <v>47962.967841416888</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I45" s="3">
+        <v>22714.205055404171</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="N45" s="3">
+        <v>27013.757437238859</v>
+      </c>
+      <c r="S45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="T45" s="3">
+        <v>17484.190023160761</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="3">
+        <v>7606.2456468757118</v>
+      </c>
+      <c r="E46" s="3">
+        <v>44076.784974205257</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I46" s="3">
+        <v>26018.82962870118</v>
+      </c>
+      <c r="M46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="N46" s="3">
+        <v>24378.651235603989</v>
+      </c>
+      <c r="S46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="T46" s="3">
+        <v>24768.97743142597</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="3">
+        <v>7535.7360952738027</v>
+      </c>
+      <c r="E47" s="3">
+        <v>54239.344323887373</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I47" s="3">
+        <v>24108.260384377842</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="N47" s="3">
+        <v>25213.660931880109</v>
+      </c>
+      <c r="S47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="T47" s="3">
+        <v>18138.828189554941</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="3">
+        <v>7170.7148357873211</v>
+      </c>
+      <c r="E48" s="3">
+        <v>63582.563860127149</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I48" s="3">
+        <v>22262.613278474098</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="N48" s="3">
+        <v>25801.094716439598</v>
+      </c>
+      <c r="S48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="T48" s="3">
+        <v>26071.070863669389</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="3">
+        <v>7246.8165271301996</v>
+      </c>
+      <c r="E49" s="3">
+        <v>61552.921761217083</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I49" s="3">
+        <v>21762.464642325151</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="N49" s="3">
+        <v>26359.244130426869</v>
+      </c>
+      <c r="S49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="T49" s="3">
+        <v>21987.527546321518</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="3">
+        <v>7389.5526797318798</v>
+      </c>
+      <c r="E50" s="3">
+        <v>56887.663075749311</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I50" s="3">
+        <v>21174.720312443231</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="N50" s="3">
+        <v>26790.604630699359</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="T50" s="3">
+        <v>20352.815826339691</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="3">
+        <v>7658.9704080663487</v>
+      </c>
+      <c r="E51" s="3">
+        <v>44901.241692915522</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I51" s="3">
+        <v>27372.740427974561</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="N51" s="3">
+        <v>25730.73638510445</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="T51" s="3">
+        <v>18445.639215712981</v>
+      </c>
+    </row>
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="3">
+        <v>7888.4768890933883</v>
+      </c>
+      <c r="E52" s="3">
+        <v>58875.970708991823</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I52" s="3">
+        <v>20963.740673206172</v>
+      </c>
+      <c r="M52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="N52" s="3">
+        <v>26960.308219800168</v>
+      </c>
+      <c r="S52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="T52" s="3">
+        <v>21782.700603451409</v>
+      </c>
+    </row>
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="3">
+        <v>7553.6412702340394</v>
+      </c>
+      <c r="E53" s="3">
+        <v>54874.120382742964</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I53" s="3">
+        <v>26174.130431244321</v>
+      </c>
+      <c r="M53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="N53" s="3">
+        <v>24106.8282212534</v>
+      </c>
+      <c r="S53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="T53" s="3">
+        <v>20043.88215149863</v>
+      </c>
+    </row>
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="3">
+        <v>7491.3349712792542</v>
+      </c>
+      <c r="E54" s="3">
+        <v>52482.709580653936</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I54" s="3">
+        <v>20206.96591825613</v>
+      </c>
+      <c r="M54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="N54" s="3">
+        <v>29653.797887738401</v>
+      </c>
+      <c r="S54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="T54" s="3">
+        <v>19469.047071207991</v>
+      </c>
+    </row>
+    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="3">
+        <f>AVERAGE(D5:D54)</f>
+        <v>7613.4964429516021</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>53571.280952895548</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I56" s="3">
+        <f>AVERAGE(I5:I54)</f>
+        <v>25129.21293262126</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N56" s="3">
+        <f>AVERAGE(N5:N54)</f>
+        <v>26693.120168508627</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T56" s="3">
+        <f>AVERAGE(T5:T54)</f>
+        <v>21033.450250214344</v>
+      </c>
+    </row>
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>201.56299174951789</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>4683.0130682009703</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I57" s="3">
+        <f>_xlfn.STDEV.S(I5:I54)</f>
+        <v>3508.9550639479116</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N57" s="3">
+        <f>_xlfn.STDEV.S(N5:N54)</f>
+        <v>2810.4640970080959</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T57" s="3">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
+        <v>2708.8431954162374</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test-23: hybrid 3 (mae)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
-    <sheet name="r2 (3Ysum)" sheetId="4" r:id="rId2"/>
-    <sheet name="mse (2Ysum)" sheetId="2" r:id="rId3"/>
-    <sheet name="mae (2Ysum)" sheetId="3" r:id="rId4"/>
+    <sheet name="mse (2Ysum)" sheetId="2" r:id="rId2"/>
+    <sheet name="mae (2Ysum)" sheetId="3" r:id="rId3"/>
+    <sheet name="r2 (3Ysum)" sheetId="4" r:id="rId4"/>
+    <sheet name="mae (3Ysum)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="16">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -67,6 +68,9 @@
   </si>
   <si>
     <t>Hybrid3 model (superdataset-24-f + 2Y + 3Y.csv)</t>
+  </si>
+  <si>
+    <t>Hybrid3-model (superdataset-24-f + 2Y + 3Y.csv)</t>
   </si>
 </sst>
 </file>
@@ -2174,1401 +2178,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O56"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.93724331009075557</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.57366576059119523</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.74759938062002673</v>
-      </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0.78489980504236645</v>
-      </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="2">
-        <f>C4+1</f>
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.9364250101722924</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.56553616521035333</v>
-      </c>
-      <c r="I5" s="2">
-        <f>I4+1</f>
-        <v>2</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.75272216793297142</v>
-      </c>
-      <c r="N5" s="2">
-        <f>N4+1</f>
-        <v>2</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0.76889713805937721</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="2">
-        <f t="shared" ref="C6:C53" si="0">C5+1</f>
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.93748788487154644</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.54048254862289968</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" ref="I6:I53" si="1">I5+1</f>
-        <v>3</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.81290062745285052</v>
-      </c>
-      <c r="N6" s="2">
-        <f t="shared" ref="N6:N53" si="2">N5+1</f>
-        <v>3</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0.80729775526569381</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.93445972011419998</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.59146116316912933</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.76359659281275505</v>
-      </c>
-      <c r="N7" s="2">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="O7" s="3">
-        <v>0.77998675978926502</v>
-      </c>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.93471122007508478</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.53550422975986045</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.7545887963884832</v>
-      </c>
-      <c r="N8" s="2">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="O8" s="3">
-        <v>0.74093244213597886</v>
-      </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.93944904316418554</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.52116622617217656</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.80385166737402391</v>
-      </c>
-      <c r="N9" s="2">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="O9" s="3">
-        <v>0.78829967713958138</v>
-      </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="2">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.93296991368132143</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.57724593823974513</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.81537059224632424</v>
-      </c>
-      <c r="N10" s="2">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="O10" s="3">
-        <v>0.73867871133666696</v>
-      </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.93890948114171424</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.5731095238741577</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0.80425470934478516</v>
-      </c>
-      <c r="N11" s="2">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="O11" s="3">
-        <v>0.79989025541292258</v>
-      </c>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.9371252243496363</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.48228783733264419</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0.7576941490745841</v>
-      </c>
-      <c r="N12" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="O12" s="3">
-        <v>0.80930455026279047</v>
-      </c>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.93524286015752645</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.55117054184852332</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0.74667295040812309</v>
-      </c>
-      <c r="N13" s="2">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="O13" s="3">
-        <v>0.77140772157724169</v>
-      </c>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.93052196850489854</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.60505452918149782</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0.78479006333818369</v>
-      </c>
-      <c r="N14" s="2">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="O14" s="3">
-        <v>0.80790040470964197</v>
-      </c>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.93493401282551636</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.53659944711091323</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0.77498508287134604</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O15" s="3">
-        <v>0.75474996548915196</v>
-      </c>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="2">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.93258856553483538</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.52478642040580104</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.76680506361277445</v>
-      </c>
-      <c r="N16" s="2">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="O16" s="3">
-        <v>0.81167527136343665</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.93688509527115338</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.53574529388184999</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0.79547860900348266</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="O17" s="3">
-        <v>0.80066366481058293</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.93353114501585321</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.53564138198092914</v>
-      </c>
-      <c r="I18" s="2">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0.80253923797160254</v>
-      </c>
-      <c r="N18" s="2">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="O18" s="3">
-        <v>0.79379990111229703</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.93554892968946057</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.52885453953339723</v>
-      </c>
-      <c r="I19" s="2">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0.75811037408550375</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="O19" s="3">
-        <v>0.79330358700648618</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.9367749269307496</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.47915484083707838</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.80959496508752071</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="O20" s="3">
-        <v>0.80364508616800112</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.93706312461485719</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0.60508478889342243</v>
-      </c>
-      <c r="I21" s="2">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0.78243223145681651</v>
-      </c>
-      <c r="N21" s="2">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="O21" s="3">
-        <v>0.8358005987200301</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="2">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.93677359188377485</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0.58097543648474426</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0.79065531295771696</v>
-      </c>
-      <c r="N22" s="2">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="O22" s="3">
-        <v>0.79355445633115396</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.93783223714103436</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.53927680252713406</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0.75111177334431645</v>
-      </c>
-      <c r="N23" s="2">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="O23" s="3">
-        <v>0.78853351229375457</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.93696198381646711</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.56684582603709277</v>
-      </c>
-      <c r="I24" s="2">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="J24" s="3">
-        <v>0.7933349338637159</v>
-      </c>
-      <c r="N24" s="2">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="O24" s="3">
-        <v>0.78748954623838974</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="2">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.93487427539249823</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0.50691574291111374</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="J25" s="3">
-        <v>0.7431987341233699</v>
-      </c>
-      <c r="N25" s="2">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="O25" s="3">
-        <v>0.80992712180274473</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="2">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.93424026651190117</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0.57549635679662603</v>
-      </c>
-      <c r="I26" s="2">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="J26" s="3">
-        <v>0.80481897041530459</v>
-      </c>
-      <c r="N26" s="2">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="O26" s="3">
-        <v>0.77620233911398839</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="2">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="D27" s="3">
-        <v>0.93473639651351537</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0.49969175042750458</v>
-      </c>
-      <c r="I27" s="2">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="J27" s="3">
-        <v>0.77831347161363618</v>
-      </c>
-      <c r="N27" s="2">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="O27" s="3">
-        <v>0.80374149857995725</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="2">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0.93618157206029939</v>
-      </c>
-      <c r="E28" s="3">
-        <v>0.58467038820419071</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="J28" s="3">
-        <v>0.73250447421016152</v>
-      </c>
-      <c r="N28" s="2">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="O28" s="3">
-        <v>0.77311927125394853</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="2">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.93779328378464677</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0.53102749996911891</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="J29" s="3">
-        <v>0.79928969776231029</v>
-      </c>
-      <c r="N29" s="2">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="O29" s="3">
-        <v>0.79561855051336716</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="2">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="D30" s="3">
-        <v>0.9361542280997095</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0.50572409800716001</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="J30" s="3">
-        <v>0.80145040301035131</v>
-      </c>
-      <c r="N30" s="2">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="O30" s="3">
-        <v>0.81308835275443048</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="2">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0.93528221458546135</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0.56921542318050067</v>
-      </c>
-      <c r="I31" s="2">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0.79203197789581958</v>
-      </c>
-      <c r="N31" s="2">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="O31" s="3">
-        <v>0.8111886017465374</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0.93542606592995337</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0.56265910362812721</v>
-      </c>
-      <c r="I32" s="2">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="J32" s="3">
-        <v>0.74549347792987275</v>
-      </c>
-      <c r="N32" s="2">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="O32" s="3">
-        <v>0.79891958026776666</v>
-      </c>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C33" s="2">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0.93482881767601267</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0.54768755466741947</v>
-      </c>
-      <c r="I33" s="2">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="J33" s="3">
-        <v>0.78356932624316888</v>
-      </c>
-      <c r="N33" s="2">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="O33" s="3">
-        <v>0.79637222780511763</v>
-      </c>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C34" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0.93902328029141957</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0.51988643654018962</v>
-      </c>
-      <c r="I34" s="2">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="J34" s="3">
-        <v>0.78165766235738088</v>
-      </c>
-      <c r="N34" s="2">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="O34" s="3">
-        <v>0.80490616625728184</v>
-      </c>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C35" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0.93558795414096219</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.56479956908036355</v>
-      </c>
-      <c r="I35" s="2">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="J35" s="3">
-        <v>0.8129048890288546</v>
-      </c>
-      <c r="N35" s="2">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="O35" s="3">
-        <v>0.79844802895196509</v>
-      </c>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C36" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0.93482386185653599</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0.52866303035105644</v>
-      </c>
-      <c r="I36" s="2">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="J36" s="3">
-        <v>0.80361307339161958</v>
-      </c>
-      <c r="N36" s="2">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="O36" s="3">
-        <v>0.81164488617488939</v>
-      </c>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C37" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0.9340720399328365</v>
-      </c>
-      <c r="E37" s="3">
-        <v>0.59449859643989855</v>
-      </c>
-      <c r="I37" s="2">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="J37" s="3">
-        <v>0.77850151482103791</v>
-      </c>
-      <c r="N37" s="2">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="O37" s="3">
-        <v>0.78931160602477124</v>
-      </c>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C38" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="D38" s="3">
-        <v>0.93654080260174999</v>
-      </c>
-      <c r="E38" s="3">
-        <v>0.51886668871919794</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="J38" s="3">
-        <v>0.76357957335404536</v>
-      </c>
-      <c r="N38" s="2">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="O38" s="3">
-        <v>0.81606363231006518</v>
-      </c>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="2">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0.93498161667326896</v>
-      </c>
-      <c r="E39" s="3">
-        <v>0.56764254581066531</v>
-      </c>
-      <c r="I39" s="2">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="J39" s="3">
-        <v>0.82719591105098256</v>
-      </c>
-      <c r="N39" s="2">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="O39" s="3">
-        <v>0.81628912563866352</v>
-      </c>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="2">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="D40" s="3">
-        <v>0.93682686758373235</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0.53679709072004633</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="J40" s="3">
-        <v>0.78768718630391255</v>
-      </c>
-      <c r="N40" s="2">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="O40" s="3">
-        <v>0.79620131781626413</v>
-      </c>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C41" s="2">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="D41" s="3">
-        <v>0.93328657464121012</v>
-      </c>
-      <c r="E41" s="3">
-        <v>0.54523526365556463</v>
-      </c>
-      <c r="I41" s="2">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="J41" s="3">
-        <v>0.80721891304325188</v>
-      </c>
-      <c r="N41" s="2">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="O41" s="3">
-        <v>0.79970030936830572</v>
-      </c>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="2">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="D42" s="3">
-        <v>0.93640122479880195</v>
-      </c>
-      <c r="E42" s="3">
-        <v>0.4984587764105497</v>
-      </c>
-      <c r="I42" s="2">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="J42" s="3">
-        <v>0.80684801694652231</v>
-      </c>
-      <c r="N42" s="2">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="O42" s="3">
-        <v>0.79815917870493136</v>
-      </c>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="2">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0.9356903120593667</v>
-      </c>
-      <c r="E43" s="3">
-        <v>0.51100008552249709</v>
-      </c>
-      <c r="I43" s="2">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="J43" s="3">
-        <v>0.77865927003954072</v>
-      </c>
-      <c r="N43" s="2">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="O43" s="3">
-        <v>0.79069923511435336</v>
-      </c>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="2">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0.93271592181688967</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0.55145626449775287</v>
-      </c>
-      <c r="I44" s="2">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="J44" s="3">
-        <v>0.78440058195670237</v>
-      </c>
-      <c r="N44" s="2">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-      <c r="O44" s="3">
-        <v>0.77816507524361822</v>
-      </c>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="D45" s="3">
-        <v>0.93345541265328213</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0.54749760292352456</v>
-      </c>
-      <c r="I45" s="2">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="J45" s="3">
-        <v>0.77517757569569157</v>
-      </c>
-      <c r="N45" s="2">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="O45" s="3">
-        <v>0.79559676665695334</v>
-      </c>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="D46" s="3">
-        <v>0.93565314714292436</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0.55762146140555124</v>
-      </c>
-      <c r="I46" s="2">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="J46" s="3">
-        <v>0.73172178530723397</v>
-      </c>
-      <c r="N46" s="2">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="O46" s="3">
-        <v>0.81422631040683591</v>
-      </c>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C47" s="2">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="D47" s="3">
-        <v>0.93810550874844734</v>
-      </c>
-      <c r="E47" s="3">
-        <v>0.5064381570260309</v>
-      </c>
-      <c r="I47" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="J47" s="3">
-        <v>0.78739711178736771</v>
-      </c>
-      <c r="N47" s="2">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="O47" s="3">
-        <v>0.83624260301461217</v>
-      </c>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C48" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="D48" s="3">
-        <v>0.93837554549820112</v>
-      </c>
-      <c r="E48" s="3">
-        <v>0.50477922207014803</v>
-      </c>
-      <c r="I48" s="2">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="J48" s="3">
-        <v>0.76981245439444945</v>
-      </c>
-      <c r="N48" s="2">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="O48" s="3">
-        <v>0.77948556828586979</v>
-      </c>
-    </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C49" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="D49" s="3">
-        <v>0.93582134710153908</v>
-      </c>
-      <c r="E49" s="3">
-        <v>0.52867142289623414</v>
-      </c>
-      <c r="I49" s="2">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="J49" s="3">
-        <v>0.74310584214061914</v>
-      </c>
-      <c r="N49" s="2">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-      <c r="O49" s="3">
-        <v>0.77052783287717719</v>
-      </c>
-    </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C50" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D50" s="3">
-        <v>0.93541897116889139</v>
-      </c>
-      <c r="E50" s="3">
-        <v>0.53645824034774159</v>
-      </c>
-      <c r="I50" s="2">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="J50" s="3">
-        <v>0.80322037948211167</v>
-      </c>
-      <c r="N50" s="2">
-        <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="O50" s="3">
-        <v>0.79610203589235684</v>
-      </c>
-    </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="2">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="D51" s="3">
-        <v>0.93503090158415247</v>
-      </c>
-      <c r="E51" s="3">
-        <v>0.49908194143210138</v>
-      </c>
-      <c r="I51" s="2">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="J51" s="3">
-        <v>0.78192280972213579</v>
-      </c>
-      <c r="N51" s="2">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="O51" s="3">
-        <v>0.75303614690770015</v>
-      </c>
-    </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C52" s="2">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="D52" s="3">
-        <v>0.9339728317282846</v>
-      </c>
-      <c r="E52" s="3">
-        <v>0.5705278001846309</v>
-      </c>
-      <c r="I52" s="2">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="J52" s="3">
-        <v>0.74027177131612953</v>
-      </c>
-      <c r="N52" s="2">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="O52" s="3">
-        <v>0.8259339337042062</v>
-      </c>
-    </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="D53" s="3">
-        <v>0.93875136668458259</v>
-      </c>
-      <c r="E53" s="3">
-        <v>0.49252797941498061</v>
-      </c>
-      <c r="I53" s="2">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="J53" s="3">
-        <v>0.77066450762997896</v>
-      </c>
-      <c r="N53" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="O53" s="3">
-        <v>0.78973831256011973</v>
-      </c>
-    </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="3">
-        <f>AVERAGE(D4:D53)</f>
-        <v>0.93574983716615889</v>
-      </c>
-      <c r="E55" s="3">
-        <f>AVERAGE(E4:E53)</f>
-        <v>0.54227290669870076</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J55" s="3">
-        <f>AVERAGE(J4:J53)</f>
-        <v>0.77970641288442966</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O55" s="3">
-        <f>AVERAGE(O4:O53)</f>
-        <v>0.79398732852027254</v>
-      </c>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="3">
-        <f>_xlfn.STDEV.S(D4:D53)</f>
-        <v>1.8551682465640584E-3</v>
-      </c>
-      <c r="E56" s="3">
-        <f>_xlfn.STDEV.S(E4:E53)</f>
-        <v>3.1918063720656198E-2</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J56" s="3">
-        <f>_xlfn.STDEV.S(J4:J53)</f>
-        <v>2.4509800244337382E-2</v>
-      </c>
-      <c r="N56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O56" s="3">
-        <f>_xlfn.STDEV.S(O4:O53)</f>
-        <v>2.0712879669264692E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:T57"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
@@ -5338,7 +3947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:S57"/>
   <sheetViews>
@@ -7106,4 +5715,2798 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:O56"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.93724331009075557</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.57366576059119523</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.74759938062002673</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.78489980504236645</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <f>C4+1</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.9364250101722924</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.56553616521035333</v>
+      </c>
+      <c r="I5" s="2">
+        <f>I4+1</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.75272216793297142</v>
+      </c>
+      <c r="N5" s="2">
+        <f>N4+1</f>
+        <v>2</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.76889713805937721</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f t="shared" ref="C6:C53" si="0">C5+1</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.93748788487154644</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.54048254862289968</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" ref="I6:I53" si="1">I5+1</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.81290062745285052</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" ref="N6:N53" si="2">N5+1</f>
+        <v>3</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.80729775526569381</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.93445972011419998</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.59146116316912933</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.76359659281275505</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.77998675978926502</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.93471122007508478</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.53550422975986045</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.7545887963884832</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.74093244213597886</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.93944904316418554</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.52116622617217656</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.80385166737402391</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.78829967713958138</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.93296991368132143</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.57724593823974513</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.81537059224632424</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.73867871133666696</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.93890948114171424</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5731095238741577</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.80425470934478516</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.79989025541292258</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.9371252243496363</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.48228783733264419</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.7576941490745841</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.80930455026279047</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.93524286015752645</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.55117054184852332</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.74667295040812309</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.77140772157724169</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.93052196850489854</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.60505452918149782</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.78479006333818369</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0.80790040470964197</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.93493401282551636</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.53659944711091323</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.77498508287134604</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0.75474996548915196</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.93258856553483538</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.52478642040580104</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.76680506361277445</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0.81167527136343665</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.93688509527115338</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.53574529388184999</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.79547860900348266</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0.80066366481058293</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.93353114501585321</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.53564138198092914</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.80253923797160254</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0.79379990111229703</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.93554892968946057</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.52885453953339723</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.75811037408550375</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.79330358700648618</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.9367749269307496</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.47915484083707838</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.80959496508752071</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0.80364508616800112</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.93706312461485719</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.60508478889342243</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.78243223145681651</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0.8358005987200301</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.93677359188377485</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.58097543648474426</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.79065531295771696</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0.79355445633115396</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.93783223714103436</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.53927680252713406</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.75111177334431645</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0.78853351229375457</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.93696198381646711</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.56684582603709277</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.7933349338637159</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O24" s="3">
+        <v>0.78748954623838974</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.93487427539249823</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.50691574291111374</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.7431987341233699</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0.80992712180274473</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.93424026651190117</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.57549635679662603</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.80481897041530459</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0.77620233911398839</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.93473639651351537</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.49969175042750458</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.77831347161363618</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0.80374149857995725</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.93618157206029939</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.58467038820419071</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.73250447421016152</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0.77311927125394853</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.93779328378464677</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.53102749996911891</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.79928969776231029</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0.79561855051336716</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.9361542280997095</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.50572409800716001</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.80145040301035131</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0.81308835275443048</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.93528221458546135</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.56921542318050067</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.79203197789581958</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0.8111886017465374</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.93542606592995337</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.56265910362812721</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.74549347792987275</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0.79891958026776666</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.93482881767601267</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.54768755466741947</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0.78356932624316888</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0.79637222780511763</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.93902328029141957</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.51988643654018962</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0.78165766235738088</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0.80490616625728184</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.93558795414096219</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.56479956908036355</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0.8129048890288546</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0.79844802895196509</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.93482386185653599</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.52866303035105644</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0.80361307339161958</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0.81164488617488939</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.9340720399328365</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.59449859643989855</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0.77850151482103791</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0.78931160602477124</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.93654080260174999</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.51886668871919794</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0.76357957335404536</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O38" s="3">
+        <v>0.81606363231006518</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.93498161667326896</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.56764254581066531</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0.82719591105098256</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0.81628912563866352</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.93682686758373235</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.53679709072004633</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0.78768718630391255</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O40" s="3">
+        <v>0.79620131781626413</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.93328657464121012</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.54523526365556463</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0.80721891304325188</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O41" s="3">
+        <v>0.79970030936830572</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.93640122479880195</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.4984587764105497</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0.80684801694652231</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0.79815917870493136</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.9356903120593667</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.51100008552249709</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0.77865927003954072</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O43" s="3">
+        <v>0.79069923511435336</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.93271592181688967</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0.55145626449775287</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0.78440058195670237</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O44" s="3">
+        <v>0.77816507524361822</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.93345541265328213</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.54749760292352456</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0.77517757569569157</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O45" s="3">
+        <v>0.79559676665695334</v>
+      </c>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.93565314714292436</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.55762146140555124</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0.73172178530723397</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O46" s="3">
+        <v>0.81422631040683591</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.93810550874844734</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.5064381570260309</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0.78739711178736771</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O47" s="3">
+        <v>0.83624260301461217</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.93837554549820112</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.50477922207014803</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0.76981245439444945</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O48" s="3">
+        <v>0.77948556828586979</v>
+      </c>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.93582134710153908</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.52867142289623414</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0.74310584214061914</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O49" s="3">
+        <v>0.77052783287717719</v>
+      </c>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.93541897116889139</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.53645824034774159</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0.80322037948211167</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O50" s="3">
+        <v>0.79610203589235684</v>
+      </c>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.93503090158415247</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.49908194143210138</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0.78192280972213579</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O51" s="3">
+        <v>0.75303614690770015</v>
+      </c>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.9339728317282846</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.5705278001846309</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0.74027177131612953</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O52" s="3">
+        <v>0.8259339337042062</v>
+      </c>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.93875136668458259</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.49252797941498061</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J53" s="3">
+        <v>0.77066450762997896</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O53" s="3">
+        <v>0.78973831256011973</v>
+      </c>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="3">
+        <f>AVERAGE(D4:D53)</f>
+        <v>0.93574983716615889</v>
+      </c>
+      <c r="E55" s="3">
+        <f>AVERAGE(E4:E53)</f>
+        <v>0.54227290669870076</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="3">
+        <f>AVERAGE(J4:J53)</f>
+        <v>0.77970641288442966</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O55" s="3">
+        <f>AVERAGE(O4:O53)</f>
+        <v>0.79398732852027254</v>
+      </c>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="3">
+        <f>_xlfn.STDEV.S(D4:D53)</f>
+        <v>1.8551682465640584E-3</v>
+      </c>
+      <c r="E56" s="3">
+        <f>_xlfn.STDEV.S(E4:E53)</f>
+        <v>3.1918063720656198E-2</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J56" s="3">
+        <f>_xlfn.STDEV.S(J4:J53)</f>
+        <v>2.4509800244337382E-2</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O56" s="3">
+        <f>_xlfn.STDEV.S(O4:O53)</f>
+        <v>2.0712879669264692E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:Q57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>76.040969495620658</v>
+      </c>
+      <c r="F5" s="3">
+        <v>216.25894927536231</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>136.70759661835751</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>128.26578549403879</v>
+      </c>
+    </row>
+    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f>D5+1</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>77.437589852008443</v>
+      </c>
+      <c r="F6" s="3">
+        <v>208.92392512077291</v>
+      </c>
+      <c r="K6" s="2">
+        <f>K5+1</f>
+        <v>2</v>
+      </c>
+      <c r="L6" s="3">
+        <v>140.02938405797099</v>
+      </c>
+      <c r="P6" s="2">
+        <f>P5+1</f>
+        <v>2</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>133.62510106320829</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f t="shared" ref="D7:D54" si="0">D6+1</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>77.399981878586516</v>
+      </c>
+      <c r="F7" s="3">
+        <v>203.42491545893719</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" ref="K7:K54" si="1">K6+1</f>
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>142.045652173913</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" ref="P7:P54" si="2">P6+1</f>
+        <v>3</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>129.6274868178424</v>
+      </c>
+    </row>
+    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>78.028819087888849</v>
+      </c>
+      <c r="F8" s="3">
+        <v>205.889347826087</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L8" s="3">
+        <v>133.6248792270531</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>127.0430453704974</v>
+      </c>
+    </row>
+    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>78.471685291452715</v>
+      </c>
+      <c r="F9" s="3">
+        <v>210.00800724637679</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L9" s="3">
+        <v>133.76469806763279</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>131.5198761410567</v>
+      </c>
+    </row>
+    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>77.598640893989725</v>
+      </c>
+      <c r="F10" s="3">
+        <v>210.55535024154591</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L10" s="3">
+        <v>147.3374033816425</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>129.9570566070802</v>
+      </c>
+    </row>
+    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>76.344327997583818</v>
+      </c>
+      <c r="F11" s="3">
+        <v>217.11873188405801</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L11" s="3">
+        <v>139.13904589371981</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>129.98991916721269</v>
+      </c>
+    </row>
+    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="3">
+        <v>77.070996677740865</v>
+      </c>
+      <c r="F12" s="3">
+        <v>216.93109903381651</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L12" s="3">
+        <v>139.21859903381639</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>129.36490352133779</v>
+      </c>
+    </row>
+    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E13" s="3">
+        <v>78.016106916339467</v>
+      </c>
+      <c r="F13" s="3">
+        <v>212.62183574879231</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L13" s="3">
+        <v>143.0381763285024</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>129.58422353535809</v>
+      </c>
+    </row>
+    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>77.145620658411346</v>
+      </c>
+      <c r="F14" s="3">
+        <v>202.3907729468599</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L14" s="3">
+        <v>132.77280193236709</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>121.55001182330319</v>
+      </c>
+    </row>
+    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E15" s="3">
+        <v>78.664759891271501</v>
+      </c>
+      <c r="F15" s="3">
+        <v>203.79548309178739</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L15" s="3">
+        <v>136.1197101449275</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>134.26603925692251</v>
+      </c>
+    </row>
+    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E16" s="3">
+        <v>79.822244035034714</v>
+      </c>
+      <c r="F16" s="3">
+        <v>184.61871980676329</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="L16" s="3">
+        <v>140.01830917874389</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>133.82663780053539</v>
+      </c>
+    </row>
+    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E17" s="3">
+        <v>77.028683177287832</v>
+      </c>
+      <c r="F17" s="3">
+        <v>210.3666062801932</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L17" s="3">
+        <v>125.62954106280191</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>128.42998078554481</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E18" s="3">
+        <v>75.970924192086983</v>
+      </c>
+      <c r="F18" s="3">
+        <v>205.06304347826091</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="L18" s="3">
+        <v>136.0615458937198</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>127.01078078249689</v>
+      </c>
+    </row>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E19" s="3">
+        <v>76.947058290546664</v>
+      </c>
+      <c r="F19" s="3">
+        <v>209.5690338164251</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="L19" s="3">
+        <v>127.596497584541</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>130.095181108622</v>
+      </c>
+    </row>
+    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E20" s="3">
+        <v>79.046052552099056</v>
+      </c>
+      <c r="F20" s="3">
+        <v>200.81948067632851</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="L20" s="3">
+        <v>132.5337198067632</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>126.8550053846193</v>
+      </c>
+    </row>
+    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E21" s="3">
+        <v>75.74309574146784</v>
+      </c>
+      <c r="F21" s="3">
+        <v>217.112077294686</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="L21" s="3">
+        <v>132.74778985507251</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>129.2379773261809</v>
+      </c>
+    </row>
+    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E22" s="3">
+        <v>77.269048625792806</v>
+      </c>
+      <c r="F22" s="3">
+        <v>199.72256038647339</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="L22" s="3">
+        <v>143.7239855072464</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>131.68170694971479</v>
+      </c>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E23" s="3">
+        <v>77.117795228027774</v>
+      </c>
+      <c r="F23" s="3">
+        <v>208.33532608695651</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="L23" s="3">
+        <v>140.0293719806763</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>128.06853639951839</v>
+      </c>
+    </row>
+    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E24" s="3">
+        <v>78.634660223497434</v>
+      </c>
+      <c r="F24" s="3">
+        <v>197.21481884057971</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L24" s="3">
+        <v>138.0535628019324</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>124.88711724754521</v>
+      </c>
+    </row>
+    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E25" s="3">
+        <v>78.4553065539112</v>
+      </c>
+      <c r="F25" s="3">
+        <v>200.88818840579711</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="L25" s="3">
+        <v>137.1313405797101</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>136.9638362364559</v>
+      </c>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E26" s="3">
+        <v>76.691760797342184</v>
+      </c>
+      <c r="F26" s="3">
+        <v>215.2133816425121</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="L26" s="3">
+        <v>143.0036111111111</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>123.8382186688814</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E27" s="3">
+        <v>78.245992147387497</v>
+      </c>
+      <c r="F27" s="3">
+        <v>213.6066666666666</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="L27" s="3">
+        <v>130.3520893719807</v>
+      </c>
+      <c r="P27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>126.3511993477499</v>
+      </c>
+    </row>
+    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E28" s="3">
+        <v>77.854089398973116</v>
+      </c>
+      <c r="F28" s="3">
+        <v>206.40169082125601</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="L28" s="3">
+        <v>138.08850241545889</v>
+      </c>
+      <c r="P28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>128.62619196929751</v>
+      </c>
+    </row>
+    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E29" s="3">
+        <v>77.379719118091202</v>
+      </c>
+      <c r="F29" s="3">
+        <v>211.1742391304347</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="L29" s="3">
+        <v>137.84788647343001</v>
+      </c>
+      <c r="P29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>135.8322929842474</v>
+      </c>
+    </row>
+    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E30" s="3">
+        <v>78.949948655995158</v>
+      </c>
+      <c r="F30" s="3">
+        <v>205.2859541062802</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="L30" s="3">
+        <v>136.52646135265701</v>
+      </c>
+      <c r="P30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>133.211285933444</v>
+      </c>
+    </row>
+    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E31" s="3">
+        <v>78.553772274237389</v>
+      </c>
+      <c r="F31" s="3">
+        <v>209.96460144927539</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="L31" s="3">
+        <v>141.22724637681159</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>132.81840961967319</v>
+      </c>
+    </row>
+    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E32" s="3">
+        <v>78.27903956508608</v>
+      </c>
+      <c r="F32" s="3">
+        <v>206.06233091787439</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="L32" s="3">
+        <v>135.13685990338161</v>
+      </c>
+      <c r="P32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>137.04150591546141</v>
+      </c>
+    </row>
+    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E33" s="3">
+        <v>77.677097553609173</v>
+      </c>
+      <c r="F33" s="3">
+        <v>201.18555555555551</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="L33" s="3">
+        <v>133.108115942029</v>
+      </c>
+      <c r="P33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>132.20322075161161</v>
+      </c>
+    </row>
+    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E34" s="3">
+        <v>77.34634853518574</v>
+      </c>
+      <c r="F34" s="3">
+        <v>206.6653260869565</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="L34" s="3">
+        <v>128.33978260869571</v>
+      </c>
+      <c r="P34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>125.6606524533037</v>
+      </c>
+    </row>
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E35" s="3">
+        <v>76.744143763213515</v>
+      </c>
+      <c r="F35" s="3">
+        <v>210.65793478260861</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="L35" s="3">
+        <v>135.25376811594199</v>
+      </c>
+      <c r="P35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>132.000601070828</v>
+      </c>
+    </row>
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E36" s="3">
+        <v>77.638731501057066</v>
+      </c>
+      <c r="F36" s="3">
+        <v>207.55211352657</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="L36" s="3">
+        <v>137.0328260869565</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>130.70111742279931</v>
+      </c>
+    </row>
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E37" s="3">
+        <v>78.21748112352762</v>
+      </c>
+      <c r="F37" s="3">
+        <v>211.44378019323671</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="L37" s="3">
+        <v>136.23909420289851</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>130.49670548926369</v>
+      </c>
+    </row>
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E38" s="3">
+        <v>77.649432195711256</v>
+      </c>
+      <c r="F38" s="3">
+        <v>207.05544685990341</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="L38" s="3">
+        <v>127.33426328502421</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>120.0395161335385</v>
+      </c>
+    </row>
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E39" s="3">
+        <v>79.359670794321957</v>
+      </c>
+      <c r="F39" s="3">
+        <v>198.01435990338169</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="L39" s="3">
+        <v>133.75925120772951</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>122.8834256338357</v>
+      </c>
+    </row>
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E40" s="3">
+        <v>76.664394442766536</v>
+      </c>
+      <c r="F40" s="3">
+        <v>214.56683574879219</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="L40" s="3">
+        <v>134.3876690821256</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>126.88575873603681</v>
+      </c>
+    </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E41" s="3">
+        <v>79.299652672908493</v>
+      </c>
+      <c r="F41" s="3">
+        <v>207.304577294686</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="L41" s="3">
+        <v>147.03033816425119</v>
+      </c>
+      <c r="P41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>139.64682838303941</v>
+      </c>
+    </row>
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E42" s="3">
+        <v>76.934808215040775</v>
+      </c>
+      <c r="F42" s="3">
+        <v>212.26068840579711</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="L42" s="3">
+        <v>130.38921497584539</v>
+      </c>
+      <c r="P42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>132.92362707447541</v>
+      </c>
+    </row>
+    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E43" s="3">
+        <v>77.887348233162186</v>
+      </c>
+      <c r="F43" s="3">
+        <v>192.08737922705311</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="L43" s="3">
+        <v>134.8178260869565</v>
+      </c>
+      <c r="P43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>124.34017943227821</v>
+      </c>
+    </row>
+    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E44" s="3">
+        <v>77.072790697674407</v>
+      </c>
+      <c r="F44" s="3">
+        <v>204.32443236714971</v>
+      </c>
+      <c r="K44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="L44" s="3">
+        <v>142.17863526570051</v>
+      </c>
+      <c r="P44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>141.23971837425131</v>
+      </c>
+    </row>
+    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E45" s="3">
+        <v>77.753304137722736</v>
+      </c>
+      <c r="F45" s="3">
+        <v>196.91400966183571</v>
+      </c>
+      <c r="K45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="L45" s="3">
+        <v>136.1986835748792</v>
+      </c>
+      <c r="P45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>130.11608710891659</v>
+      </c>
+    </row>
+    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E46" s="3">
+        <v>77.297496224705526</v>
+      </c>
+      <c r="F46" s="3">
+        <v>216.0747342995169</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="L46" s="3">
+        <v>132.6260144927536</v>
+      </c>
+      <c r="P46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>125.51807460491619</v>
+      </c>
+    </row>
+    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E47" s="3">
+        <v>75.581356085774686</v>
+      </c>
+      <c r="F47" s="3">
+        <v>214.19390096618349</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="L47" s="3">
+        <v>132.69594202898551</v>
+      </c>
+      <c r="P47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>136.47943497056241</v>
+      </c>
+    </row>
+    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E48" s="3">
+        <v>77.405297493204458</v>
+      </c>
+      <c r="F48" s="3">
+        <v>201.84665458937201</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="L48" s="3">
+        <v>137.0407729468599</v>
+      </c>
+      <c r="P48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>126.73580691821979</v>
+      </c>
+    </row>
+    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E49" s="3">
+        <v>77.616629417094529</v>
+      </c>
+      <c r="F49" s="3">
+        <v>215.09971014492751</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="L49" s="3">
+        <v>140.53869565217391</v>
+      </c>
+      <c r="P49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>141.23559237161999</v>
+      </c>
+    </row>
+    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E50" s="3">
+        <v>75.610564784053139</v>
+      </c>
+      <c r="F50" s="3">
+        <v>221.140652173913</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="L50" s="3">
+        <v>145.40161835748791</v>
+      </c>
+      <c r="P50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>136.73420574325519</v>
+      </c>
+    </row>
+    <row r="51" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E51" s="3">
+        <v>77.37492902446391</v>
+      </c>
+      <c r="F51" s="3">
+        <v>209.0242028985507</v>
+      </c>
+      <c r="K51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="L51" s="3">
+        <v>140.2756642512077</v>
+      </c>
+      <c r="P51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>133.9830523298638</v>
+      </c>
+    </row>
+    <row r="52" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E52" s="3">
+        <v>77.999003322259128</v>
+      </c>
+      <c r="F52" s="3">
+        <v>197.6072946859903</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="L52" s="3">
+        <v>140.66734299516909</v>
+      </c>
+      <c r="P52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>131.2224712100662</v>
+      </c>
+    </row>
+    <row r="53" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E53" s="3">
+        <v>77.598501963153097</v>
+      </c>
+      <c r="F53" s="3">
+        <v>209.78096618357489</v>
+      </c>
+      <c r="K53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="L53" s="3">
+        <v>132.01683574879229</v>
+      </c>
+      <c r="P53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>132.4690521927084</v>
+      </c>
+    </row>
+    <row r="54" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E54" s="3">
+        <v>78.19132890365448</v>
+      </c>
+      <c r="F54" s="3">
+        <v>194.1978260869565</v>
+      </c>
+      <c r="K54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="L54" s="3">
+        <v>140.04112318840581</v>
+      </c>
+      <c r="P54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>126.631875892145</v>
+      </c>
+    </row>
+    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>77.582580006040459</v>
+      </c>
+      <c r="F56" s="3">
+        <f>AVERAGE(F5:F54)</f>
+        <v>207.1667103864734</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L56" s="3">
+        <f>AVERAGE(L5:L54)</f>
+        <v>136.73759492753624</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q56" s="3">
+        <f>AVERAGE(Q5:Q54)</f>
+        <v>130.39432635110768</v>
+      </c>
+    </row>
+    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>0.95798694002007079</v>
+      </c>
+      <c r="F57" s="3">
+        <f>_xlfn.STDEV.S(F5:F54)</f>
+        <v>7.3329690189643877</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L57" s="3">
+        <f>_xlfn.STDEV.S(L5:L54)</f>
+        <v>4.9685652830725484</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q57" s="3">
+        <f>_xlfn.STDEV.S(Q5:Q54)</f>
+        <v>4.7585997477790096</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test-23: hybrid3 model (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="mae (2Ysum)" sheetId="3" r:id="rId3"/>
     <sheet name="r2 (3Ysum)" sheetId="4" r:id="rId4"/>
     <sheet name="mae (3Ysum)" sheetId="5" r:id="rId5"/>
+    <sheet name="mse (3Ysum)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="16">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -7116,8 +7117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8509,4 +8510,1402 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:P57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>14472.64988106312</v>
+      </c>
+      <c r="E5" s="3">
+        <v>106931.6096601449</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>53910.977389492742</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3">
+        <v>39006.772192397009</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>14305.45225496829</v>
+      </c>
+      <c r="E6" s="3">
+        <v>88916.10351884058</v>
+      </c>
+      <c r="J6" s="2">
+        <f>J5+1</f>
+        <v>2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>50096.715575362308</v>
+      </c>
+      <c r="O6" s="2">
+        <f>O5+1</f>
+        <v>2</v>
+      </c>
+      <c r="P6" s="3">
+        <v>47733.867400683142</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>14524.73927236485</v>
+      </c>
+      <c r="E7" s="3">
+        <v>101449.7523981884</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" ref="J7:J54" si="1">J6+1</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="3">
+        <v>35222.748448067621</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" ref="O7:O54" si="2">O6+1</f>
+        <v>3</v>
+      </c>
+      <c r="P7" s="3">
+        <v>45164.441367669169</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>13808.563179039569</v>
+      </c>
+      <c r="E8" s="3">
+        <v>96576.152567270517</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K8" s="3">
+        <v>47993.271027294657</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
+        <v>45249.927797043427</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>14399.87203600121</v>
+      </c>
+      <c r="E9" s="3">
+        <v>117724.33400954099</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K9" s="3">
+        <v>44127.120558454088</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="P9" s="3">
+        <v>46666.908726800379</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>13869.836735759591</v>
+      </c>
+      <c r="E10" s="3">
+        <v>107362.4577018116</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K10" s="3">
+        <v>46044.093117753611</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="P10" s="3">
+        <v>39610.820316505968</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>14512.47776635457</v>
+      </c>
+      <c r="E11" s="3">
+        <v>101786.78091328499</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K11" s="3">
+        <v>44652.600970531377</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="P11" s="3">
+        <v>41517.573482272317</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>13976.63547088493</v>
+      </c>
+      <c r="E12" s="3">
+        <v>115816.4717109903</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K12" s="3">
+        <v>48462.159571618336</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="P12" s="3">
+        <v>38511.678189972081</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>14164.36500006041</v>
+      </c>
+      <c r="E13" s="3">
+        <v>101737.0387826087</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K13" s="3">
+        <v>53709.71522971012</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="P13" s="3">
+        <v>37856.255232051291</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>14274.595672153429</v>
+      </c>
+      <c r="E14" s="3">
+        <v>85807.5686190821</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K14" s="3">
+        <v>46608.68287463767</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="P14" s="3">
+        <v>42811.744130845997</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>13999.72534167925</v>
+      </c>
+      <c r="E15" s="3">
+        <v>92459.487969323658</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="K15" s="3">
+        <v>38590.6025874396</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="P15" s="3">
+        <v>42717.032815501218</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>13686.852489127161</v>
+      </c>
+      <c r="E16" s="3">
+        <v>100323.37681050719</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K16" s="3">
+        <v>45850.156096497572</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="P16" s="3">
+        <v>49696.344082386589</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="3">
+        <v>13857.024899577171</v>
+      </c>
+      <c r="E17" s="3">
+        <v>102861.1459449275</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K17" s="3">
+        <v>45611.040309420277</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="P17" s="3">
+        <v>40635.625035213758</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>13917.57896886137</v>
+      </c>
+      <c r="E18" s="3">
+        <v>102841.4126152174</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="K18" s="3">
+        <v>42803.785097222208</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="P18" s="3">
+        <v>38167.46125496718</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <v>14612.74516508608</v>
+      </c>
+      <c r="E19" s="3">
+        <v>95352.06761908211</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="K19" s="3">
+        <v>47706.269455917864</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="P19" s="3">
+        <v>55919.680124425278</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>14719.25502893386</v>
+      </c>
+      <c r="E20" s="3">
+        <v>92022.831638768097</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="K20" s="3">
+        <v>55071.717099396141</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="P20" s="3">
+        <v>35008.584443794243</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3">
+        <v>14435.72537879795</v>
+      </c>
+      <c r="E21" s="3">
+        <v>97111.946798550707</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="K21" s="3">
+        <v>42209.511441545903</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="P21" s="3">
+        <v>43544.710408757492</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3">
+        <v>14636.825242917541</v>
+      </c>
+      <c r="E22" s="3">
+        <v>92629.269923550688</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="K22" s="3">
+        <v>49682.020270289853</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="P22" s="3">
+        <v>48046.159090094123</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>14012.21186523709</v>
+      </c>
+      <c r="E23" s="3">
+        <v>109907.2718836956</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="K23" s="3">
+        <v>49311.683922463752</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="P23" s="3">
+        <v>48669.792198569798</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="3">
+        <v>14120.70826324373</v>
+      </c>
+      <c r="E24" s="3">
+        <v>117379.05523393719</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K24" s="3">
+        <v>39064.704778140083</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="P24" s="3">
+        <v>50289.550007839753</v>
+      </c>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="3">
+        <v>14009.62938384174</v>
+      </c>
+      <c r="E25" s="3">
+        <v>98210.676894082106</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="K25" s="3">
+        <v>41983.070560990323</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="P25" s="3">
+        <v>60817.454827383262</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="3">
+        <v>14034.98290721836</v>
+      </c>
+      <c r="E26" s="3">
+        <v>104687.82698913039</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="K26" s="3">
+        <v>56149.619405072437</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="P26" s="3">
+        <v>42204.776910945322</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="3">
+        <v>14107.5000550891</v>
+      </c>
+      <c r="E27" s="3">
+        <v>102515.8324177536</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="K27" s="3">
+        <v>43317.098553502386</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="P27" s="3">
+        <v>46342.243827842372</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="3">
+        <v>13661.858402083961</v>
+      </c>
+      <c r="E28" s="3">
+        <v>126454.99967729471</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="K28" s="3">
+        <v>47764.68925603864</v>
+      </c>
+      <c r="O28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="P28" s="3">
+        <v>47142.793646105951</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>13759.03128631833</v>
+      </c>
+      <c r="E29" s="3">
+        <v>110677.04665724641</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="K29" s="3">
+        <v>47005.041559057943</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="P29" s="3">
+        <v>50337.450980638983</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="3">
+        <v>13650.724136605249</v>
+      </c>
+      <c r="E30" s="3">
+        <v>94867.477355313982</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="K30" s="3">
+        <v>51930.882647584527</v>
+      </c>
+      <c r="O30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="P30" s="3">
+        <v>40127.910379273548</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3">
+        <v>14229.626088825131</v>
+      </c>
+      <c r="E31" s="3">
+        <v>101831.08670881639</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="K31" s="3">
+        <v>54694.252778985508</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="P31" s="3">
+        <v>48037.636582938037</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="3">
+        <v>14501.703433162191</v>
+      </c>
+      <c r="E32" s="3">
+        <v>93467.273605917857</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="K32" s="3">
+        <v>44476.25490277775</v>
+      </c>
+      <c r="O32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="P32" s="3">
+        <v>40658.443962036399</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="3">
+        <v>14561.99219981878</v>
+      </c>
+      <c r="E33" s="3">
+        <v>102589.9004944444</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="K33" s="3">
+        <v>45825.90305362318</v>
+      </c>
+      <c r="O33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="P33" s="3">
+        <v>48095.118633339021</v>
+      </c>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="3">
+        <v>13693.48984971308</v>
+      </c>
+      <c r="E34" s="3">
+        <v>114580.7192165459</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K34" s="3">
+        <v>40826.333127173893</v>
+      </c>
+      <c r="O34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="P34" s="3">
+        <v>43738.795843558997</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="3">
+        <v>13900.405796949561</v>
+      </c>
+      <c r="E35" s="3">
+        <v>93515.348788768082</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="K35" s="3">
+        <v>43269.059705555548</v>
+      </c>
+      <c r="O35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="P35" s="3">
+        <v>38232.851050016987</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="3">
+        <v>13966.472064874661</v>
+      </c>
+      <c r="E36" s="3">
+        <v>88972.667498550698</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K36" s="3">
+        <v>48590.220545289849</v>
+      </c>
+      <c r="O36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="P36" s="3">
+        <v>43530.890776404507</v>
+      </c>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="3">
+        <v>14595.97997124736</v>
+      </c>
+      <c r="E37" s="3">
+        <v>81875.273417512071</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="K37" s="3">
+        <v>50665.984278019299</v>
+      </c>
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="P37" s="3">
+        <v>41049.915703464721</v>
+      </c>
+    </row>
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="3">
+        <v>14139.08958372093</v>
+      </c>
+      <c r="E38" s="3">
+        <v>93863.921420169063</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K38" s="3">
+        <v>43188.038527777768</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="P38" s="3">
+        <v>42807.43649225837</v>
+      </c>
+    </row>
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="3">
+        <v>14337.830077771059</v>
+      </c>
+      <c r="E39" s="3">
+        <v>106356.1402423913</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="K39" s="3">
+        <v>46723.236136352643</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="P39" s="3">
+        <v>37022.076416313917</v>
+      </c>
+    </row>
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="3">
+        <v>14230.124794019939</v>
+      </c>
+      <c r="E40" s="3">
+        <v>90332.861859420285</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="K40" s="3">
+        <v>41983.045774879211</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="P40" s="3">
+        <v>46372.431892333218</v>
+      </c>
+    </row>
+    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="3">
+        <v>14170.686421413469</v>
+      </c>
+      <c r="E41" s="3">
+        <v>102687.47743816421</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="K41" s="3">
+        <v>44475.251282367128</v>
+      </c>
+      <c r="O41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="P41" s="3">
+        <v>37394.644561750858</v>
+      </c>
+    </row>
+    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="3">
+        <v>13727.467442011481</v>
+      </c>
+      <c r="E42" s="3">
+        <v>90191.616622705318</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="K42" s="3">
+        <v>43919.014241908197</v>
+      </c>
+      <c r="O42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="P42" s="3">
+        <v>42989.305727892373</v>
+      </c>
+    </row>
+    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="3">
+        <v>14349.93850434914</v>
+      </c>
+      <c r="E43" s="3">
+        <v>118227.6784173913</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="K43" s="3">
+        <v>49965.224176690812</v>
+      </c>
+      <c r="O43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="P43" s="3">
+        <v>59114.40698198069</v>
+      </c>
+    </row>
+    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>14070.141570764121</v>
+      </c>
+      <c r="E44" s="3">
+        <v>95998.21083369563</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="K44" s="3">
+        <v>45448.302644082098</v>
+      </c>
+      <c r="O44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="P44" s="3">
+        <v>42599.521412786933</v>
+      </c>
+    </row>
+    <row r="45" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="3">
+        <v>13984.843108939889</v>
+      </c>
+      <c r="E45" s="3">
+        <v>101136.1420095411</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="K45" s="3">
+        <v>57046.581365096623</v>
+      </c>
+      <c r="O45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="P45" s="3">
+        <v>44165.999187277339</v>
+      </c>
+    </row>
+    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="3">
+        <v>14637.799070582911</v>
+      </c>
+      <c r="E46" s="3">
+        <v>95495.367235507219</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="K46" s="3">
+        <v>51849.101043236718</v>
+      </c>
+      <c r="O46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="P46" s="3">
+        <v>43993.52235304963</v>
+      </c>
+    </row>
+    <row r="47" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="3">
+        <v>13866.987629386889</v>
+      </c>
+      <c r="E47" s="3">
+        <v>99834.700167028976</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="K47" s="3">
+        <v>47776.05933115942</v>
+      </c>
+      <c r="O47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="P47" s="3">
+        <v>38780.100139815353</v>
+      </c>
+    </row>
+    <row r="48" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="3">
+        <v>14018.17507765025</v>
+      </c>
+      <c r="E48" s="3">
+        <v>106086.0673585749</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="K48" s="3">
+        <v>63866.519510024162</v>
+      </c>
+      <c r="O48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="P48" s="3">
+        <v>54017.109314865571</v>
+      </c>
+    </row>
+    <row r="49" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="3">
+        <v>13640.824842192689</v>
+      </c>
+      <c r="E49" s="3">
+        <v>97269.419271618346</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="K49" s="3">
+        <v>50267.479442874377</v>
+      </c>
+      <c r="O49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="P49" s="3">
+        <v>47912.575040021628</v>
+      </c>
+    </row>
+    <row r="50" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="3">
+        <v>14827.913353760199</v>
+      </c>
+      <c r="E50" s="3">
+        <v>90625.013886111119</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="K50" s="3">
+        <v>48853.398831521707</v>
+      </c>
+      <c r="O50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="P50" s="3">
+        <v>43434.446787438843</v>
+      </c>
+    </row>
+    <row r="51" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="3">
+        <v>14047.412587012979</v>
+      </c>
+      <c r="E51" s="3">
+        <v>97636.170390942018</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="K51" s="3">
+        <v>53105.532463888892</v>
+      </c>
+      <c r="O51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="P51" s="3">
+        <v>40703.061288956553</v>
+      </c>
+    </row>
+    <row r="52" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="3">
+        <v>13694.23739942616</v>
+      </c>
+      <c r="E52" s="3">
+        <v>102472.6262135266</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="K52" s="3">
+        <v>40680.08984927534</v>
+      </c>
+      <c r="O52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="P52" s="3">
+        <v>55575.226855439301</v>
+      </c>
+    </row>
+    <row r="53" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="3">
+        <v>14242.88542808819</v>
+      </c>
+      <c r="E53" s="3">
+        <v>106191.5808006038</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="K53" s="3">
+        <v>38670.934781763273</v>
+      </c>
+      <c r="O53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="P53" s="3">
+        <v>42928.353085234281</v>
+      </c>
+    </row>
+    <row r="54" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="3">
+        <v>13300.985269465409</v>
+      </c>
+      <c r="E54" s="3">
+        <v>111203.94121135261</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K54" s="3">
+        <v>42767.607619927519</v>
+      </c>
+      <c r="O54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="P54" s="3">
+        <v>47179.19244073861</v>
+      </c>
+    </row>
+    <row r="56" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="3">
+        <f>AVERAGE(D5:D54)</f>
+        <v>14125.371552968289</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>100937.0240283889</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K56" s="3">
+        <f>AVERAGE(K5:K54)</f>
+        <v>47076.26806435507</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P56" s="3">
+        <f>AVERAGE(P5:P54)</f>
+        <v>44682.612427997839</v>
+      </c>
+    </row>
+    <row r="57" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>341.10332299795226</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>9225.3637577135632</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="3">
+        <f>_xlfn.STDEV.S(K5:K54)</f>
+        <v>5443.0499555306624</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P57" s="3">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>5667.3617182787521</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new dataset for extrapol 2.0
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -414,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T57"/>
+  <dimension ref="C3:O57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,13 +431,10 @@
         <v>6</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>1</v>
@@ -453,12 +450,8 @@
       <c r="O4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -478,16 +471,10 @@
         <v>1</v>
       </c>
       <c r="O5" s="3">
-        <v>0.74995119740402449</v>
-      </c>
-      <c r="S5" s="2">
-        <v>1</v>
-      </c>
-      <c r="T5" s="3">
         <v>0.77416454041178173</v>
       </c>
     </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -510,17 +497,10 @@
         <v>2</v>
       </c>
       <c r="O6" s="3">
-        <v>0.72994623940247072</v>
-      </c>
-      <c r="S6" s="2">
-        <f>S5+1</f>
-        <v>2</v>
-      </c>
-      <c r="T6" s="3">
         <v>0.81470395155608155</v>
       </c>
     </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -543,17 +523,10 @@
         <v>3</v>
       </c>
       <c r="O7" s="3">
-        <v>0.78747870174024426</v>
-      </c>
-      <c r="S7" s="2">
-        <f t="shared" ref="S7:S54" si="3">S6+1</f>
-        <v>3</v>
-      </c>
-      <c r="T7" s="3">
         <v>0.79668886926260762</v>
       </c>
     </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -576,17 +549,10 @@
         <v>4</v>
       </c>
       <c r="O8" s="3">
-        <v>0.76590417310426728</v>
-      </c>
-      <c r="S8" s="2">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="T8" s="3">
         <v>0.82680697690012384</v>
       </c>
     </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -609,17 +575,10 @@
         <v>5</v>
       </c>
       <c r="O9" s="3">
-        <v>0.74365369599550224</v>
-      </c>
-      <c r="S9" s="2">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="T9" s="3">
         <v>0.79599042243084228</v>
       </c>
     </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -642,17 +601,10 @@
         <v>6</v>
       </c>
       <c r="O10" s="3">
-        <v>0.80488910579054207</v>
-      </c>
-      <c r="S10" s="2">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="T10" s="3">
         <v>0.81328937809939206</v>
       </c>
     </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -675,17 +627,10 @@
         <v>7</v>
       </c>
       <c r="O11" s="3">
-        <v>0.73546295652133042</v>
-      </c>
-      <c r="S11" s="2">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="T11" s="3">
         <v>0.84615624245033449</v>
       </c>
     </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -708,17 +653,10 @@
         <v>8</v>
       </c>
       <c r="O12" s="3">
-        <v>0.75905178300506737</v>
-      </c>
-      <c r="S12" s="2">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="T12" s="3">
         <v>0.82600602571101966</v>
       </c>
     </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -741,17 +679,10 @@
         <v>9</v>
       </c>
       <c r="O13" s="3">
-        <v>0.73192789792037583</v>
-      </c>
-      <c r="S13" s="2">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="T13" s="3">
         <v>0.84772188847685637</v>
       </c>
     </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -774,17 +705,10 @@
         <v>10</v>
       </c>
       <c r="O14" s="3">
-        <v>0.78510939810378322</v>
-      </c>
-      <c r="S14" s="2">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="T14" s="3">
         <v>0.78644683967295803</v>
       </c>
     </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -807,17 +731,10 @@
         <v>11</v>
       </c>
       <c r="O15" s="3">
-        <v>0.75414727289791361</v>
-      </c>
-      <c r="S15" s="2">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="T15" s="3">
         <v>0.81561038790464979</v>
       </c>
     </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -840,17 +757,10 @@
         <v>12</v>
       </c>
       <c r="O16" s="3">
-        <v>0.76915500421989946</v>
-      </c>
-      <c r="S16" s="2">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="T16" s="3">
         <v>0.81301942736522181</v>
       </c>
     </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -873,17 +783,10 @@
         <v>13</v>
       </c>
       <c r="O17" s="3">
-        <v>0.7408840928606053</v>
-      </c>
-      <c r="S17" s="2">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="T17" s="3">
         <v>0.81317080735560143</v>
       </c>
     </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -906,17 +809,10 @@
         <v>14</v>
       </c>
       <c r="O18" s="3">
-        <v>0.76972414196612637</v>
-      </c>
-      <c r="S18" s="2">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="T18" s="3">
         <v>0.81435946408164983</v>
       </c>
     </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -939,17 +835,10 @@
         <v>15</v>
       </c>
       <c r="O19" s="3">
-        <v>0.74528569226484565</v>
-      </c>
-      <c r="S19" s="2">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="T19" s="3">
         <v>0.82837639320219147</v>
       </c>
     </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -972,17 +861,10 @@
         <v>16</v>
       </c>
       <c r="O20" s="3">
-        <v>0.75338963090976008</v>
-      </c>
-      <c r="S20" s="2">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="T20" s="3">
         <v>0.79600110005296199</v>
       </c>
     </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1005,17 +887,10 @@
         <v>17</v>
       </c>
       <c r="O21" s="3">
-        <v>0.78271669402007271</v>
-      </c>
-      <c r="S21" s="2">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="T21" s="3">
         <v>0.83485973930006085</v>
       </c>
     </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1038,17 +913,10 @@
         <v>18</v>
       </c>
       <c r="O22" s="3">
-        <v>0.79082521425867958</v>
-      </c>
-      <c r="S22" s="2">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="T22" s="3">
         <v>0.80729127609344387</v>
       </c>
     </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1071,17 +939,10 @@
         <v>19</v>
       </c>
       <c r="O23" s="3">
-        <v>0.73813935433949185</v>
-      </c>
-      <c r="S23" s="2">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="T23" s="3">
         <v>0.82725519878723419</v>
       </c>
     </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1104,17 +965,10 @@
         <v>20</v>
       </c>
       <c r="O24" s="3">
-        <v>0.74509551410407893</v>
-      </c>
-      <c r="S24" s="2">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="T24" s="3">
         <v>0.78742391426437586</v>
       </c>
     </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1137,17 +991,10 @@
         <v>21</v>
       </c>
       <c r="O25" s="3">
-        <v>0.76642778565008984</v>
-      </c>
-      <c r="S25" s="2">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="T25" s="3">
         <v>0.80218053446485138</v>
       </c>
     </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1170,17 +1017,10 @@
         <v>22</v>
       </c>
       <c r="O26" s="3">
-        <v>0.76718742642304072</v>
-      </c>
-      <c r="S26" s="2">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="T26" s="3">
         <v>0.79450839053483002</v>
       </c>
     </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1203,17 +1043,10 @@
         <v>23</v>
       </c>
       <c r="O27" s="3">
-        <v>0.75424973380895755</v>
-      </c>
-      <c r="S27" s="2">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="T27" s="3">
         <v>0.86202123167247502</v>
       </c>
     </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1236,17 +1069,10 @@
         <v>24</v>
       </c>
       <c r="O28" s="3">
-        <v>0.75307341057087318</v>
-      </c>
-      <c r="S28" s="2">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="T28" s="3">
         <v>0.78195071034764496</v>
       </c>
     </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1269,17 +1095,10 @@
         <v>25</v>
       </c>
       <c r="O29" s="3">
-        <v>0.72056234999534308</v>
-      </c>
-      <c r="S29" s="2">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="T29" s="3">
         <v>0.79314593534820421</v>
       </c>
     </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1302,17 +1121,10 @@
         <v>26</v>
       </c>
       <c r="O30" s="3">
-        <v>0.72554415739991618</v>
-      </c>
-      <c r="S30" s="2">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="T30" s="3">
         <v>0.81402559140618924</v>
       </c>
     </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1335,17 +1147,10 @@
         <v>27</v>
       </c>
       <c r="O31" s="3">
-        <v>0.7626359930255292</v>
-      </c>
-      <c r="S31" s="2">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="T31" s="3">
         <v>0.78820680055015324</v>
       </c>
     </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1368,17 +1173,10 @@
         <v>28</v>
       </c>
       <c r="O32" s="3">
-        <v>0.77240527493968014</v>
-      </c>
-      <c r="S32" s="2">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="T32" s="3">
         <v>0.8178386849140391</v>
       </c>
     </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1401,17 +1199,10 @@
         <v>29</v>
       </c>
       <c r="O33" s="3">
-        <v>0.77538005867413284</v>
-      </c>
-      <c r="S33" s="2">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="T33" s="3">
         <v>0.84278138295276883</v>
       </c>
     </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1434,17 +1225,10 @@
         <v>30</v>
       </c>
       <c r="O34" s="3">
-        <v>0.75390166007005976</v>
-      </c>
-      <c r="S34" s="2">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="T34" s="3">
         <v>0.80607507815925672</v>
       </c>
     </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1467,17 +1251,10 @@
         <v>31</v>
       </c>
       <c r="O35" s="3">
-        <v>0.74711139504130619</v>
-      </c>
-      <c r="S35" s="2">
-        <f t="shared" si="3"/>
-        <v>31</v>
-      </c>
-      <c r="T35" s="3">
         <v>0.82818800642345725</v>
       </c>
     </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1500,17 +1277,10 @@
         <v>32</v>
       </c>
       <c r="O36" s="3">
-        <v>0.72502240747618041</v>
-      </c>
-      <c r="S36" s="2">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="T36" s="3">
         <v>0.81190564529530607</v>
       </c>
     </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1533,17 +1303,10 @@
         <v>33</v>
       </c>
       <c r="O37" s="3">
-        <v>0.71253520940690906</v>
-      </c>
-      <c r="S37" s="2">
-        <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="T37" s="3">
         <v>0.79449826576024463</v>
       </c>
     </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1566,17 +1329,10 @@
         <v>34</v>
       </c>
       <c r="O38" s="3">
-        <v>0.79798960787518869</v>
-      </c>
-      <c r="S38" s="2">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="T38" s="3">
         <v>0.81763901691612373</v>
       </c>
     </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1599,17 +1355,10 @@
         <v>35</v>
       </c>
       <c r="O39" s="3">
-        <v>0.76621468970142592</v>
-      </c>
-      <c r="S39" s="2">
-        <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="T39" s="3">
         <v>0.78509042492134218</v>
       </c>
     </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1632,17 +1381,10 @@
         <v>36</v>
       </c>
       <c r="O40" s="3">
-        <v>0.76014353324770312</v>
-      </c>
-      <c r="S40" s="2">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="T40" s="3">
         <v>0.81191859816540612</v>
       </c>
     </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1665,17 +1407,10 @@
         <v>37</v>
       </c>
       <c r="O41" s="3">
-        <v>0.76665951138330413</v>
-      </c>
-      <c r="S41" s="2">
-        <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="T41" s="3">
         <v>0.75496777019358352</v>
       </c>
     </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1698,17 +1433,10 @@
         <v>38</v>
       </c>
       <c r="O42" s="3">
-        <v>0.77116390542677904</v>
-      </c>
-      <c r="S42" s="2">
-        <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="T42" s="3">
         <v>0.74517830310758759</v>
       </c>
     </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1731,17 +1459,10 @@
         <v>39</v>
       </c>
       <c r="O43" s="3">
-        <v>0.75177730984304492</v>
-      </c>
-      <c r="S43" s="2">
-        <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="T43" s="3">
         <v>0.80147272402531078</v>
       </c>
     </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1764,17 +1485,10 @@
         <v>40</v>
       </c>
       <c r="O44" s="3">
-        <v>0.77197291722174777</v>
-      </c>
-      <c r="S44" s="2">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="T44" s="3">
         <v>0.82840780253290558</v>
       </c>
     </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1797,17 +1511,10 @@
         <v>41</v>
       </c>
       <c r="O45" s="3">
-        <v>0.75155626397156294</v>
-      </c>
-      <c r="S45" s="2">
-        <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="T45" s="3">
         <v>0.77580755396999934</v>
       </c>
     </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1830,17 +1537,10 @@
         <v>42</v>
       </c>
       <c r="O46" s="3">
-        <v>0.75272651768634424</v>
-      </c>
-      <c r="S46" s="2">
-        <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="T46" s="3">
         <v>0.82723461960263767</v>
       </c>
     </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1863,17 +1563,10 @@
         <v>43</v>
       </c>
       <c r="O47" s="3">
-        <v>0.77299045571756364</v>
-      </c>
-      <c r="S47" s="2">
-        <f t="shared" si="3"/>
-        <v>43</v>
-      </c>
-      <c r="T47" s="3">
         <v>0.7972870139940641</v>
       </c>
     </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1896,17 +1589,10 @@
         <v>44</v>
       </c>
       <c r="O48" s="3">
-        <v>0.7332146947029119</v>
-      </c>
-      <c r="S48" s="2">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-      <c r="T48" s="3">
         <v>0.80851865595522121</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1929,17 +1615,10 @@
         <v>45</v>
       </c>
       <c r="O49" s="3">
-        <v>0.70291196689766799</v>
-      </c>
-      <c r="S49" s="2">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="T49" s="3">
         <v>0.79871773121946599</v>
       </c>
     </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1962,17 +1641,10 @@
         <v>46</v>
       </c>
       <c r="O50" s="3">
-        <v>0.78000263064132591</v>
-      </c>
-      <c r="S50" s="2">
-        <f t="shared" si="3"/>
-        <v>46</v>
-      </c>
-      <c r="T50" s="3">
         <v>0.80906595380597757</v>
       </c>
     </row>
-    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1995,17 +1667,10 @@
         <v>47</v>
       </c>
       <c r="O51" s="3">
-        <v>0.73635078630843065</v>
-      </c>
-      <c r="S51" s="2">
-        <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-      <c r="T51" s="3">
         <v>0.81236383469910156</v>
       </c>
     </row>
-    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2028,17 +1693,10 @@
         <v>48</v>
       </c>
       <c r="O52" s="3">
-        <v>0.75421281482107705</v>
-      </c>
-      <c r="S52" s="2">
-        <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="T52" s="3">
         <v>0.76696230705211443</v>
       </c>
     </row>
-    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2061,17 +1719,10 @@
         <v>49</v>
       </c>
       <c r="O53" s="3">
-        <v>0.75278289519513475</v>
-      </c>
-      <c r="S53" s="2">
-        <f t="shared" si="3"/>
-        <v>49</v>
-      </c>
-      <c r="T53" s="3">
         <v>0.83155911174817732</v>
       </c>
     </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2094,17 +1745,10 @@
         <v>50</v>
       </c>
       <c r="O54" s="3">
-        <v>0.76275529405823606</v>
-      </c>
-      <c r="S54" s="2">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="T54" s="3">
         <v>0.84055654148265013</v>
       </c>
     </row>
-    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
@@ -2128,17 +1772,10 @@
       </c>
       <c r="O56" s="3">
         <f>AVERAGE(O5:O54)</f>
-        <v>0.75608400836021072</v>
-      </c>
-      <c r="S56" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="T56" s="3">
-        <f>AVERAGE(T5:T54)</f>
         <v>0.80830834129200924</v>
       </c>
     </row>
-    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
@@ -2162,13 +1799,6 @@
       </c>
       <c r="O57" s="3">
         <f>_xlfn.STDEV.S(O5:O54)</f>
-        <v>2.1434777788001756E-2</v>
-      </c>
-      <c r="S57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T57" s="3">
-        <f>_xlfn.STDEV.S(T5:T54)</f>
         <v>2.3491932191148177E-2</v>
       </c>
     </row>
@@ -8516,7 +8146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test-23: extrapol 2.0 (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -2184,8 +2184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Y57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,7 +2252,9 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3">
+        <v>58789.30188842296</v>
+      </c>
       <c r="M5" s="2">
         <v>1</v>
       </c>
@@ -2287,7 +2289,9 @@
         <f>H5+1</f>
         <v>2</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3">
+        <v>58353.090796718323</v>
+      </c>
       <c r="M6" s="2">
         <f>M5+1</f>
         <v>2</v>
@@ -2325,7 +2329,9 @@
         <f t="shared" ref="H7:H54" si="1">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3">
+        <v>47771.303146399259</v>
+      </c>
       <c r="M7" s="2">
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
@@ -2363,7 +2369,9 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3">
+        <v>49384.22289407473</v>
+      </c>
       <c r="M8" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -2401,7 +2409,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3">
+        <v>52187.876648678197</v>
+      </c>
       <c r="M9" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -2439,7 +2449,9 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3">
+        <v>56394.403604740197</v>
+      </c>
       <c r="M10" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -2477,7 +2489,9 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3">
+        <v>54372.188824065619</v>
+      </c>
       <c r="M11" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -2515,7 +2529,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="3">
+        <v>48378.437620419318</v>
+      </c>
       <c r="M12" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -2553,7 +2569,9 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3">
+        <v>55529.720906107548</v>
+      </c>
       <c r="M13" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -2591,7 +2609,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="3">
+        <v>61876.329092433902</v>
+      </c>
       <c r="M14" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -2629,7 +2649,9 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="3">
+        <v>65716.366343846836</v>
+      </c>
       <c r="M15" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -2667,7 +2689,9 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="3"/>
+      <c r="I16" s="3">
+        <v>60736.560403281663</v>
+      </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -2705,7 +2729,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3">
+        <v>53517.142083865081</v>
+      </c>
       <c r="M17" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -2743,7 +2769,9 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="I18" s="3">
+        <v>55772.388477666347</v>
+      </c>
       <c r="M18" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -2781,7 +2809,9 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="3">
+        <v>64843.628944393793</v>
+      </c>
       <c r="M19" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -2819,7 +2849,9 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3">
+        <v>58095.807893163183</v>
+      </c>
       <c r="M20" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -2857,7 +2889,9 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3">
+        <v>63688.883221877833</v>
+      </c>
       <c r="M21" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -2895,7 +2929,9 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="3">
+        <v>53637.518534184142</v>
+      </c>
       <c r="M22" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -2933,7 +2969,9 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3">
+        <v>48588.413708295353</v>
+      </c>
       <c r="M23" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -2971,7 +3009,9 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I24" s="3"/>
+      <c r="I24" s="3">
+        <v>57697.781987237911</v>
+      </c>
       <c r="M24" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -3009,7 +3049,9 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="3"/>
+      <c r="I25" s="3">
+        <v>47610.993459252502</v>
+      </c>
       <c r="M25" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -3047,7 +3089,9 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3">
+        <v>49567.226243573357</v>
+      </c>
       <c r="M26" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -3085,7 +3129,9 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3">
+        <v>61553.383186144019</v>
+      </c>
       <c r="M27" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -3123,7 +3169,9 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I28" s="3"/>
+      <c r="I28" s="3">
+        <v>46832.874643937997</v>
+      </c>
       <c r="M28" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -3161,7 +3209,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I29" s="3"/>
+      <c r="I29" s="3">
+        <v>57160.73610865997</v>
+      </c>
       <c r="M29" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -3199,7 +3249,9 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I30" s="3"/>
+      <c r="I30" s="3">
+        <v>56281.028445214208</v>
+      </c>
       <c r="M30" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -3237,7 +3289,9 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I31" s="3"/>
+      <c r="I31" s="3">
+        <v>60906.498506472177</v>
+      </c>
       <c r="M31" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -3275,7 +3329,9 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I32" s="3"/>
+      <c r="I32" s="3">
+        <v>58480.290138195072</v>
+      </c>
       <c r="M32" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -3313,7 +3369,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I33" s="3"/>
+      <c r="I33" s="3">
+        <v>53555.518752597993</v>
+      </c>
       <c r="M33" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -3351,7 +3409,9 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I34" s="3"/>
+      <c r="I34" s="3">
+        <v>50678.366734731069</v>
+      </c>
       <c r="M34" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -3389,7 +3449,9 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I35" s="3"/>
+      <c r="I35" s="3">
+        <v>53909.591462898803</v>
+      </c>
       <c r="M35" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -3427,7 +3489,9 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I36" s="3"/>
+      <c r="I36" s="3">
+        <v>44975.392831358236</v>
+      </c>
       <c r="M36" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -3465,7 +3529,9 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I37" s="3"/>
+      <c r="I37" s="3">
+        <v>46166.058468915209</v>
+      </c>
       <c r="M37" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -3503,7 +3569,9 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I38" s="3"/>
+      <c r="I38" s="3">
+        <v>47622.842572834998</v>
+      </c>
       <c r="M38" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -3541,7 +3609,9 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I39" s="3"/>
+      <c r="I39" s="3">
+        <v>51473.153155515029</v>
+      </c>
       <c r="M39" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -3579,7 +3649,9 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I40" s="3"/>
+      <c r="I40" s="3">
+        <v>53315.195839197797</v>
+      </c>
       <c r="M40" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -3617,7 +3689,9 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I41" s="3"/>
+      <c r="I41" s="3">
+        <v>65478.192139288949</v>
+      </c>
       <c r="M41" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -3655,7 +3729,9 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I42" s="3"/>
+      <c r="I42" s="3">
+        <v>57196.846229717397</v>
+      </c>
       <c r="M42" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -3693,7 +3769,9 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I43" s="3"/>
+      <c r="I43" s="3">
+        <v>49758.585839562438</v>
+      </c>
       <c r="M43" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -3731,7 +3809,9 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I44" s="3"/>
+      <c r="I44" s="3">
+        <v>52729.098355150403</v>
+      </c>
       <c r="M44" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -3769,7 +3849,9 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I45" s="3"/>
+      <c r="I45" s="3">
+        <v>46374.834440109393</v>
+      </c>
       <c r="M45" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -3807,7 +3889,9 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I46" s="3"/>
+      <c r="I46" s="3">
+        <v>59935.955940929802</v>
+      </c>
       <c r="M46" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -3845,7 +3929,9 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I47" s="3"/>
+      <c r="I47" s="3">
+        <v>52550.335505195988</v>
+      </c>
       <c r="M47" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -3883,7 +3969,9 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I48" s="3"/>
+      <c r="I48" s="3">
+        <v>50068.88495314493</v>
+      </c>
       <c r="M48" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -3921,7 +4009,9 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I49" s="3"/>
+      <c r="I49" s="3">
+        <v>53130.362081312662</v>
+      </c>
       <c r="M49" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -3959,7 +4049,9 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I50" s="3"/>
+      <c r="I50" s="3">
+        <v>58535.611685323602</v>
+      </c>
       <c r="M50" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -3997,7 +4089,9 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I51" s="3"/>
+      <c r="I51" s="3">
+        <v>49339.398987055603</v>
+      </c>
       <c r="M51" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4035,7 +4129,9 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I52" s="3"/>
+      <c r="I52" s="3">
+        <v>57632.969994530533</v>
+      </c>
       <c r="M52" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -4073,7 +4169,9 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I53" s="3"/>
+      <c r="I53" s="3">
+        <v>59948.99582825887</v>
+      </c>
       <c r="M53" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -4111,7 +4209,9 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I54" s="3"/>
+      <c r="I54" s="3">
+        <v>54918.069017684589</v>
+      </c>
       <c r="M54" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -4149,9 +4249,9 @@
       <c r="H56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I56" s="3" t="e">
+      <c r="I56" s="3">
         <f>AVERAGE(I5:I54)</f>
-        <v>#DIV/0!</v>
+        <v>54660.3731713327</v>
       </c>
       <c r="M56" s="2" t="s">
         <v>3</v>
@@ -4190,9 +4290,9 @@
       <c r="H57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I57" s="3" t="e">
+      <c r="I57" s="3">
         <f>_xlfn.STDEV.S(I5:I54)</f>
-        <v>#DIV/0!</v>
+        <v>5460.6045760079778</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
test-23: hybrid model 2.0 (r2)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -56,9 +56,6 @@
     <t>test (MSE)</t>
   </si>
   <si>
-    <t>RF-100 (superdataset-24-f 2Ysum.csv + extrapol)</t>
-  </si>
-  <si>
     <t>train (MAE)</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>RF-100 (superdataset-24-f.csv + extrapol 2.0)</t>
+  </si>
+  <si>
+    <t>Hybrid model 2.0 (superdataset-24-f + 2Y.csv)</t>
   </si>
 </sst>
 </file>
@@ -108,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,13 +134,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -417,30 +431,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T57"/>
+  <dimension ref="C3:Y57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="J3" s="5"/>
       <c r="N3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="5"/>
+      <c r="X3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>1</v>
@@ -448,20 +467,24 @@
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2" t="s">
+      <c r="S4" s="6"/>
+      <c r="T4" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -471,10 +494,10 @@
       <c r="E5" s="3">
         <v>0.48158352219436151</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="6">
         <v>1</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="7">
         <v>0.7328261160883589</v>
       </c>
       <c r="N5" s="2">
@@ -483,14 +506,20 @@
       <c r="O5" s="3">
         <v>0.48585768673676921</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="6">
         <v>1</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="7">
         <v>0.77416454041178173</v>
       </c>
-    </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0.53787943050918186</v>
+      </c>
+    </row>
+    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -501,11 +530,11 @@
       <c r="E6" s="3">
         <v>0.51374867566029625</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="6">
         <f>I5+1</f>
         <v>2</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="7">
         <v>0.81156795793393999</v>
       </c>
       <c r="N6" s="2">
@@ -515,15 +544,22 @@
       <c r="O6" s="3">
         <v>0.46997684088905922</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="6">
         <f>S5+1</f>
         <v>2</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="7">
         <v>0.81470395155608155</v>
       </c>
-    </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X6" s="2">
+        <f>X5+1</f>
+        <v>2</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0.52172195277324573</v>
+      </c>
+    </row>
+    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -534,11 +570,11 @@
       <c r="E7" s="3">
         <v>0.53398838623476363</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="6">
         <f t="shared" ref="I7:I54" si="1">I6+1</f>
         <v>3</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="7">
         <v>0.78895231922312026</v>
       </c>
       <c r="N7" s="2">
@@ -548,15 +584,22 @@
       <c r="O7" s="3">
         <v>0.48664350879027718</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="6">
         <f t="shared" ref="S7:S54" si="3">S6+1</f>
         <v>3</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7" s="7">
         <v>0.79668886926260762</v>
       </c>
-    </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X7" s="2">
+        <f t="shared" ref="X7:X54" si="4">X6+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0.49471750653135321</v>
+      </c>
+    </row>
+    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -567,11 +610,11 @@
       <c r="E8" s="3">
         <v>0.53561266794425677</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="7">
         <v>0.83283066195875255</v>
       </c>
       <c r="N8" s="2">
@@ -581,15 +624,22 @@
       <c r="O8" s="3">
         <v>0.4911794151504556</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="7">
         <v>0.82680697690012384</v>
       </c>
-    </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X8" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0.54547642738241164</v>
+      </c>
+    </row>
+    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -600,11 +650,11 @@
       <c r="E9" s="3">
         <v>0.45748876950753081</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="7">
         <v>0.77883834797005469</v>
       </c>
       <c r="N9" s="2">
@@ -614,15 +664,22 @@
       <c r="O9" s="3">
         <v>0.51324110796766143</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="7">
         <v>0.79599042243084228</v>
       </c>
-    </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X9" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0.54283617759121294</v>
+      </c>
+    </row>
+    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -633,11 +690,11 @@
       <c r="E10" s="3">
         <v>0.48381749646353017</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="7">
         <v>0.76571336575083537</v>
       </c>
       <c r="N10" s="2">
@@ -647,15 +704,22 @@
       <c r="O10" s="3">
         <v>0.47885978766596859</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S10" s="6">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10" s="7">
         <v>0.81328937809939206</v>
       </c>
-    </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X10" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0.54215700625694019</v>
+      </c>
+    </row>
+    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -666,11 +730,11 @@
       <c r="E11" s="3">
         <v>0.53083944161761398</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="7">
         <v>0.77190474471957016</v>
       </c>
       <c r="N11" s="2">
@@ -680,15 +744,22 @@
       <c r="O11" s="3">
         <v>0.46104827381552521</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11" s="6">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11" s="7">
         <v>0.84615624245033449</v>
       </c>
-    </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X11" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>0.50084309543214212</v>
+      </c>
+    </row>
+    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -699,11 +770,11 @@
       <c r="E12" s="3">
         <v>0.48766686221497091</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="7">
         <v>0.74143615641260419</v>
       </c>
       <c r="N12" s="2">
@@ -713,15 +784,22 @@
       <c r="O12" s="3">
         <v>0.49597654320565537</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12" s="6">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="T12" s="3">
+      <c r="T12" s="7">
         <v>0.82600602571101966</v>
       </c>
-    </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X12" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>0.56350555319978346</v>
+      </c>
+    </row>
+    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -732,11 +810,11 @@
       <c r="E13" s="3">
         <v>0.50731254894258271</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="7">
         <v>0.81948870997368461</v>
       </c>
       <c r="N13" s="2">
@@ -746,15 +824,22 @@
       <c r="O13" s="3">
         <v>0.5312650729883327</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13" s="6">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13" s="7">
         <v>0.84772188847685637</v>
       </c>
-    </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X13" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>0.50400362772184892</v>
+      </c>
+    </row>
+    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -765,11 +850,11 @@
       <c r="E14" s="3">
         <v>0.48798875019573951</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="7">
         <v>0.77034405579522025</v>
       </c>
       <c r="N14" s="2">
@@ -779,15 +864,22 @@
       <c r="O14" s="3">
         <v>0.49799316943206812</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="6">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="T14" s="3">
+      <c r="T14" s="7">
         <v>0.78644683967295803</v>
       </c>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X14" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>0.55313527786981698</v>
+      </c>
+    </row>
+    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -798,11 +890,11 @@
       <c r="E15" s="3">
         <v>0.49795235066818172</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="6">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="7">
         <v>0.79758876088385089</v>
       </c>
       <c r="N15" s="2">
@@ -812,15 +904,22 @@
       <c r="O15" s="3">
         <v>0.50932067816428583</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15" s="6">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T15" s="7">
         <v>0.81561038790464979</v>
       </c>
-    </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X15" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>0.55126871946140332</v>
+      </c>
+    </row>
+    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -831,11 +930,11 @@
       <c r="E16" s="3">
         <v>0.51559911271845593</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="6">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="7">
         <v>0.76195408003286547</v>
       </c>
       <c r="N16" s="2">
@@ -845,15 +944,22 @@
       <c r="O16" s="3">
         <v>0.48578728884047379</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="6">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="T16" s="3">
+      <c r="T16" s="7">
         <v>0.81301942736522181</v>
       </c>
-    </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X16" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>0.51994740280510632</v>
+      </c>
+    </row>
+    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -864,11 +970,11 @@
       <c r="E17" s="3">
         <v>0.50873136960700849</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="7">
         <v>0.74964674834410983</v>
       </c>
       <c r="N17" s="2">
@@ -878,15 +984,22 @@
       <c r="O17" s="3">
         <v>0.49391616859276533</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17" s="6">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="T17" s="3">
+      <c r="T17" s="7">
         <v>0.81317080735560143</v>
       </c>
-    </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X17" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0.54879976287117405</v>
+      </c>
+    </row>
+    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -897,11 +1010,11 @@
       <c r="E18" s="3">
         <v>0.51909231727920913</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="6">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="7">
         <v>0.75346932384082188</v>
       </c>
       <c r="N18" s="2">
@@ -911,15 +1024,22 @@
       <c r="O18" s="3">
         <v>0.45214439222312408</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S18" s="6">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="T18" s="3">
+      <c r="T18" s="7">
         <v>0.81435946408164983</v>
       </c>
-    </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X18" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0.52691030365813596</v>
+      </c>
+    </row>
+    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -930,11 +1050,11 @@
       <c r="E19" s="3">
         <v>0.48324327911865861</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="6">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="7">
         <v>0.78668206422229736</v>
       </c>
       <c r="N19" s="2">
@@ -944,15 +1064,22 @@
       <c r="O19" s="3">
         <v>0.46823202444304679</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S19" s="6">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="T19" s="3">
+      <c r="T19" s="7">
         <v>0.82837639320219147</v>
       </c>
-    </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X19" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>0.49729418702305561</v>
+      </c>
+    </row>
+    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -963,11 +1090,11 @@
       <c r="E20" s="3">
         <v>0.53677297537956636</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="6">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="7">
         <v>0.75543843228912744</v>
       </c>
       <c r="N20" s="2">
@@ -977,15 +1104,22 @@
       <c r="O20" s="3">
         <v>0.50382976988217476</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S20" s="6">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="T20" s="3">
+      <c r="T20" s="7">
         <v>0.79600110005296199</v>
       </c>
-    </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X20" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0.48405284357378098</v>
+      </c>
+    </row>
+    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -996,11 +1130,11 @@
       <c r="E21" s="3">
         <v>0.54593808844202818</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="7">
         <v>0.78173828401931256</v>
       </c>
       <c r="N21" s="2">
@@ -1010,15 +1144,22 @@
       <c r="O21" s="3">
         <v>0.50292562220898707</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S21" s="6">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="T21" s="3">
+      <c r="T21" s="7">
         <v>0.83485973930006085</v>
       </c>
-    </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X21" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>0.56535689798466282</v>
+      </c>
+    </row>
+    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1029,11 +1170,11 @@
       <c r="E22" s="3">
         <v>0.5126328686153625</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="7">
         <v>0.7927907612647439</v>
       </c>
       <c r="N22" s="2">
@@ -1043,15 +1184,22 @@
       <c r="O22" s="3">
         <v>0.466232870566619</v>
       </c>
-      <c r="S22" s="2">
+      <c r="S22" s="6">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="T22" s="3">
+      <c r="T22" s="7">
         <v>0.80729127609344387</v>
       </c>
-    </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X22" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0.54759831330009612</v>
+      </c>
+    </row>
+    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1062,11 +1210,11 @@
       <c r="E23" s="3">
         <v>0.50504173424329535</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="6">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="7">
         <v>0.7992002650369554</v>
       </c>
       <c r="N23" s="2">
@@ -1076,15 +1224,22 @@
       <c r="O23" s="3">
         <v>0.44496206822140139</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S23" s="6">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="T23" s="3">
+      <c r="T23" s="7">
         <v>0.82725519878723419</v>
       </c>
-    </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X23" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>0.51000316296569659</v>
+      </c>
+    </row>
+    <row r="24" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1095,11 +1250,11 @@
       <c r="E24" s="3">
         <v>0.54118422614498574</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="6">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="7">
         <v>0.79576976186300852</v>
       </c>
       <c r="N24" s="2">
@@ -1109,15 +1264,22 @@
       <c r="O24" s="3">
         <v>0.45463727043787749</v>
       </c>
-      <c r="S24" s="2">
+      <c r="S24" s="6">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="T24" s="3">
+      <c r="T24" s="7">
         <v>0.78742391426437586</v>
       </c>
-    </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X24" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>0.50706054677830492</v>
+      </c>
+    </row>
+    <row r="25" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1128,11 +1290,11 @@
       <c r="E25" s="3">
         <v>0.52363980369992436</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="6">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="7">
         <v>0.75158070984674707</v>
       </c>
       <c r="N25" s="2">
@@ -1142,15 +1304,22 @@
       <c r="O25" s="3">
         <v>0.51684732825614099</v>
       </c>
-      <c r="S25" s="2">
+      <c r="S25" s="6">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="T25" s="3">
+      <c r="T25" s="7">
         <v>0.80218053446485138</v>
       </c>
-    </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X25" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>0.55051465627433016</v>
+      </c>
+    </row>
+    <row r="26" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1161,11 +1330,11 @@
       <c r="E26" s="3">
         <v>0.47924862956313141</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="6">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="7">
         <v>0.7800408627700568</v>
       </c>
       <c r="N26" s="2">
@@ -1175,15 +1344,22 @@
       <c r="O26" s="3">
         <v>0.53633519266939189</v>
       </c>
-      <c r="S26" s="2">
+      <c r="S26" s="6">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="T26" s="3">
+      <c r="T26" s="7">
         <v>0.79450839053483002</v>
       </c>
-    </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X26" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>0.48395963834496991</v>
+      </c>
+    </row>
+    <row r="27" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1194,11 +1370,11 @@
       <c r="E27" s="3">
         <v>0.52125520804731207</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="6">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="7">
         <v>0.77870660781914558</v>
       </c>
       <c r="N27" s="2">
@@ -1208,15 +1384,22 @@
       <c r="O27" s="3">
         <v>0.45876194671857418</v>
       </c>
-      <c r="S27" s="2">
+      <c r="S27" s="6">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="T27" s="3">
+      <c r="T27" s="7">
         <v>0.86202123167247502</v>
       </c>
-    </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X27" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="Y27" s="3">
+        <v>0.54816126020368983</v>
+      </c>
+    </row>
+    <row r="28" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1227,11 +1410,11 @@
       <c r="E28" s="3">
         <v>0.49940020845842881</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="6">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="7">
         <v>0.76174899013519481</v>
       </c>
       <c r="N28" s="2">
@@ -1241,15 +1424,22 @@
       <c r="O28" s="3">
         <v>0.50084267925145642</v>
       </c>
-      <c r="S28" s="2">
+      <c r="S28" s="6">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="T28" s="3">
+      <c r="T28" s="7">
         <v>0.78195071034764496</v>
       </c>
-    </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X28" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>0.5769788282568078</v>
+      </c>
+    </row>
+    <row r="29" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1260,11 +1450,11 @@
       <c r="E29" s="3">
         <v>0.53843839502352986</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="6">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="7">
         <v>0.77091959415287703</v>
       </c>
       <c r="N29" s="2">
@@ -1274,15 +1464,22 @@
       <c r="O29" s="3">
         <v>0.463510866312148</v>
       </c>
-      <c r="S29" s="2">
+      <c r="S29" s="6">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="T29" s="3">
+      <c r="T29" s="7">
         <v>0.79314593534820421</v>
       </c>
-    </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X29" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>0.45429005423941338</v>
+      </c>
+    </row>
+    <row r="30" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1293,11 +1490,11 @@
       <c r="E30" s="3">
         <v>0.54402084820828944</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="6">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="7">
         <v>0.77427505679205644</v>
       </c>
       <c r="N30" s="2">
@@ -1307,15 +1504,22 @@
       <c r="O30" s="3">
         <v>0.48758900905594549</v>
       </c>
-      <c r="S30" s="2">
+      <c r="S30" s="6">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="T30" s="3">
+      <c r="T30" s="7">
         <v>0.81402559140618924</v>
       </c>
-    </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X30" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>0.5703702240767472</v>
+      </c>
+    </row>
+    <row r="31" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1326,11 +1530,11 @@
       <c r="E31" s="3">
         <v>0.52084507191612883</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="7">
         <v>0.75058708408046437</v>
       </c>
       <c r="N31" s="2">
@@ -1340,15 +1544,22 @@
       <c r="O31" s="3">
         <v>0.47976955269481703</v>
       </c>
-      <c r="S31" s="2">
+      <c r="S31" s="6">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="T31" s="3">
+      <c r="T31" s="7">
         <v>0.78820680055015324</v>
       </c>
-    </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X31" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>0.52202914394533373</v>
+      </c>
+    </row>
+    <row r="32" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1359,11 +1570,11 @@
       <c r="E32" s="3">
         <v>0.52333816497346608</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="6">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="7">
         <v>0.80091715014380749</v>
       </c>
       <c r="N32" s="2">
@@ -1373,15 +1584,22 @@
       <c r="O32" s="3">
         <v>0.45655899437112157</v>
       </c>
-      <c r="S32" s="2">
+      <c r="S32" s="6">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="T32" s="3">
+      <c r="T32" s="7">
         <v>0.8178386849140391</v>
       </c>
-    </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X32" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="Y32" s="3">
+        <v>0.5031900619279589</v>
+      </c>
+    </row>
+    <row r="33" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1392,11 +1610,11 @@
       <c r="E33" s="3">
         <v>0.48551896960273833</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="6">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="7">
         <v>0.79280340328115162</v>
       </c>
       <c r="N33" s="2">
@@ -1406,15 +1624,22 @@
       <c r="O33" s="3">
         <v>0.43071576656378269</v>
       </c>
-      <c r="S33" s="2">
+      <c r="S33" s="6">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="T33" s="3">
+      <c r="T33" s="7">
         <v>0.84278138295276883</v>
       </c>
-    </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X33" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="Y33" s="3">
+        <v>0.51129780489923193</v>
+      </c>
+    </row>
+    <row r="34" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1425,11 +1650,11 @@
       <c r="E34" s="3">
         <v>0.49931852176302838</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="6">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="7">
         <v>0.73302701977319129</v>
       </c>
       <c r="N34" s="2">
@@ -1439,15 +1664,22 @@
       <c r="O34" s="3">
         <v>0.54633640060438782</v>
       </c>
-      <c r="S34" s="2">
+      <c r="S34" s="6">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="T34" s="3">
+      <c r="T34" s="7">
         <v>0.80607507815925672</v>
       </c>
-    </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X34" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="Y34" s="3">
+        <v>0.54175671058825792</v>
+      </c>
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1458,11 +1690,11 @@
       <c r="E35" s="3">
         <v>0.5292294032568301</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="6">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="7">
         <v>0.76039576791459251</v>
       </c>
       <c r="N35" s="2">
@@ -1472,15 +1704,22 @@
       <c r="O35" s="3">
         <v>0.48302705720169897</v>
       </c>
-      <c r="S35" s="2">
+      <c r="S35" s="6">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="T35" s="3">
+      <c r="T35" s="7">
         <v>0.82818800642345725</v>
       </c>
-    </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X35" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="Y35" s="3">
+        <v>0.5146972282291733</v>
+      </c>
+    </row>
+    <row r="36" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1491,11 +1730,11 @@
       <c r="E36" s="3">
         <v>0.53820389859832418</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="6">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="7">
         <v>0.78802817783949064</v>
       </c>
       <c r="N36" s="2">
@@ -1505,15 +1744,22 @@
       <c r="O36" s="3">
         <v>0.50711215180208413</v>
       </c>
-      <c r="S36" s="2">
+      <c r="S36" s="6">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="T36" s="3">
+      <c r="T36" s="7">
         <v>0.81190564529530607</v>
       </c>
-    </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X36" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="Y36" s="3">
+        <v>0.52965157818399633</v>
+      </c>
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1524,11 +1770,11 @@
       <c r="E37" s="3">
         <v>0.50577583149120409</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="6">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="7">
         <v>0.81305402062467935</v>
       </c>
       <c r="N37" s="2">
@@ -1538,15 +1784,22 @@
       <c r="O37" s="3">
         <v>0.46186551164474271</v>
       </c>
-      <c r="S37" s="2">
+      <c r="S37" s="6">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="T37" s="3">
+      <c r="T37" s="7">
         <v>0.79449826576024463</v>
       </c>
-    </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X37" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="Y37" s="3">
+        <v>0.5197008813327052</v>
+      </c>
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1557,11 +1810,11 @@
       <c r="E38" s="3">
         <v>0.48600758598846161</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="6">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="7">
         <v>0.68953577597343774</v>
       </c>
       <c r="N38" s="2">
@@ -1571,15 +1824,22 @@
       <c r="O38" s="3">
         <v>0.46607125704649782</v>
       </c>
-      <c r="S38" s="2">
+      <c r="S38" s="6">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="T38" s="3">
+      <c r="T38" s="7">
         <v>0.81763901691612373</v>
       </c>
-    </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X38" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="Y38" s="3">
+        <v>0.56916195669869762</v>
+      </c>
+    </row>
+    <row r="39" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1590,11 +1850,11 @@
       <c r="E39" s="3">
         <v>0.53388510925371924</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="6">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="7">
         <v>0.81338973318411723</v>
       </c>
       <c r="N39" s="2">
@@ -1604,15 +1864,22 @@
       <c r="O39" s="3">
         <v>0.46052487800813419</v>
       </c>
-      <c r="S39" s="2">
+      <c r="S39" s="6">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="T39" s="3">
+      <c r="T39" s="7">
         <v>0.78509042492134218</v>
       </c>
-    </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X39" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="Y39" s="3">
+        <v>0.51188398274966307</v>
+      </c>
+    </row>
+    <row r="40" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1623,11 +1890,11 @@
       <c r="E40" s="3">
         <v>0.52663097730093922</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="6">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="7">
         <v>0.78162820883950246</v>
       </c>
       <c r="N40" s="2">
@@ -1637,15 +1904,22 @@
       <c r="O40" s="3">
         <v>0.47061413133913482</v>
       </c>
-      <c r="S40" s="2">
+      <c r="S40" s="6">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="T40" s="3">
+      <c r="T40" s="7">
         <v>0.81191859816540612</v>
       </c>
-    </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X40" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="Y40" s="3">
+        <v>0.54364056797771576</v>
+      </c>
+    </row>
+    <row r="41" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1656,11 +1930,11 @@
       <c r="E41" s="3">
         <v>0.51237572861077141</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="6">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="7">
         <v>0.76374453810411369</v>
       </c>
       <c r="N41" s="2">
@@ -1670,15 +1944,22 @@
       <c r="O41" s="3">
         <v>0.487191274033967</v>
       </c>
-      <c r="S41" s="2">
+      <c r="S41" s="6">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="T41" s="3">
+      <c r="T41" s="7">
         <v>0.75496777019358352</v>
       </c>
-    </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X41" s="2">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>0.51731063290640233</v>
+      </c>
+    </row>
+    <row r="42" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1689,11 +1970,11 @@
       <c r="E42" s="3">
         <v>0.47810807611232747</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="6">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="7">
         <v>0.7745329274249132</v>
       </c>
       <c r="N42" s="2">
@@ -1703,15 +1984,22 @@
       <c r="O42" s="3">
         <v>0.50167664290008862</v>
       </c>
-      <c r="S42" s="2">
+      <c r="S42" s="6">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="T42" s="3">
+      <c r="T42" s="7">
         <v>0.74517830310758759</v>
       </c>
-    </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X42" s="2">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="Y42" s="3">
+        <v>0.52299393862923738</v>
+      </c>
+    </row>
+    <row r="43" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1722,11 +2010,11 @@
       <c r="E43" s="3">
         <v>0.49101890834140161</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="6">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="7">
         <v>0.78949950132067181</v>
       </c>
       <c r="N43" s="2">
@@ -1736,15 +2024,22 @@
       <c r="O43" s="3">
         <v>0.48094964727964201</v>
       </c>
-      <c r="S43" s="2">
+      <c r="S43" s="6">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="T43" s="3">
+      <c r="T43" s="7">
         <v>0.80147272402531078</v>
       </c>
-    </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X43" s="2">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="Y43" s="3">
+        <v>0.50869794921009204</v>
+      </c>
+    </row>
+    <row r="44" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1755,11 +2050,11 @@
       <c r="E44" s="3">
         <v>0.46302753934504709</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="6">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="7">
         <v>0.78153021711246362</v>
       </c>
       <c r="N44" s="2">
@@ -1769,15 +2064,22 @@
       <c r="O44" s="3">
         <v>0.50316650328602031</v>
       </c>
-      <c r="S44" s="2">
+      <c r="S44" s="6">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="T44" s="3">
+      <c r="T44" s="7">
         <v>0.82840780253290558</v>
       </c>
-    </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X44" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="Y44" s="3">
+        <v>0.52404916108462807</v>
+      </c>
+    </row>
+    <row r="45" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1788,11 +2090,11 @@
       <c r="E45" s="3">
         <v>0.55389486553546741</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="6">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="7">
         <v>0.75739746440256905</v>
       </c>
       <c r="N45" s="2">
@@ -1802,15 +2104,22 @@
       <c r="O45" s="3">
         <v>0.5052569476747234</v>
       </c>
-      <c r="S45" s="2">
+      <c r="S45" s="6">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="T45" s="3">
+      <c r="T45" s="7">
         <v>0.77580755396999934</v>
       </c>
-    </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X45" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="Y45" s="3">
+        <v>0.57016482871192276</v>
+      </c>
+    </row>
+    <row r="46" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1821,11 +2130,11 @@
       <c r="E46" s="3">
         <v>0.51485494765265138</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="6">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="7">
         <v>0.77051436374736282</v>
       </c>
       <c r="N46" s="2">
@@ -1835,15 +2144,22 @@
       <c r="O46" s="3">
         <v>0.52906844598753511</v>
       </c>
-      <c r="S46" s="2">
+      <c r="S46" s="6">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="T46" s="3">
+      <c r="T46" s="7">
         <v>0.82723461960263767</v>
       </c>
-    </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X46" s="2">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="Y46" s="3">
+        <v>0.54780157430407894</v>
+      </c>
+    </row>
+    <row r="47" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1854,11 +2170,11 @@
       <c r="E47" s="3">
         <v>0.50449484961317359</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="6">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="7">
         <v>0.7815408127343475</v>
       </c>
       <c r="N47" s="2">
@@ -1868,15 +2184,22 @@
       <c r="O47" s="3">
         <v>0.48271053502059069</v>
       </c>
-      <c r="S47" s="2">
+      <c r="S47" s="6">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="T47" s="3">
+      <c r="T47" s="7">
         <v>0.7972870139940641</v>
       </c>
-    </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X47" s="2">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="Y47" s="3">
+        <v>0.52421133472147807</v>
+      </c>
+    </row>
+    <row r="48" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1887,11 +2210,11 @@
       <c r="E48" s="3">
         <v>0.4850380192935817</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="6">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="7">
         <v>0.75794159724765886</v>
       </c>
       <c r="N48" s="2">
@@ -1901,15 +2224,22 @@
       <c r="O48" s="3">
         <v>0.46552741001835329</v>
       </c>
-      <c r="S48" s="2">
+      <c r="S48" s="6">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="T48" s="3">
+      <c r="T48" s="7">
         <v>0.80851865595522121</v>
       </c>
-    </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X48" s="2">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="Y48" s="3">
+        <v>0.52073423792576179</v>
+      </c>
+    </row>
+    <row r="49" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1920,11 +2250,11 @@
       <c r="E49" s="3">
         <v>0.51056899530882083</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="6">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="7">
         <v>0.7767275661938231</v>
       </c>
       <c r="N49" s="2">
@@ -1934,15 +2264,22 @@
       <c r="O49" s="3">
         <v>0.44845145212877752</v>
       </c>
-      <c r="S49" s="2">
+      <c r="S49" s="6">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="T49" s="3">
+      <c r="T49" s="7">
         <v>0.79871773121946599</v>
       </c>
-    </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X49" s="2">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="Y49" s="3">
+        <v>0.54273209415494361</v>
+      </c>
+    </row>
+    <row r="50" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1953,11 +2290,11 @@
       <c r="E50" s="3">
         <v>0.52226631985304439</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I50" s="6">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="7">
         <v>0.78347363738138953</v>
       </c>
       <c r="N50" s="2">
@@ -1967,15 +2304,22 @@
       <c r="O50" s="3">
         <v>0.48215744357236662</v>
       </c>
-      <c r="S50" s="2">
+      <c r="S50" s="6">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="T50" s="3">
+      <c r="T50" s="7">
         <v>0.80906595380597757</v>
       </c>
-    </row>
-    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X50" s="2">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="Y50" s="3">
+        <v>0.56409021685949856</v>
+      </c>
+    </row>
+    <row r="51" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1986,11 +2330,11 @@
       <c r="E51" s="3">
         <v>0.56792770501704881</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="6">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="7">
         <v>0.78451508270848291</v>
       </c>
       <c r="N51" s="2">
@@ -2000,15 +2344,22 @@
       <c r="O51" s="3">
         <v>0.49192473491481659</v>
       </c>
-      <c r="S51" s="2">
+      <c r="S51" s="6">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="T51" s="3">
+      <c r="T51" s="7">
         <v>0.81236383469910156</v>
       </c>
-    </row>
-    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X51" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="Y51" s="3">
+        <v>0.5109538848187547</v>
+      </c>
+    </row>
+    <row r="52" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2019,11 +2370,11 @@
       <c r="E52" s="3">
         <v>0.52142898800581849</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I52" s="6">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="7">
         <v>0.7571682834862079</v>
       </c>
       <c r="N52" s="2">
@@ -2033,15 +2384,22 @@
       <c r="O52" s="3">
         <v>0.48957236403586218</v>
       </c>
-      <c r="S52" s="2">
+      <c r="S52" s="6">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="T52" s="3">
+      <c r="T52" s="7">
         <v>0.76696230705211443</v>
       </c>
-    </row>
-    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X52" s="2">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="Y52" s="3">
+        <v>0.51229020436857264</v>
+      </c>
+    </row>
+    <row r="53" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2052,11 +2410,11 @@
       <c r="E53" s="3">
         <v>0.5658557211999734</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I53" s="6">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="7">
         <v>0.79481763168054775</v>
       </c>
       <c r="N53" s="2">
@@ -2066,15 +2424,22 @@
       <c r="O53" s="3">
         <v>0.45088991236579973</v>
       </c>
-      <c r="S53" s="2">
+      <c r="S53" s="6">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="T53" s="3">
+      <c r="T53" s="7">
         <v>0.83155911174817732</v>
       </c>
-    </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X53" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="Y53" s="3">
+        <v>0.46749914939390169</v>
+      </c>
+    </row>
+    <row r="54" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2085,11 +2450,11 @@
       <c r="E54" s="3">
         <v>0.51379303350812111</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I54" s="6">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="7">
         <v>0.77251168034336959</v>
       </c>
       <c r="N54" s="2">
@@ -2099,15 +2464,28 @@
       <c r="O54" s="3">
         <v>0.5094821033282888</v>
       </c>
-      <c r="S54" s="2">
+      <c r="S54" s="6">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="T54" s="3">
+      <c r="T54" s="7">
         <v>0.84055654148265013</v>
       </c>
-    </row>
-    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X54" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="Y54" s="3">
+        <v>0.55868754229778328</v>
+      </c>
+    </row>
+    <row r="55" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+    </row>
+    <row r="56" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
@@ -2119,10 +2497,10 @@
         <f>AVERAGE(E5:E54)</f>
         <v>0.51291291535470207</v>
       </c>
-      <c r="I56" s="2" t="s">
+      <c r="I56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="7">
         <f>AVERAGE(J5:J54)</f>
         <v>0.77549468769363328</v>
       </c>
@@ -2133,15 +2511,22 @@
         <f>AVERAGE(O5:O54)</f>
         <v>0.4849707540061885</v>
       </c>
-      <c r="S56" s="2" t="s">
+      <c r="S56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="T56" s="3">
+      <c r="T56" s="7">
         <f>AVERAGE(T5:T54)</f>
         <v>0.80830834129200924</v>
       </c>
-    </row>
-    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y56" s="3">
+        <f>AVERAGE(Y5:Y54)</f>
+        <v>0.52816139046010202</v>
+      </c>
+    </row>
+    <row r="57" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
@@ -2153,10 +2538,10 @@
         <f>_xlfn.STDEV.S(E5:E54)</f>
         <v>2.4908626127406807E-2</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="I57" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="7">
         <f>_xlfn.STDEV.S(J5:J54)</f>
         <v>2.4855103371876817E-2</v>
       </c>
@@ -2167,12 +2552,19 @@
         <f>_xlfn.STDEV.S(O5:O54)</f>
         <v>2.5163949660280679E-2</v>
       </c>
-      <c r="S57" s="2" t="s">
+      <c r="S57" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="T57" s="3">
+      <c r="T57" s="7">
         <f>_xlfn.STDEV.S(T5:T54)</f>
         <v>2.3491932191148177E-2</v>
+      </c>
+      <c r="X57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y57" s="3">
+        <f>_xlfn.STDEV.S(Y5:Y54)</f>
+        <v>2.7516935600987003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2182,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:Y57"/>
+  <dimension ref="C3:AD57"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,26 +2587,32 @@
     <col min="20" max="20" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="R3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="X3" s="1" t="s">
+      <c r="S3" s="5"/>
+      <c r="T3" s="1"/>
+      <c r="W3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" s="5"/>
+      <c r="AC3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AD3" s="5"/>
+    </row>
+    <row r="4" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -2230,16 +2628,20 @@
       <c r="N4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2" t="s">
+      <c r="W4" s="6"/>
+      <c r="X4" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -2258,23 +2660,27 @@
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="3"/>
+      <c r="R5" s="6">
+        <v>1</v>
+      </c>
+      <c r="S5" s="7">
         <v>19988.180811262479</v>
       </c>
-      <c r="R5" s="2">
+      <c r="W5" s="6">
         <v>1</v>
       </c>
-      <c r="S5" s="3">
+      <c r="X5" s="7">
         <v>34502.219893551322</v>
       </c>
-      <c r="X5" s="2">
+      <c r="AC5" s="6">
         <v>1</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="AD5" s="7">
         <v>21663.98982334241</v>
       </c>
     </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -2296,25 +2702,30 @@
         <f>M5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="3">
-        <v>25762.852665213439</v>
-      </c>
-      <c r="R6" s="2">
+      <c r="N6" s="3"/>
+      <c r="R6" s="6">
         <f>R5+1</f>
         <v>2</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="7">
+        <v>25762.852665213439</v>
+      </c>
+      <c r="W6" s="6">
+        <f>W5+1</f>
+        <v>2</v>
+      </c>
+      <c r="X6" s="7">
         <v>25575.293685376921</v>
       </c>
-      <c r="X6" s="2">
-        <f>X5+1</f>
+      <c r="AC6" s="6">
+        <f>AC5+1</f>
         <v>2</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="AD6" s="7">
         <v>18599.50895286103</v>
       </c>
     </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -2336,25 +2747,30 @@
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="3">
-        <v>25352.916455949129</v>
-      </c>
-      <c r="R7" s="2">
+      <c r="N7" s="3"/>
+      <c r="R7" s="6">
         <f t="shared" ref="R7:R54" si="3">R6+1</f>
         <v>3</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="7">
+        <v>25352.916455949129</v>
+      </c>
+      <c r="W7" s="6">
+        <f t="shared" ref="W7:W54" si="4">W6+1</f>
+        <v>3</v>
+      </c>
+      <c r="X7" s="7">
         <v>27527.12490572207</v>
       </c>
-      <c r="X7" s="2">
-        <f t="shared" ref="X7:X54" si="4">X6+1</f>
+      <c r="AC7" s="6">
+        <f t="shared" ref="AC7:AC54" si="5">AC6+1</f>
         <v>3</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="AD7" s="7">
         <v>18386.542879927329</v>
       </c>
     </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2376,25 +2792,30 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="3"/>
+      <c r="R8" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S8" s="7">
         <v>24894.749163669389</v>
       </c>
-      <c r="R8" s="2">
-        <f t="shared" si="3"/>
+      <c r="W8" s="6">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S8" s="3">
+      <c r="X8" s="7">
         <v>21384.566414532241</v>
       </c>
-      <c r="X8" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC8" s="6">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="AD8" s="7">
         <v>17922.602198092642</v>
       </c>
     </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2416,25 +2837,30 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="3"/>
+      <c r="R9" s="6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S9" s="7">
         <v>26957.038760762938</v>
       </c>
-      <c r="R9" s="2">
-        <f t="shared" si="3"/>
+      <c r="W9" s="6">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="S9" s="3">
+      <c r="X9" s="7">
         <v>27085.683077565842</v>
       </c>
-      <c r="X9" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC9" s="6">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="AD9" s="7">
         <v>19444.21708083561</v>
       </c>
     </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2456,25 +2882,30 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="3"/>
+      <c r="R10" s="6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S10" s="7">
         <v>24830.75390735695</v>
       </c>
-      <c r="R10" s="2">
-        <f t="shared" si="3"/>
+      <c r="W10" s="6">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="S10" s="3">
+      <c r="X10" s="7">
         <v>28476.734489373299</v>
       </c>
-      <c r="X10" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC10" s="6">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="Y10" s="3">
+      <c r="AD10" s="7">
         <v>18654.721078383289</v>
       </c>
     </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2496,25 +2927,30 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="3"/>
+      <c r="R11" s="6">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S11" s="7">
         <v>24969.679909173479</v>
       </c>
-      <c r="R11" s="2">
-        <f t="shared" si="3"/>
+      <c r="W11" s="6">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="S11" s="3">
+      <c r="X11" s="7">
         <v>27077.582967484101</v>
       </c>
-      <c r="X11" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC11" s="6">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="Y11" s="3">
+      <c r="AD11" s="7">
         <v>23943.555937420519</v>
       </c>
     </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2536,25 +2972,30 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="3"/>
+      <c r="R12" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S12" s="7">
         <v>22185.101828156221</v>
       </c>
-      <c r="R12" s="2">
-        <f t="shared" si="3"/>
+      <c r="W12" s="6">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="S12" s="3">
+      <c r="X12" s="7">
         <v>26628.425764577649</v>
       </c>
-      <c r="X12" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC12" s="6">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="Y12" s="3">
+      <c r="AD12" s="7">
         <v>17582.05317674841</v>
       </c>
     </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2576,25 +3017,30 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="3"/>
+      <c r="R13" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S13" s="7">
         <v>31867.699928792001</v>
       </c>
-      <c r="R13" s="2">
-        <f t="shared" si="3"/>
+      <c r="W13" s="6">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="S13" s="3">
+      <c r="X13" s="7">
         <v>29405.42495404177</v>
       </c>
-      <c r="X13" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC13" s="6">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="AD13" s="7">
         <v>22379.753733878289</v>
       </c>
     </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2616,25 +3062,30 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="3"/>
+      <c r="R14" s="6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S14" s="7">
         <v>21240.903485921881</v>
       </c>
-      <c r="R14" s="2">
-        <f t="shared" si="3"/>
+      <c r="W14" s="6">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="S14" s="3">
+      <c r="X14" s="7">
         <v>28703.283207266111</v>
       </c>
-      <c r="X14" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC14" s="6">
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="AD14" s="7">
         <v>17194.889912715709</v>
       </c>
     </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2656,25 +3107,30 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="3"/>
+      <c r="R15" s="6">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S15" s="7">
         <v>21795.601074659389</v>
       </c>
-      <c r="R15" s="2">
-        <f t="shared" si="3"/>
+      <c r="W15" s="6">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="S15" s="3">
+      <c r="X15" s="7">
         <v>22092.301140781099</v>
       </c>
-      <c r="X15" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC15" s="6">
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="AD15" s="7">
         <v>22304.639723433229</v>
       </c>
     </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2696,25 +3152,30 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="3"/>
+      <c r="R16" s="6">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S16" s="7">
         <v>22037.024806176199</v>
       </c>
-      <c r="R16" s="2">
-        <f t="shared" si="3"/>
+      <c r="W16" s="6">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="S16" s="3">
+      <c r="X16" s="7">
         <v>25953.812155131691</v>
       </c>
-      <c r="X16" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC16" s="6">
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="AD16" s="7">
         <v>27248.285171480471</v>
       </c>
     </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2736,25 +3197,30 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="3"/>
+      <c r="R17" s="6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S17" s="7">
         <v>26236.623352225241</v>
       </c>
-      <c r="R17" s="2">
-        <f t="shared" si="3"/>
+      <c r="W17" s="6">
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="S17" s="3">
+      <c r="X17" s="7">
         <v>27821.480453769302</v>
       </c>
-      <c r="X17" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC17" s="6">
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="Y17" s="3">
+      <c r="AD17" s="7">
         <v>19862.88902397819</v>
       </c>
     </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2776,25 +3242,30 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="3"/>
+      <c r="R18" s="6">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S18" s="7">
         <v>27147.73105467757</v>
       </c>
-      <c r="R18" s="2">
-        <f t="shared" si="3"/>
+      <c r="W18" s="6">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="S18" s="3">
+      <c r="X18" s="7">
         <v>27838.79081525885</v>
       </c>
-      <c r="X18" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC18" s="6">
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="Y18" s="3">
+      <c r="AD18" s="7">
         <v>20928.38678855585</v>
       </c>
     </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2816,25 +3287,30 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="3"/>
+      <c r="R19" s="6">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S19" s="7">
         <v>20544.2572544959</v>
       </c>
-      <c r="R19" s="2">
-        <f t="shared" si="3"/>
+      <c r="W19" s="6">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="S19" s="3">
+      <c r="X19" s="7">
         <v>25870.22933914623</v>
       </c>
-      <c r="X19" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC19" s="6">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="Y19" s="3">
+      <c r="AD19" s="7">
         <v>21287.515517257041</v>
       </c>
     </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2856,25 +3332,30 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="3"/>
+      <c r="R20" s="6">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S20" s="7">
         <v>19110.42362470481</v>
       </c>
-      <c r="R20" s="2">
-        <f t="shared" si="3"/>
+      <c r="W20" s="6">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="S20" s="3">
+      <c r="X20" s="7">
         <v>24846.992360762939</v>
       </c>
-      <c r="X20" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC20" s="6">
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="Y20" s="3">
+      <c r="AD20" s="7">
         <v>19211.921113987279</v>
       </c>
     </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2896,25 +3377,30 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="3"/>
+      <c r="R21" s="6">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S21" s="7">
         <v>25860.425137874648</v>
       </c>
-      <c r="R21" s="2">
-        <f t="shared" si="3"/>
+      <c r="W21" s="6">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="S21" s="3">
+      <c r="X21" s="7">
         <v>23736.14106557675</v>
       </c>
-      <c r="X21" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC21" s="6">
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="Y21" s="3">
+      <c r="AD21" s="7">
         <v>23136.30079128065</v>
       </c>
     </row>
-    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2936,25 +3422,30 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="3"/>
+      <c r="R22" s="6">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S22" s="7">
         <v>27472.0514990009</v>
       </c>
-      <c r="R22" s="2">
-        <f t="shared" si="3"/>
+      <c r="W22" s="6">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="S22" s="3">
+      <c r="X22" s="7">
         <v>26362.956930790191</v>
       </c>
-      <c r="X22" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC22" s="6">
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="Y22" s="3">
+      <c r="AD22" s="7">
         <v>21145.99625912806</v>
       </c>
     </row>
-    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2976,25 +3467,30 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="3"/>
+      <c r="R23" s="6">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S23" s="7">
         <v>27885.479411080829</v>
       </c>
-      <c r="R23" s="2">
-        <f t="shared" si="3"/>
+      <c r="W23" s="6">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="S23" s="3">
+      <c r="X23" s="7">
         <v>27480.216748047231</v>
       </c>
-      <c r="X23" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC23" s="6">
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="Y23" s="3">
+      <c r="AD23" s="7">
         <v>23775.2739065395</v>
       </c>
     </row>
-    <row r="24" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3016,25 +3512,30 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="3"/>
+      <c r="R24" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S24" s="7">
         <v>22540.642134423251</v>
       </c>
-      <c r="R24" s="2">
-        <f t="shared" si="3"/>
+      <c r="W24" s="6">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="S24" s="3">
+      <c r="X24" s="7">
         <v>24043.32874586738</v>
       </c>
-      <c r="X24" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC24" s="6">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="Y24" s="3">
+      <c r="AD24" s="7">
         <v>22588.26661562216</v>
       </c>
     </row>
-    <row r="25" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3056,25 +3557,30 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="3"/>
+      <c r="R25" s="6">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S25" s="7">
         <v>29237.82799527701</v>
       </c>
-      <c r="R25" s="2">
-        <f t="shared" si="3"/>
+      <c r="W25" s="6">
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="S25" s="3">
+      <c r="X25" s="7">
         <v>28385.239127702091</v>
       </c>
-      <c r="X25" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC25" s="6">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="AD25" s="7">
         <v>27922.982265031791</v>
       </c>
     </row>
-    <row r="26" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3096,25 +3602,30 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="3"/>
+      <c r="R26" s="6">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S26" s="7">
         <v>23716.743336603078</v>
       </c>
-      <c r="R26" s="2">
-        <f t="shared" si="3"/>
+      <c r="W26" s="6">
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="S26" s="3">
+      <c r="X26" s="7">
         <v>20175.915136784741</v>
       </c>
-      <c r="X26" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC26" s="6">
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="Y26" s="3">
+      <c r="AD26" s="7">
         <v>22856.326849591271</v>
       </c>
     </row>
-    <row r="27" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3136,25 +3647,30 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="3"/>
+      <c r="R27" s="6">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S27" s="7">
         <v>29189.776946775652</v>
       </c>
-      <c r="R27" s="2">
-        <f t="shared" si="3"/>
+      <c r="W27" s="6">
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="S27" s="3">
+      <c r="X27" s="7">
         <v>27921.91306158037</v>
       </c>
-      <c r="X27" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC27" s="6">
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="Y27" s="3">
+      <c r="AD27" s="7">
         <v>22432.51333178928</v>
       </c>
     </row>
-    <row r="28" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3176,25 +3692,30 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="3"/>
+      <c r="R28" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S28" s="7">
         <v>24353.516116621238</v>
       </c>
-      <c r="R28" s="2">
-        <f t="shared" si="3"/>
+      <c r="W28" s="6">
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="S28" s="3">
+      <c r="X28" s="7">
         <v>27791.54312588555</v>
       </c>
-      <c r="X28" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC28" s="6">
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="Y28" s="3">
+      <c r="AD28" s="7">
         <v>17730.622855222518</v>
       </c>
     </row>
-    <row r="29" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3216,25 +3737,30 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="3"/>
+      <c r="R29" s="6">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S29" s="7">
         <v>23709.83611952771</v>
       </c>
-      <c r="R29" s="2">
-        <f t="shared" si="3"/>
+      <c r="W29" s="6">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="S29" s="3">
+      <c r="X29" s="7">
         <v>21539.069658128981</v>
       </c>
-      <c r="X29" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC29" s="6">
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="Y29" s="3">
+      <c r="AD29" s="7">
         <v>18720.238376566751</v>
       </c>
     </row>
-    <row r="30" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3256,25 +3782,30 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30" s="3"/>
+      <c r="R30" s="6">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S30" s="7">
         <v>18306.851416167119</v>
       </c>
-      <c r="R30" s="2">
-        <f t="shared" si="3"/>
+      <c r="W30" s="6">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="S30" s="3">
+      <c r="X30" s="7">
         <v>33628.939120799267</v>
       </c>
-      <c r="X30" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC30" s="6">
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
-      <c r="Y30" s="3">
+      <c r="AD30" s="7">
         <v>20426.31913342416</v>
       </c>
     </row>
-    <row r="31" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3296,25 +3827,30 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="3"/>
+      <c r="R31" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S31" s="7">
         <v>29864.813650862841</v>
       </c>
-      <c r="R31" s="2">
-        <f t="shared" si="3"/>
+      <c r="W31" s="6">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="S31" s="3">
+      <c r="X31" s="7">
         <v>31318.72610426883</v>
       </c>
-      <c r="X31" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC31" s="6">
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="Y31" s="3">
+      <c r="AD31" s="7">
         <v>22420.379969936421</v>
       </c>
     </row>
-    <row r="32" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3336,25 +3872,30 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="3"/>
+      <c r="R32" s="6">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S32" s="7">
         <v>25500.028851952771</v>
       </c>
-      <c r="R32" s="2">
-        <f t="shared" si="3"/>
+      <c r="W32" s="6">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="S32" s="3">
+      <c r="X32" s="7">
         <v>27313.788173297002</v>
       </c>
-      <c r="X32" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC32" s="6">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="Y32" s="3">
+      <c r="AD32" s="7">
         <v>24989.127697366031</v>
       </c>
     </row>
-    <row r="33" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3376,25 +3917,30 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="3"/>
+      <c r="R33" s="6">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S33" s="7">
         <v>27626.105386012721</v>
       </c>
-      <c r="R33" s="2">
-        <f t="shared" si="3"/>
+      <c r="W33" s="6">
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="S33" s="3">
+      <c r="X33" s="7">
         <v>26192.68274296094</v>
       </c>
-      <c r="X33" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC33" s="6">
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="Y33" s="3">
+      <c r="AD33" s="7">
         <v>19748.76884632152</v>
       </c>
     </row>
-    <row r="34" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3416,25 +3962,30 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="3"/>
+      <c r="R34" s="6">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S34" s="7">
         <v>29556.621621435061</v>
       </c>
-      <c r="R34" s="2">
-        <f t="shared" si="3"/>
+      <c r="W34" s="6">
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="S34" s="3">
+      <c r="X34" s="7">
         <v>22778.67878328792</v>
       </c>
-      <c r="X34" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC34" s="6">
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="Y34" s="3">
+      <c r="AD34" s="7">
         <v>21015.266439327879</v>
       </c>
     </row>
-    <row r="35" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3456,25 +4007,30 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35" s="3"/>
+      <c r="R35" s="6">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S35" s="7">
         <v>29468.62768937329</v>
       </c>
-      <c r="R35" s="2">
-        <f t="shared" si="3"/>
+      <c r="W35" s="6">
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="S35" s="3">
+      <c r="X35" s="7">
         <v>28720.51647956403</v>
       </c>
-      <c r="X35" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC35" s="6">
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
-      <c r="Y35" s="3">
+      <c r="AD35" s="7">
         <v>18538.354909173471</v>
       </c>
     </row>
-    <row r="36" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3496,25 +4052,30 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36" s="3"/>
+      <c r="R36" s="6">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S36" s="7">
         <v>26302.726810535871</v>
       </c>
-      <c r="R36" s="2">
-        <f t="shared" si="3"/>
+      <c r="W36" s="6">
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="S36" s="3">
+      <c r="X36" s="7">
         <v>25526.191755858312</v>
       </c>
-      <c r="X36" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC36" s="6">
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="Y36" s="3">
+      <c r="AD36" s="7">
         <v>18735.437490917349</v>
       </c>
     </row>
-    <row r="37" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3536,25 +4097,30 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37" s="3"/>
+      <c r="R37" s="6">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S37" s="7">
         <v>23987.593416893731</v>
       </c>
-      <c r="R37" s="2">
-        <f t="shared" si="3"/>
+      <c r="W37" s="6">
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
-      <c r="S37" s="3">
+      <c r="X37" s="7">
         <v>27571.763638147131</v>
       </c>
-      <c r="X37" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC37" s="6">
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="Y37" s="3">
+      <c r="AD37" s="7">
         <v>22397.248349137149</v>
       </c>
     </row>
-    <row r="38" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3576,25 +4142,30 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38" s="3"/>
+      <c r="R38" s="6">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S38" s="7">
         <v>22007.317797275209</v>
       </c>
-      <c r="R38" s="2">
-        <f t="shared" si="3"/>
+      <c r="W38" s="6">
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
-      <c r="S38" s="3">
+      <c r="X38" s="7">
         <v>30256.78878801089</v>
       </c>
-      <c r="X38" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC38" s="6">
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="Y38" s="3">
+      <c r="AD38" s="7">
         <v>24820.39397874659</v>
       </c>
     </row>
-    <row r="39" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3616,25 +4187,30 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39" s="3"/>
+      <c r="R39" s="6">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S39" s="7">
         <v>33985.91971335149</v>
       </c>
-      <c r="R39" s="2">
-        <f t="shared" si="3"/>
+      <c r="W39" s="6">
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="S39" s="3">
+      <c r="X39" s="7">
         <v>24169.101326067201</v>
       </c>
-      <c r="X39" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC39" s="6">
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="Y39" s="3">
+      <c r="AD39" s="7">
         <v>18504.760334150771</v>
       </c>
     </row>
-    <row r="40" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3656,25 +4232,30 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40" s="3"/>
+      <c r="R40" s="6">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S40" s="7">
         <v>30214.322368392379</v>
       </c>
-      <c r="R40" s="2">
-        <f t="shared" si="3"/>
+      <c r="W40" s="6">
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="S40" s="3">
+      <c r="X40" s="7">
         <v>23871.78472043596</v>
       </c>
-      <c r="X40" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC40" s="6">
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
-      <c r="Y40" s="3">
+      <c r="AD40" s="7">
         <v>21995.620856039961</v>
       </c>
     </row>
-    <row r="41" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3696,25 +4277,30 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41" s="3"/>
+      <c r="R41" s="6">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S41" s="7">
         <v>26575.209826339691</v>
       </c>
-      <c r="R41" s="2">
-        <f t="shared" si="3"/>
+      <c r="W41" s="6">
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
-      <c r="S41" s="3">
+      <c r="X41" s="7">
         <v>29646.2960959128</v>
       </c>
-      <c r="X41" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC41" s="6">
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
-      <c r="Y41" s="3">
+      <c r="AD41" s="7">
         <v>24134.164480926422</v>
       </c>
     </row>
-    <row r="42" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3736,25 +4322,30 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42" s="3"/>
+      <c r="R42" s="6">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S42" s="7">
         <v>29032.851417257039</v>
       </c>
-      <c r="R42" s="2">
-        <f t="shared" si="3"/>
+      <c r="W42" s="6">
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="S42" s="3">
+      <c r="X42" s="7">
         <v>28792.718485013618</v>
       </c>
-      <c r="X42" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC42" s="6">
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
-      <c r="Y42" s="3">
+      <c r="AD42" s="7">
         <v>18026.155254405079</v>
       </c>
     </row>
-    <row r="43" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3776,25 +4367,30 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43" s="3"/>
+      <c r="R43" s="6">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S43" s="7">
         <v>22909.176117711158</v>
       </c>
-      <c r="R43" s="2">
-        <f t="shared" si="3"/>
+      <c r="W43" s="6">
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
-      <c r="S43" s="3">
+      <c r="X43" s="7">
         <v>25922.16662270662</v>
       </c>
-      <c r="X43" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC43" s="6">
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
-      <c r="Y43" s="3">
+      <c r="AD43" s="7">
         <v>23064.1741421435</v>
       </c>
     </row>
-    <row r="44" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3816,25 +4412,30 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44" s="3"/>
+      <c r="R44" s="6">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S44" s="7">
         <v>29475.973014713891</v>
       </c>
-      <c r="R44" s="2">
-        <f t="shared" si="3"/>
+      <c r="W44" s="6">
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="S44" s="3">
+      <c r="X44" s="7">
         <v>28710.912568210711</v>
       </c>
-      <c r="X44" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC44" s="6">
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="Y44" s="3">
+      <c r="AD44" s="7">
         <v>17387.668342688459</v>
       </c>
     </row>
-    <row r="45" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3856,25 +4457,30 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45" s="3"/>
+      <c r="R45" s="6">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S45" s="7">
         <v>22714.205055404171</v>
       </c>
-      <c r="R45" s="2">
-        <f t="shared" si="3"/>
+      <c r="W45" s="6">
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
-      <c r="S45" s="3">
+      <c r="X45" s="7">
         <v>27013.757437238859</v>
       </c>
-      <c r="X45" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC45" s="6">
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
-      <c r="Y45" s="3">
+      <c r="AD45" s="7">
         <v>17484.190023160761</v>
       </c>
     </row>
-    <row r="46" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3896,25 +4502,30 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="3">
+      <c r="N46" s="3"/>
+      <c r="R46" s="6">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S46" s="7">
         <v>26018.82962870118</v>
       </c>
-      <c r="R46" s="2">
-        <f t="shared" si="3"/>
+      <c r="W46" s="6">
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="S46" s="3">
+      <c r="X46" s="7">
         <v>24378.651235603989</v>
       </c>
-      <c r="X46" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC46" s="6">
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="Y46" s="3">
+      <c r="AD46" s="7">
         <v>24768.97743142597</v>
       </c>
     </row>
-    <row r="47" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3936,25 +4547,30 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="3"/>
+      <c r="R47" s="6">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S47" s="7">
         <v>24108.260384377842</v>
       </c>
-      <c r="R47" s="2">
-        <f t="shared" si="3"/>
+      <c r="W47" s="6">
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="S47" s="3">
+      <c r="X47" s="7">
         <v>25213.660931880109</v>
       </c>
-      <c r="X47" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC47" s="6">
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
-      <c r="Y47" s="3">
+      <c r="AD47" s="7">
         <v>18138.828189554941</v>
       </c>
     </row>
-    <row r="48" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3976,25 +4592,30 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48" s="3"/>
+      <c r="R48" s="6">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S48" s="7">
         <v>22262.613278474098</v>
       </c>
-      <c r="R48" s="2">
-        <f t="shared" si="3"/>
+      <c r="W48" s="6">
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="S48" s="3">
+      <c r="X48" s="7">
         <v>25801.094716439598</v>
       </c>
-      <c r="X48" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC48" s="6">
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
-      <c r="Y48" s="3">
+      <c r="AD48" s="7">
         <v>26071.070863669389</v>
       </c>
     </row>
-    <row r="49" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -4016,25 +4637,30 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N49" s="3"/>
+      <c r="R49" s="6">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S49" s="7">
         <v>21762.464642325151</v>
       </c>
-      <c r="R49" s="2">
-        <f t="shared" si="3"/>
+      <c r="W49" s="6">
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="S49" s="3">
+      <c r="X49" s="7">
         <v>26359.244130426869</v>
       </c>
-      <c r="X49" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC49" s="6">
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
-      <c r="Y49" s="3">
+      <c r="AD49" s="7">
         <v>21987.527546321518</v>
       </c>
     </row>
-    <row r="50" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4056,25 +4682,30 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50" s="3"/>
+      <c r="R50" s="6">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S50" s="7">
         <v>21174.720312443231</v>
       </c>
-      <c r="R50" s="2">
-        <f t="shared" si="3"/>
+      <c r="W50" s="6">
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="S50" s="3">
+      <c r="X50" s="7">
         <v>26790.604630699359</v>
       </c>
-      <c r="X50" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC50" s="6">
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
-      <c r="Y50" s="3">
+      <c r="AD50" s="7">
         <v>20352.815826339691</v>
       </c>
     </row>
-    <row r="51" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4096,25 +4727,30 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51" s="3"/>
+      <c r="R51" s="6">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S51" s="7">
         <v>27372.740427974561</v>
       </c>
-      <c r="R51" s="2">
-        <f t="shared" si="3"/>
+      <c r="W51" s="6">
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
-      <c r="S51" s="3">
+      <c r="X51" s="7">
         <v>25730.73638510445</v>
       </c>
-      <c r="X51" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC51" s="6">
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="Y51" s="3">
+      <c r="AD51" s="7">
         <v>18445.639215712981</v>
       </c>
     </row>
-    <row r="52" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4136,25 +4772,30 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52" s="3"/>
+      <c r="R52" s="6">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S52" s="7">
         <v>20963.740673206172</v>
       </c>
-      <c r="R52" s="2">
-        <f t="shared" si="3"/>
+      <c r="W52" s="6">
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="S52" s="3">
+      <c r="X52" s="7">
         <v>26960.308219800168</v>
       </c>
-      <c r="X52" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC52" s="6">
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="Y52" s="3">
+      <c r="AD52" s="7">
         <v>21782.700603451409</v>
       </c>
     </row>
-    <row r="53" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4176,25 +4817,30 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="3">
+      <c r="N53" s="3"/>
+      <c r="R53" s="6">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S53" s="7">
         <v>26174.130431244321</v>
       </c>
-      <c r="R53" s="2">
-        <f t="shared" si="3"/>
+      <c r="W53" s="6">
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="S53" s="3">
+      <c r="X53" s="7">
         <v>24106.8282212534</v>
       </c>
-      <c r="X53" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC53" s="6">
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="Y53" s="3">
+      <c r="AD53" s="7">
         <v>20043.88215149863</v>
       </c>
     </row>
-    <row r="54" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4216,25 +4862,38 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="3">
+      <c r="N54" s="3"/>
+      <c r="R54" s="6">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S54" s="7">
         <v>20206.96591825613</v>
       </c>
-      <c r="R54" s="2">
-        <f t="shared" si="3"/>
+      <c r="W54" s="6">
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="S54" s="3">
+      <c r="X54" s="7">
         <v>29653.797887738401</v>
       </c>
-      <c r="X54" s="2">
-        <f t="shared" si="4"/>
+      <c r="AC54" s="6">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="Y54" s="3">
+      <c r="AD54" s="7">
         <v>19469.047071207991</v>
       </c>
     </row>
-    <row r="56" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="5"/>
+    </row>
+    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
@@ -4256,26 +4915,33 @@
       <c r="M56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N56" s="3">
+      <c r="N56" s="3" t="e">
         <f>AVERAGE(N5:N54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="S56" s="7">
+        <f>AVERAGE(S5:S54)</f>
         <v>25129.21293262126</v>
       </c>
-      <c r="R56" s="2" t="s">
+      <c r="W56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="S56" s="3">
-        <f>AVERAGE(S5:S54)</f>
+      <c r="X56" s="7">
+        <f>AVERAGE(X5:X54)</f>
         <v>26693.120168508627</v>
       </c>
-      <c r="X56" s="2" t="s">
+      <c r="AC56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Y56" s="3">
-        <f>AVERAGE(Y5:Y54)</f>
+      <c r="AD56" s="7">
+        <f>AVERAGE(AD5:AD54)</f>
         <v>21033.450250214344</v>
       </c>
     </row>
-    <row r="57" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
@@ -4297,22 +4963,29 @@
       <c r="M57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N57" s="3">
+      <c r="N57" s="3" t="e">
         <f>_xlfn.STDEV.S(N5:N54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R57" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S57" s="7">
+        <f>_xlfn.STDEV.S(S5:S54)</f>
         <v>3508.9550639479116</v>
       </c>
-      <c r="R57" s="2" t="s">
+      <c r="W57" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="S57" s="3">
-        <f>_xlfn.STDEV.S(S5:S54)</f>
+      <c r="X57" s="7">
+        <f>_xlfn.STDEV.S(X5:X54)</f>
         <v>2810.4640970080959</v>
       </c>
-      <c r="X57" s="2" t="s">
+      <c r="AC57" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Y57" s="3">
-        <f>_xlfn.STDEV.S(Y5:Y54)</f>
+      <c r="AD57" s="7">
+        <f>_xlfn.STDEV.S(AD5:AD54)</f>
         <v>2708.8431954162374</v>
       </c>
     </row>
@@ -4325,7 +4998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:X57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -4341,7 +5014,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1"/>
       <c r="M3" s="1" t="s">
@@ -4358,26 +5031,26 @@
     <row r="4" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W4" s="2"/>
       <c r="X4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="3:24" x14ac:dyDescent="0.25">
@@ -6474,14 +7147,14 @@
   <sheetData>
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1"/>
       <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="3:15" x14ac:dyDescent="0.25">
@@ -7873,31 +8546,31 @@
   <sheetData>
     <row r="3" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1"/>
       <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.25">
@@ -9271,14 +9944,14 @@
   <sheetData>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1"/>
       <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test-23: hybrid model 2.0 (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="17">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -2576,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AD57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2660,7 +2660,9 @@
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="3"/>
+      <c r="N5" s="3">
+        <v>40783.27438681318</v>
+      </c>
       <c r="R5" s="6">
         <v>1</v>
       </c>
@@ -2702,7 +2704,9 @@
         <f>M5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="3"/>
+      <c r="N6" s="3">
+        <v>54752.830912179481</v>
+      </c>
       <c r="R6" s="6">
         <f>R5+1</f>
         <v>2</v>
@@ -2747,7 +2751,9 @@
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="3"/>
+      <c r="N7" s="3">
+        <v>43329.340262728932</v>
+      </c>
       <c r="R7" s="6">
         <f t="shared" ref="R7:R54" si="3">R6+1</f>
         <v>3</v>
@@ -2792,7 +2798,9 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="3"/>
+      <c r="N8" s="3">
+        <v>53826.335530769233</v>
+      </c>
       <c r="R8" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -2837,7 +2845,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="3"/>
+      <c r="N9" s="3">
+        <v>46911.347733333321</v>
+      </c>
       <c r="R9" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -2882,7 +2892,9 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="3"/>
+      <c r="N10" s="3">
+        <v>44188.580889194127</v>
+      </c>
       <c r="R10" s="6">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -2927,7 +2939,9 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="3"/>
+      <c r="N11" s="3">
+        <v>49049.673366117211</v>
+      </c>
       <c r="R11" s="6">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -2972,7 +2986,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="3"/>
+      <c r="N12" s="3">
+        <v>50994.725730769227</v>
+      </c>
       <c r="R12" s="6">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -3017,7 +3033,9 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="3"/>
+      <c r="N13" s="3">
+        <v>46830.665860805857</v>
+      </c>
       <c r="R13" s="6">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -3062,7 +3080,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="3"/>
+      <c r="N14" s="3">
+        <v>46565.741602472517</v>
+      </c>
       <c r="R14" s="6">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -3107,7 +3127,9 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="3"/>
+      <c r="N15" s="3">
+        <v>46212.191784157512</v>
+      </c>
       <c r="R15" s="6">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -3152,7 +3174,9 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="N16" s="3">
+        <v>45897.369295604389</v>
+      </c>
       <c r="R16" s="6">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -3197,7 +3221,9 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="3"/>
+      <c r="N17" s="3">
+        <v>46834.432859065942</v>
+      </c>
       <c r="R17" s="6">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -3242,7 +3268,9 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3">
+        <v>50320.426366758227</v>
+      </c>
       <c r="R18" s="6">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -3287,7 +3315,9 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="3"/>
+      <c r="N19" s="3">
+        <v>49521.623250274723</v>
+      </c>
       <c r="R19" s="6">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -3332,7 +3362,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="3"/>
+      <c r="N20" s="3">
+        <v>46741.884842948712</v>
+      </c>
       <c r="R20" s="6">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -3377,7 +3409,9 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="3"/>
+      <c r="N21" s="3">
+        <v>41494.827555860807</v>
+      </c>
       <c r="R21" s="6">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -3422,7 +3456,9 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="3"/>
+      <c r="N22" s="3">
+        <v>41888.334459157501</v>
+      </c>
       <c r="R22" s="6">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -3467,7 +3503,9 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="3"/>
+      <c r="N23" s="3">
+        <v>38535.791719505491</v>
+      </c>
       <c r="R23" s="6">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -3512,7 +3550,9 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="3"/>
+      <c r="N24" s="3">
+        <v>44261.689069505483</v>
+      </c>
       <c r="R24" s="6">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -3557,7 +3597,9 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="3"/>
+      <c r="N25" s="3">
+        <v>42649.46274844322</v>
+      </c>
       <c r="R25" s="6">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -3602,7 +3644,9 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="3"/>
+      <c r="N26" s="3">
+        <v>43788.119101282042</v>
+      </c>
       <c r="R26" s="6">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -3647,7 +3691,9 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="3"/>
+      <c r="N27" s="3">
+        <v>54556.354364377279</v>
+      </c>
       <c r="R27" s="6">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -3692,7 +3738,9 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="3"/>
+      <c r="N28" s="3">
+        <v>41178.944960714281</v>
+      </c>
       <c r="R28" s="6">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -3737,7 +3785,9 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="3"/>
+      <c r="N29" s="3">
+        <v>42840.081619597069</v>
+      </c>
       <c r="R29" s="6">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -3782,7 +3832,9 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="3"/>
+      <c r="N30" s="3">
+        <v>43415.976069413919</v>
+      </c>
       <c r="R30" s="6">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -3827,7 +3879,9 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="3"/>
+      <c r="N31" s="3">
+        <v>51457.621184065923</v>
+      </c>
       <c r="R31" s="6">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -3872,7 +3926,9 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="3"/>
+      <c r="N32" s="3">
+        <v>43131.912982600727</v>
+      </c>
       <c r="R32" s="6">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -3917,7 +3973,9 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="3"/>
+      <c r="N33" s="3">
+        <v>48406.000911721603</v>
+      </c>
       <c r="R33" s="6">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -3962,7 +4020,9 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="3"/>
+      <c r="N34" s="3">
+        <v>41483.977893315008</v>
+      </c>
       <c r="R34" s="6">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -4007,7 +4067,9 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="3"/>
+      <c r="N35" s="3">
+        <v>48601.631034706952</v>
+      </c>
       <c r="R35" s="6">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -4052,7 +4114,9 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="3"/>
+      <c r="N36" s="3">
+        <v>47502.389884981669</v>
+      </c>
       <c r="R36" s="6">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -4097,7 +4161,9 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="3"/>
+      <c r="N37" s="3">
+        <v>52207.718065842491</v>
+      </c>
       <c r="R37" s="6">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -4142,7 +4208,9 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="3"/>
+      <c r="N38" s="3">
+        <v>42691.970096611723</v>
+      </c>
       <c r="R38" s="6">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -4187,7 +4255,9 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="3"/>
+      <c r="N39" s="3">
+        <v>50975.185325732593</v>
+      </c>
       <c r="R39" s="6">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -4232,7 +4302,9 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="3"/>
+      <c r="N40" s="3">
+        <v>47424.042013369959</v>
+      </c>
       <c r="R40" s="6">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -4277,7 +4349,9 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="3"/>
+      <c r="N41" s="3">
+        <v>47390.54655824176</v>
+      </c>
       <c r="R41" s="6">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -4322,7 +4396,9 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="3"/>
+      <c r="N42" s="3">
+        <v>43571.470498351649</v>
+      </c>
       <c r="R42" s="6">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -4367,7 +4443,9 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="3"/>
+      <c r="N43" s="3">
+        <v>45788.508652472519</v>
+      </c>
       <c r="R43" s="6">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -4412,7 +4490,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="3"/>
+      <c r="N44" s="3">
+        <v>45419.365946245409</v>
+      </c>
       <c r="R44" s="6">
         <f t="shared" si="3"/>
         <v>40</v>
@@ -4457,7 +4537,9 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="3"/>
+      <c r="N45" s="3">
+        <v>53005.334921336987</v>
+      </c>
       <c r="R45" s="6">
         <f t="shared" si="3"/>
         <v>41</v>
@@ -4502,7 +4584,9 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="3"/>
+      <c r="N46" s="3">
+        <v>53949.983955769218</v>
+      </c>
       <c r="R46" s="6">
         <f t="shared" si="3"/>
         <v>42</v>
@@ -4547,7 +4631,9 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="3"/>
+      <c r="N47" s="3">
+        <v>47819.14284459706</v>
+      </c>
       <c r="R47" s="6">
         <f t="shared" si="3"/>
         <v>43</v>
@@ -4592,7 +4678,9 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="3"/>
+      <c r="N48" s="3">
+        <v>43486.465521245424</v>
+      </c>
       <c r="R48" s="6">
         <f t="shared" si="3"/>
         <v>44</v>
@@ -4637,7 +4725,9 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="3"/>
+      <c r="N49" s="3">
+        <v>46688.86552316849</v>
+      </c>
       <c r="R49" s="6">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -4682,7 +4772,9 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="3"/>
+      <c r="N50" s="3">
+        <v>46016.715044139193</v>
+      </c>
       <c r="R50" s="6">
         <f t="shared" si="3"/>
         <v>46</v>
@@ -4727,7 +4819,9 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="3"/>
+      <c r="N51" s="3">
+        <v>48975.944619505492</v>
+      </c>
       <c r="R51" s="6">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -4772,7 +4866,9 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="3"/>
+      <c r="N52" s="3">
+        <v>54025.002115659343</v>
+      </c>
       <c r="R52" s="6">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -4817,7 +4913,9 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="3"/>
+      <c r="N53" s="3">
+        <v>49288.811329945049</v>
+      </c>
       <c r="R53" s="6">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -4862,7 +4960,9 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="3"/>
+      <c r="N54" s="3">
+        <v>56523.561707600733</v>
+      </c>
       <c r="R54" s="6">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -4915,9 +5015,9 @@
       <c r="M56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N56" s="3" t="e">
+      <c r="N56" s="3">
         <f>AVERAGE(N5:N54)</f>
-        <v>#DIV/0!</v>
+        <v>47064.04389946154</v>
       </c>
       <c r="R56" s="6" t="s">
         <v>3</v>
@@ -4963,9 +5063,9 @@
       <c r="M57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N57" s="3" t="e">
+      <c r="N57" s="3">
         <f>_xlfn.STDEV.S(N5:N54)</f>
-        <v>#DIV/0!</v>
+        <v>4255.6181299830268</v>
       </c>
       <c r="R57" s="6" t="s">
         <v>4</v>
@@ -4996,10 +5096,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:X57"/>
+  <dimension ref="C3:AC57"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5008,7 +5108,7 @@
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5018,17 +5118,28 @@
       </c>
       <c r="J3" s="1"/>
       <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="5"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="AC3" s="5"/>
+    </row>
+    <row r="4" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -5044,16 +5155,26 @@
       <c r="N4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2" t="s">
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -5072,23 +5193,33 @@
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="3"/>
+      <c r="R5" s="6">
+        <v>1</v>
+      </c>
+      <c r="S5" s="7">
         <v>97.469482288828331</v>
       </c>
-      <c r="R5" s="2">
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="6">
         <v>1</v>
       </c>
-      <c r="S5" s="3">
+      <c r="X5" s="7">
         <v>108.2972025431426</v>
       </c>
-      <c r="W5" s="2">
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="6">
         <v>1</v>
       </c>
-      <c r="X5" s="3">
+      <c r="AC5" s="7">
         <v>91.764632152588561</v>
       </c>
     </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -5110,25 +5241,36 @@
         <f>M5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="3">
-        <v>102.0591099000908</v>
-      </c>
-      <c r="R6" s="2">
+      <c r="N6" s="3"/>
+      <c r="R6" s="6">
         <f>R5+1</f>
         <v>2</v>
       </c>
-      <c r="S6" s="3">
-        <v>102.626012715713</v>
-      </c>
-      <c r="W6" s="2">
+      <c r="S6" s="7">
+        <v>102.0591099000908</v>
+      </c>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="6">
         <f>W5+1</f>
         <v>2</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6" s="7">
+        <v>102.626012715713</v>
+      </c>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="6">
+        <f>AB5+1</f>
+        <v>2</v>
+      </c>
+      <c r="AC6" s="7">
         <v>90.774341507720237</v>
       </c>
     </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -5150,25 +5292,36 @@
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="3">
-        <v>96.433514986376011</v>
-      </c>
-      <c r="R7" s="2">
+      <c r="N7" s="3"/>
+      <c r="R7" s="6">
         <f t="shared" ref="R7:R54" si="3">R6+1</f>
         <v>3</v>
       </c>
-      <c r="S7" s="3">
-        <v>106.4411807447775</v>
-      </c>
-      <c r="W7" s="2">
+      <c r="S7" s="7">
+        <v>96.433514986376011</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="6">
         <f t="shared" ref="W7:W54" si="4">W6+1</f>
         <v>3</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7" s="7">
+        <v>106.4411807447775</v>
+      </c>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="6">
+        <f t="shared" ref="AB7:AB54" si="5">AB6+1</f>
+        <v>3</v>
+      </c>
+      <c r="AC7" s="7">
         <v>85.78519527702089</v>
       </c>
     </row>
-    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5190,25 +5343,36 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="3"/>
+      <c r="R8" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S8" s="7">
         <v>97.722670299727497</v>
       </c>
-      <c r="R8" s="2">
-        <f t="shared" si="3"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="6">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S8" s="3">
+      <c r="X8" s="7">
         <v>107.03734786557671</v>
       </c>
-      <c r="W8" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="6">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="X8" s="3">
+      <c r="AC8" s="7">
         <v>87.162788374205263</v>
       </c>
     </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5230,25 +5394,36 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="3"/>
+      <c r="R9" s="6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S9" s="7">
         <v>95.699636693914599</v>
       </c>
-      <c r="R9" s="2">
-        <f t="shared" si="3"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="6">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="S9" s="3">
+      <c r="X9" s="7">
         <v>106.6933514986376</v>
       </c>
-      <c r="W9" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="6">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="X9" s="3">
+      <c r="AC9" s="7">
         <v>82.645903723887344</v>
       </c>
     </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5270,25 +5445,36 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="3"/>
+      <c r="R10" s="6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S10" s="7">
         <v>99.081525885558563</v>
       </c>
-      <c r="R10" s="2">
-        <f t="shared" si="3"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="6">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="S10" s="3">
+      <c r="X10" s="7">
         <v>108.07188010899181</v>
       </c>
-      <c r="W10" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="6">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="X10" s="3">
+      <c r="AC10" s="7">
         <v>91.93674841053587</v>
       </c>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5310,25 +5496,36 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="3"/>
+      <c r="R11" s="6">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S11" s="7">
         <v>100.8880653950954</v>
       </c>
-      <c r="R11" s="2">
-        <f t="shared" si="3"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="6">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="S11" s="3">
+      <c r="X11" s="7">
         <v>107.61495004541329</v>
       </c>
-      <c r="W11" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="6">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="X11" s="3">
+      <c r="AC11" s="7">
         <v>93.432107175295158</v>
       </c>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5350,25 +5547,36 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="3"/>
+      <c r="R12" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S12" s="7">
         <v>102.371625794732</v>
       </c>
-      <c r="R12" s="2">
-        <f t="shared" si="3"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="6">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="S12" s="3">
+      <c r="X12" s="7">
         <v>101.9230336058129</v>
       </c>
-      <c r="W12" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="6">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="X12" s="3">
+      <c r="AC12" s="7">
         <v>94.673678474114411</v>
       </c>
     </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5390,25 +5598,36 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="3"/>
+      <c r="R13" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S13" s="7">
         <v>95.690445049954576</v>
       </c>
-      <c r="R13" s="2">
-        <f t="shared" si="3"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="6">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="S13" s="3">
+      <c r="X13" s="7">
         <v>97.759981834695751</v>
       </c>
-      <c r="W13" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="6">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="X13" s="3">
+      <c r="AC13" s="7">
         <v>87.75546775658492</v>
       </c>
     </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5430,25 +5649,36 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="3"/>
+      <c r="R14" s="6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S14" s="7">
         <v>94.250808356039954</v>
       </c>
-      <c r="R14" s="2">
-        <f t="shared" si="3"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="6">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="S14" s="3">
+      <c r="X14" s="7">
         <v>103.3532970027248</v>
       </c>
-      <c r="W14" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="6">
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="X14" s="3">
+      <c r="AC14" s="7">
         <v>86.013742052679362</v>
       </c>
     </row>
-    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5470,25 +5700,36 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="3"/>
+      <c r="R15" s="6">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S15" s="7">
         <v>99.481180744777447</v>
       </c>
-      <c r="R15" s="2">
-        <f t="shared" si="3"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="6">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="S15" s="3">
+      <c r="X15" s="7">
         <v>107.103178928247</v>
       </c>
-      <c r="W15" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="6">
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="X15" s="3">
+      <c r="AC15" s="7">
         <v>86.780753860127149</v>
       </c>
     </row>
-    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5510,25 +5751,36 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="3"/>
+      <c r="R16" s="6">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S16" s="7">
         <v>97.16806539509534</v>
       </c>
-      <c r="R16" s="2">
-        <f t="shared" si="3"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="6">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="S16" s="3">
+      <c r="X16" s="7">
         <v>100.7662488646685</v>
       </c>
-      <c r="W16" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="6">
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="X16" s="3">
+      <c r="AC16" s="7">
         <v>89.040590372388721</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5550,25 +5802,36 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="3"/>
+      <c r="R17" s="6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S17" s="7">
         <v>97.226920980926394</v>
       </c>
-      <c r="R17" s="2">
-        <f t="shared" si="3"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="6">
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="S17" s="3">
+      <c r="X17" s="7">
         <v>99.653841961852848</v>
       </c>
-      <c r="W17" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="6">
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="X17" s="3">
+      <c r="AC17" s="7">
         <v>85.379364214350588</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5590,25 +5853,36 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="3"/>
+      <c r="R18" s="6">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S18" s="7">
         <v>97.207338782924595</v>
       </c>
-      <c r="R18" s="2">
-        <f t="shared" si="3"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="6">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="S18" s="3">
+      <c r="X18" s="7">
         <v>96.098819255222509</v>
       </c>
-      <c r="W18" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="6">
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="X18" s="3">
+      <c r="AC18" s="7">
         <v>94.881226158038118</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5630,25 +5904,36 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="3"/>
+      <c r="R19" s="6">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S19" s="7">
         <v>98.519945504087175</v>
       </c>
-      <c r="R19" s="2">
-        <f t="shared" si="3"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="6">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="S19" s="3">
+      <c r="X19" s="7">
         <v>104.7041598546776</v>
       </c>
-      <c r="W19" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="6">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="X19" s="3">
+      <c r="AC19" s="7">
         <v>92.52339691189826</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5670,25 +5955,36 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="3"/>
+      <c r="R20" s="6">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S20" s="7">
         <v>96.685867393278855</v>
       </c>
-      <c r="R20" s="2">
-        <f t="shared" si="3"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="6">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="S20" s="3">
+      <c r="X20" s="7">
         <v>102.98421435059041</v>
       </c>
-      <c r="W20" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="6">
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="X20" s="3">
+      <c r="AC20" s="7">
         <v>86.403278837420515</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5710,25 +6006,36 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="3"/>
+      <c r="R21" s="6">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S21" s="7">
         <v>92.225940054495894</v>
       </c>
-      <c r="R21" s="2">
-        <f t="shared" si="3"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="6">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="S21" s="3">
+      <c r="X21" s="7">
         <v>101.3662670299727</v>
       </c>
-      <c r="W21" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="6">
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="X21" s="3">
+      <c r="AC21" s="7">
         <v>98.631534968210701</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5750,25 +6057,36 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="3"/>
+      <c r="R22" s="6">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S22" s="7">
         <v>98.478583106267038</v>
       </c>
-      <c r="R22" s="2">
-        <f t="shared" si="3"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="6">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="S22" s="3">
+      <c r="X22" s="7">
         <v>99.515113533151663</v>
       </c>
-      <c r="W22" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="6">
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="X22" s="3">
+      <c r="AC22" s="7">
         <v>88.959645776566731</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5790,25 +6108,36 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="3"/>
+      <c r="R23" s="6">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S23" s="7">
         <v>97.470535876475935</v>
       </c>
-      <c r="R23" s="2">
-        <f t="shared" si="3"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="6">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="S23" s="3">
+      <c r="X23" s="7">
         <v>100.7651771117166</v>
       </c>
-      <c r="W23" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="6">
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="X23" s="3">
+      <c r="AC23" s="7">
         <v>88.016557674841053</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5830,25 +6159,36 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="3"/>
+      <c r="R24" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S24" s="7">
         <v>96.242870118074478</v>
       </c>
-      <c r="R24" s="2">
-        <f t="shared" si="3"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="6">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="S24" s="3">
+      <c r="X24" s="7">
         <v>104.752570390554</v>
       </c>
-      <c r="W24" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="6">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="X24" s="3">
+      <c r="AC24" s="7">
         <v>89.143533151680288</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5870,25 +6210,36 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="3"/>
+      <c r="R25" s="6">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S25" s="7">
         <v>95.880617620345134</v>
       </c>
-      <c r="R25" s="2">
-        <f t="shared" si="3"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="6">
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="S25" s="3">
+      <c r="X25" s="7">
         <v>105.5956403269755</v>
       </c>
-      <c r="W25" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="6">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="X25" s="3">
+      <c r="AC25" s="7">
         <v>87.67952770208899</v>
       </c>
     </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5910,25 +6261,36 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="3"/>
+      <c r="R26" s="6">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S26" s="7">
         <v>98.342270663033617</v>
       </c>
-      <c r="R26" s="2">
-        <f t="shared" si="3"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="6">
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="S26" s="3">
+      <c r="X26" s="7">
         <v>99.840454132606709</v>
       </c>
-      <c r="W26" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="6">
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="X26" s="3">
+      <c r="AC26" s="7">
         <v>90.313015440508607</v>
       </c>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5950,25 +6312,36 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="3"/>
+      <c r="R27" s="6">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S27" s="7">
         <v>96.742325158946372</v>
       </c>
-      <c r="R27" s="2">
-        <f t="shared" si="3"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="6">
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="S27" s="3">
+      <c r="X27" s="7">
         <v>101.5761671207992</v>
       </c>
-      <c r="W27" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="6">
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="X27" s="3">
+      <c r="AC27" s="7">
         <v>87.004931880108984</v>
       </c>
     </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5990,25 +6363,36 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="3"/>
+      <c r="R28" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S28" s="7">
         <v>88.842833787465921</v>
       </c>
-      <c r="R28" s="2">
-        <f t="shared" si="3"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="6">
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="S28" s="3">
+      <c r="X28" s="7">
         <v>102.16663033605811</v>
       </c>
-      <c r="W28" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="6">
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="X28" s="3">
+      <c r="AC28" s="7">
         <v>85.882979109900063</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6030,25 +6414,36 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="3"/>
+      <c r="R29" s="6">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S29" s="7">
         <v>96.177057220708434</v>
       </c>
-      <c r="R29" s="2">
-        <f t="shared" si="3"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="6">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="S29" s="3">
+      <c r="X29" s="7">
         <v>103.1237783832879</v>
       </c>
-      <c r="W29" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="6">
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="X29" s="3">
+      <c r="AC29" s="7">
         <v>91.296830154405072</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6070,25 +6465,36 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30" s="3"/>
+      <c r="R30" s="6">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S30" s="7">
         <v>100.1052861035422</v>
       </c>
-      <c r="R30" s="2">
-        <f t="shared" si="3"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="6">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="S30" s="3">
+      <c r="X30" s="7">
         <v>103.6975840145322</v>
       </c>
-      <c r="W30" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="6">
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
-      <c r="X30" s="3">
+      <c r="AC30" s="7">
         <v>88.128301544050856</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6110,25 +6516,36 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="3"/>
+      <c r="R31" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S31" s="7">
         <v>96.344232515894632</v>
       </c>
-      <c r="R31" s="2">
-        <f t="shared" si="3"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="6">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="S31" s="3">
+      <c r="X31" s="7">
         <v>110.5325340599455</v>
       </c>
-      <c r="W31" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="6">
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="X31" s="3">
+      <c r="AC31" s="7">
         <v>90.746021798365121</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6150,25 +6567,36 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="3"/>
+      <c r="R32" s="6">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S32" s="7">
         <v>94.506394187102615</v>
       </c>
-      <c r="R32" s="2">
-        <f t="shared" si="3"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="6">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="S32" s="3">
+      <c r="X32" s="7">
         <v>103.8625613079019</v>
       </c>
-      <c r="W32" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="6">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="X32" s="3">
+      <c r="AC32" s="7">
         <v>90.751389645776555</v>
       </c>
     </row>
-    <row r="33" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6190,25 +6618,36 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="3"/>
+      <c r="R33" s="6">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S33" s="7">
         <v>96.508446866484988</v>
       </c>
-      <c r="R33" s="2">
-        <f t="shared" si="3"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="6">
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="S33" s="3">
+      <c r="X33" s="7">
         <v>102.9285013623978</v>
       </c>
-      <c r="W33" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="6">
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="X33" s="3">
+      <c r="AC33" s="7">
         <v>88.930199818346935</v>
       </c>
     </row>
-    <row r="34" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -6230,25 +6669,36 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="3"/>
+      <c r="R34" s="6">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S34" s="7">
         <v>93.649445958219786</v>
       </c>
-      <c r="R34" s="2">
-        <f t="shared" si="3"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="6">
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="S34" s="3">
+      <c r="X34" s="7">
         <v>107.4908446866485</v>
       </c>
-      <c r="W34" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="6">
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="X34" s="3">
+      <c r="AC34" s="7">
         <v>95.490772025431397</v>
       </c>
     </row>
-    <row r="35" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -6270,25 +6720,36 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35" s="3"/>
+      <c r="R35" s="6">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S35" s="7">
         <v>99.279636693914597</v>
       </c>
-      <c r="R35" s="2">
-        <f t="shared" si="3"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="6">
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="S35" s="3">
+      <c r="X35" s="7">
         <v>99.137584014532237</v>
       </c>
-      <c r="W35" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="6">
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
-      <c r="X35" s="3">
+      <c r="AC35" s="7">
         <v>91.276875567665755</v>
       </c>
     </row>
-    <row r="36" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -6310,25 +6771,36 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36" s="3"/>
+      <c r="R36" s="6">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S36" s="7">
         <v>91.810299727520416</v>
       </c>
-      <c r="R36" s="2">
-        <f t="shared" si="3"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="6">
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="S36" s="3">
+      <c r="X36" s="7">
         <v>105.4259945504087</v>
       </c>
-      <c r="W36" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="6">
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="X36" s="3">
+      <c r="AC36" s="7">
         <v>91.509618528610346</v>
       </c>
     </row>
-    <row r="37" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -6350,25 +6822,36 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37" s="3"/>
+      <c r="R37" s="6">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S37" s="7">
         <v>96.733896457765667</v>
       </c>
-      <c r="R37" s="2">
-        <f t="shared" si="3"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="6">
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
-      <c r="S37" s="3">
+      <c r="X37" s="7">
         <v>96.313496821071723</v>
       </c>
-      <c r="W37" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="6">
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="X37" s="3">
+      <c r="AC37" s="7">
         <v>84.262098092643058</v>
       </c>
     </row>
-    <row r="38" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -6390,25 +6873,36 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38" s="3"/>
+      <c r="R38" s="6">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S38" s="7">
         <v>96.777075386012697</v>
       </c>
-      <c r="R38" s="2">
-        <f t="shared" si="3"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="6">
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
-      <c r="S38" s="3">
+      <c r="X38" s="7">
         <v>98.811771117166188</v>
       </c>
-      <c r="W38" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="6">
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="X38" s="3">
+      <c r="AC38" s="7">
         <v>87.599827429609419</v>
       </c>
     </row>
-    <row r="39" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -6430,25 +6924,36 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39" s="3"/>
+      <c r="R39" s="6">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S39" s="7">
         <v>88.399436875567645</v>
       </c>
-      <c r="R39" s="2">
-        <f t="shared" si="3"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="6">
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="S39" s="3">
+      <c r="X39" s="7">
         <v>101.2734059945504</v>
       </c>
-      <c r="W39" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="6">
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="X39" s="3">
+      <c r="AC39" s="7">
         <v>90.224386920980919</v>
       </c>
     </row>
-    <row r="40" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -6470,25 +6975,36 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40" s="3"/>
+      <c r="R40" s="6">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S40" s="7">
         <v>95.027593097184365</v>
       </c>
-      <c r="R40" s="2">
-        <f t="shared" si="3"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="6">
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="S40" s="3">
+      <c r="X40" s="7">
         <v>104.6140599455041</v>
       </c>
-      <c r="W40" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="6">
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
-      <c r="X40" s="3">
+      <c r="AC40" s="7">
         <v>87.5166303360581</v>
       </c>
     </row>
-    <row r="41" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -6510,25 +7026,36 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41" s="3"/>
+      <c r="R41" s="6">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S41" s="7">
         <v>99.227556766575816</v>
       </c>
-      <c r="R41" s="2">
-        <f t="shared" si="3"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="6">
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
-      <c r="S41" s="3">
+      <c r="X41" s="7">
         <v>107.5674114441417</v>
       </c>
-      <c r="W41" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="6">
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
-      <c r="X41" s="3">
+      <c r="AC41" s="7">
         <v>91.114931880108983</v>
       </c>
     </row>
-    <row r="42" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -6550,25 +7077,36 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42" s="3"/>
+      <c r="R42" s="6">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S42" s="7">
         <v>94.925104450499546</v>
       </c>
-      <c r="R42" s="2">
-        <f t="shared" si="3"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="6">
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="S42" s="3">
+      <c r="X42" s="7">
         <v>100.45193460490459</v>
       </c>
-      <c r="W42" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="6">
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
-      <c r="X42" s="3">
+      <c r="AC42" s="7">
         <v>85.231998183469571</v>
       </c>
     </row>
-    <row r="43" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -6590,25 +7128,36 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43" s="3"/>
+      <c r="R43" s="6">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S43" s="7">
         <v>96.752425068119877</v>
       </c>
-      <c r="R43" s="2">
-        <f t="shared" si="3"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="6">
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
-      <c r="S43" s="3">
+      <c r="X43" s="7">
         <v>99.968446866485024</v>
       </c>
-      <c r="W43" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="6">
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
-      <c r="X43" s="3">
+      <c r="AC43" s="7">
         <v>97.581153496821045</v>
       </c>
     </row>
-    <row r="44" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -6630,25 +7179,36 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44" s="3"/>
+      <c r="R44" s="6">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S44" s="7">
         <v>93.38519527702087</v>
       </c>
-      <c r="R44" s="2">
-        <f t="shared" si="3"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="6">
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="S44" s="3">
+      <c r="X44" s="7">
         <v>104.2006176203451</v>
       </c>
-      <c r="W44" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="6">
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="X44" s="3">
+      <c r="AC44" s="7">
         <v>88.226839237057206</v>
       </c>
     </row>
-    <row r="45" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -6670,25 +7230,36 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45" s="3"/>
+      <c r="R45" s="6">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S45" s="7">
         <v>97.961271571298823</v>
       </c>
-      <c r="R45" s="2">
-        <f t="shared" si="3"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="6">
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
-      <c r="S45" s="3">
+      <c r="X45" s="7">
         <v>101.72713896457761</v>
       </c>
-      <c r="W45" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="6">
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
-      <c r="X45" s="3">
+      <c r="AC45" s="7">
         <v>89.008274296094442</v>
       </c>
     </row>
-    <row r="46" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -6710,25 +7281,36 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="3">
+      <c r="N46" s="3"/>
+      <c r="R46" s="6">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S46" s="7">
         <v>100.3552770208901</v>
       </c>
-      <c r="R46" s="2">
-        <f t="shared" si="3"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="6">
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="S46" s="3">
+      <c r="X46" s="7">
         <v>102.7732243415077</v>
       </c>
-      <c r="W46" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="6">
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="X46" s="3">
+      <c r="AC46" s="7">
         <v>89.192125340599432</v>
       </c>
     </row>
-    <row r="47" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -6750,25 +7332,36 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="3"/>
+      <c r="R47" s="6">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S47" s="7">
         <v>88.122034514078095</v>
       </c>
-      <c r="R47" s="2">
-        <f t="shared" si="3"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="6">
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="S47" s="3">
+      <c r="X47" s="7">
         <v>96.002670299727498</v>
       </c>
-      <c r="W47" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="6">
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
-      <c r="X47" s="3">
+      <c r="AC47" s="7">
         <v>88.577783832879192</v>
       </c>
     </row>
-    <row r="48" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -6790,25 +7383,36 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48" s="3"/>
+      <c r="R48" s="6">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S48" s="7">
         <v>96.941798365122608</v>
       </c>
-      <c r="R48" s="2">
-        <f t="shared" si="3"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="6">
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="S48" s="3">
+      <c r="X48" s="7">
         <v>103.0816712079927</v>
       </c>
-      <c r="W48" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="6">
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
-      <c r="X48" s="3">
+      <c r="AC48" s="7">
         <v>85.697974568574026</v>
       </c>
     </row>
-    <row r="49" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -6830,25 +7434,36 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N49" s="3"/>
+      <c r="R49" s="6">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S49" s="7">
         <v>100.921689373297</v>
       </c>
-      <c r="R49" s="2">
-        <f t="shared" si="3"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="6">
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="S49" s="3">
+      <c r="X49" s="7">
         <v>109.4195095367847</v>
       </c>
-      <c r="W49" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="5"/>
+      <c r="AB49" s="6">
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
-      <c r="X49" s="3">
+      <c r="AC49" s="7">
         <v>88.000681198910087</v>
       </c>
     </row>
-    <row r="50" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -6870,25 +7485,36 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50" s="3"/>
+      <c r="R50" s="6">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S50" s="7">
         <v>100.47603996366939</v>
       </c>
-      <c r="R50" s="2">
-        <f t="shared" si="3"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="6">
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="S50" s="3">
+      <c r="X50" s="7">
         <v>106.3633605812897</v>
       </c>
-      <c r="W50" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="6">
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
-      <c r="X50" s="3">
+      <c r="AC50" s="7">
         <v>91.759391462306979</v>
       </c>
     </row>
-    <row r="51" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -6910,25 +7536,36 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51" s="3"/>
+      <c r="R51" s="6">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S51" s="7">
         <v>97.53785649409626</v>
       </c>
-      <c r="R51" s="2">
-        <f t="shared" si="3"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="6">
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
-      <c r="S51" s="3">
+      <c r="X51" s="7">
         <v>105.8273569482289</v>
       </c>
-      <c r="W51" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="6">
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="X51" s="3">
+      <c r="AC51" s="7">
         <v>92.005994550408701</v>
       </c>
     </row>
-    <row r="52" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -6950,25 +7587,36 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52" s="3"/>
+      <c r="R52" s="6">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S52" s="7">
         <v>94.146539509536751</v>
       </c>
-      <c r="R52" s="2">
-        <f t="shared" si="3"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="6">
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="S52" s="3">
+      <c r="X52" s="7">
         <v>97.299218891916411</v>
       </c>
-      <c r="W52" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y52" s="5"/>
+      <c r="Z52" s="5"/>
+      <c r="AA52" s="5"/>
+      <c r="AB52" s="6">
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="X52" s="3">
+      <c r="AC52" s="7">
         <v>90.787511353315168</v>
       </c>
     </row>
-    <row r="53" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -6990,25 +7638,36 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="3">
+      <c r="N53" s="3"/>
+      <c r="R53" s="6">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S53" s="7">
         <v>91.838655767484099</v>
       </c>
-      <c r="R53" s="2">
-        <f t="shared" si="3"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="6">
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="S53" s="3">
+      <c r="X53" s="7">
         <v>99.88263396911897</v>
       </c>
-      <c r="W53" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="5"/>
+      <c r="AB53" s="6">
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="X53" s="3">
+      <c r="AC53" s="7">
         <v>92.229909173478632</v>
       </c>
     </row>
-    <row r="54" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -7030,25 +7689,50 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="3">
+      <c r="N54" s="3"/>
+      <c r="R54" s="6">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S54" s="7">
         <v>92.166957311534972</v>
       </c>
-      <c r="R54" s="2">
-        <f t="shared" si="3"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="6">
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="S54" s="3">
+      <c r="X54" s="7">
         <v>103.7087011807448</v>
       </c>
-      <c r="W54" s="2">
-        <f t="shared" si="4"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="6">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="X54" s="3">
+      <c r="AC54" s="7">
         <v>91.308319709355118</v>
       </c>
     </row>
-    <row r="56" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="5"/>
+      <c r="AC55" s="5"/>
+    </row>
+    <row r="56" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
@@ -7070,26 +7754,39 @@
       <c r="M56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N56" s="3">
+      <c r="N56" s="3" t="e">
         <f>AVERAGE(N5:N54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="S56" s="7">
+        <f>AVERAGE(S5:S54)</f>
         <v>96.445187647593102</v>
       </c>
-      <c r="R56" s="2" t="s">
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="S56" s="3">
-        <f>AVERAGE(S5:S54)</f>
+      <c r="X56" s="7">
+        <f>AVERAGE(X5:X54)</f>
         <v>103.04385467756582</v>
       </c>
-      <c r="W56" s="2" t="s">
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="X56" s="3">
-        <f>AVERAGE(X5:X54)</f>
+      <c r="AC56" s="7">
+        <f>AVERAGE(AC5:AC54)</f>
         <v>89.620815622161643</v>
       </c>
     </row>
-    <row r="57" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
@@ -7111,22 +7808,35 @@
       <c r="M57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N57" s="3">
+      <c r="N57" s="3" t="e">
         <f>_xlfn.STDEV.S(N5:N54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R57" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S57" s="7">
+        <f>_xlfn.STDEV.S(S5:S54)</f>
         <v>3.2340449236910516</v>
       </c>
-      <c r="R57" s="2" t="s">
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="S57" s="3">
-        <f>_xlfn.STDEV.S(S5:S54)</f>
+      <c r="X57" s="7">
+        <f>_xlfn.STDEV.S(X5:X54)</f>
         <v>3.5862149092731741</v>
       </c>
-      <c r="W57" s="2" t="s">
+      <c r="Y57" s="5"/>
+      <c r="Z57" s="5"/>
+      <c r="AA57" s="5"/>
+      <c r="AB57" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X57" s="3">
-        <f>_xlfn.STDEV.S(X5:X54)</f>
+      <c r="AC57" s="7">
+        <f>_xlfn.STDEV.S(AC5:AC54)</f>
         <v>3.3003922255215064</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test-23: hybrid model 2.0 (mae)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -5098,8 +5098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AC57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5193,7 +5193,9 @@
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="3"/>
+      <c r="N5" s="3">
+        <v>151.31760073260071</v>
+      </c>
       <c r="R5" s="6">
         <v>1</v>
       </c>
@@ -5241,7 +5243,9 @@
         <f>M5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="3"/>
+      <c r="N6" s="3">
+        <v>146.75019230769229</v>
+      </c>
       <c r="R6" s="6">
         <f>R5+1</f>
         <v>2</v>
@@ -5292,7 +5296,9 @@
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="3"/>
+      <c r="N7" s="3">
+        <v>151.75852564102561</v>
+      </c>
       <c r="R7" s="6">
         <f t="shared" ref="R7:R54" si="3">R6+1</f>
         <v>3</v>
@@ -5343,7 +5349,9 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="3"/>
+      <c r="N8" s="3">
+        <v>146.52972527472531</v>
+      </c>
       <c r="R8" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -5394,7 +5402,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="3"/>
+      <c r="N9" s="3">
+        <v>150.58698717948721</v>
+      </c>
       <c r="R9" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -5445,7 +5455,9 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="3"/>
+      <c r="N10" s="3">
+        <v>148.0550366300366</v>
+      </c>
       <c r="R10" s="6">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -5496,7 +5508,9 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="3"/>
+      <c r="N11" s="3">
+        <v>152.37920329670331</v>
+      </c>
       <c r="R11" s="6">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -5547,7 +5561,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="3"/>
+      <c r="N12" s="3">
+        <v>150.49828754578749</v>
+      </c>
       <c r="R12" s="6">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -5598,7 +5614,9 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="3"/>
+      <c r="N13" s="3">
+        <v>146.59293956043959</v>
+      </c>
       <c r="R13" s="6">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -5649,7 +5667,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="3"/>
+      <c r="N14" s="3">
+        <v>147.73905677655679</v>
+      </c>
       <c r="R14" s="6">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -5700,7 +5720,9 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="3"/>
+      <c r="N15" s="3">
+        <v>143.57090659340659</v>
+      </c>
       <c r="R15" s="6">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -5751,7 +5773,9 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="N16" s="3">
+        <v>147.86541208791209</v>
+      </c>
       <c r="R16" s="6">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -5802,7 +5826,9 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="3"/>
+      <c r="N17" s="3">
+        <v>152.67599816849821</v>
+      </c>
       <c r="R17" s="6">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -5853,7 +5879,9 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3">
+        <v>152.52029304029301</v>
+      </c>
       <c r="R18" s="6">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -5904,7 +5932,9 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="3"/>
+      <c r="N19" s="3">
+        <v>149.13102564102559</v>
+      </c>
       <c r="R19" s="6">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -5955,7 +5985,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="3"/>
+      <c r="N20" s="3">
+        <v>156.84835164835161</v>
+      </c>
       <c r="R20" s="6">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -6006,7 +6038,9 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="3"/>
+      <c r="N21" s="3">
+        <v>149.82247252747251</v>
+      </c>
       <c r="R21" s="6">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -6057,7 +6091,9 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="3"/>
+      <c r="N22" s="3">
+        <v>148.12906593406589</v>
+      </c>
       <c r="R22" s="6">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -6108,7 +6144,9 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="3"/>
+      <c r="N23" s="3">
+        <v>152.40857142857141</v>
+      </c>
       <c r="R23" s="6">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -6159,7 +6197,9 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="3"/>
+      <c r="N24" s="3">
+        <v>153.9892765567765</v>
+      </c>
       <c r="R24" s="6">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -6210,7 +6250,9 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="3"/>
+      <c r="N25" s="3">
+        <v>149.8605494505494</v>
+      </c>
       <c r="R25" s="6">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -6261,7 +6303,9 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="3"/>
+      <c r="N26" s="3">
+        <v>149.01124542124541</v>
+      </c>
       <c r="R26" s="6">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -6312,7 +6356,9 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="3"/>
+      <c r="N27" s="3">
+        <v>141.23052197802201</v>
+      </c>
       <c r="R27" s="6">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -6363,7 +6409,9 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="3"/>
+      <c r="N28" s="3">
+        <v>146.41163003662999</v>
+      </c>
       <c r="R28" s="6">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -6414,7 +6462,9 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="3"/>
+      <c r="N29" s="3">
+        <v>146.99540293040289</v>
+      </c>
       <c r="R29" s="6">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -6465,7 +6515,9 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="3"/>
+      <c r="N30" s="3">
+        <v>158.6069413919414</v>
+      </c>
       <c r="R30" s="6">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -6516,7 +6568,9 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="3"/>
+      <c r="N31" s="3">
+        <v>152.46016483516479</v>
+      </c>
       <c r="R31" s="6">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -6567,7 +6621,9 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="3"/>
+      <c r="N32" s="3">
+        <v>152.61486263736259</v>
+      </c>
       <c r="R32" s="6">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -6618,7 +6674,9 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="3"/>
+      <c r="N33" s="3">
+        <v>153.1728113553113</v>
+      </c>
       <c r="R33" s="6">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -6669,7 +6727,9 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="3"/>
+      <c r="N34" s="3">
+        <v>149.62616300366301</v>
+      </c>
       <c r="R34" s="6">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -6720,7 +6780,9 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="3"/>
+      <c r="N35" s="3">
+        <v>149.36065934065931</v>
+      </c>
       <c r="R35" s="6">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -6771,7 +6833,9 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="3"/>
+      <c r="N36" s="3">
+        <v>156.1604487179487</v>
+      </c>
       <c r="R36" s="6">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -6822,7 +6886,9 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="3"/>
+      <c r="N37" s="3">
+        <v>151.00489926739931</v>
+      </c>
       <c r="R37" s="6">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -6873,7 +6939,9 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="3"/>
+      <c r="N38" s="3">
+        <v>148.1982692307692</v>
+      </c>
       <c r="R38" s="6">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -6924,7 +6992,9 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="3"/>
+      <c r="N39" s="3">
+        <v>163.35634615384609</v>
+      </c>
       <c r="R39" s="6">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -6975,7 +7045,9 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="3"/>
+      <c r="N40" s="3">
+        <v>146.98697802197799</v>
+      </c>
       <c r="R40" s="6">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -7026,7 +7098,9 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="3"/>
+      <c r="N41" s="3">
+        <v>155.32771062271061</v>
+      </c>
       <c r="R41" s="6">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -7077,7 +7151,9 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="3"/>
+      <c r="N42" s="3">
+        <v>147.7697527472528</v>
+      </c>
       <c r="R42" s="6">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -7128,7 +7204,9 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="3"/>
+      <c r="N43" s="3">
+        <v>148.12145604395599</v>
+      </c>
       <c r="R43" s="6">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -7179,7 +7257,9 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="3"/>
+      <c r="N44" s="3">
+        <v>142.25531135531131</v>
+      </c>
       <c r="R44" s="6">
         <f t="shared" si="3"/>
         <v>40</v>
@@ -7230,7 +7310,9 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="3"/>
+      <c r="N45" s="3">
+        <v>141.5760714285714</v>
+      </c>
       <c r="R45" s="6">
         <f t="shared" si="3"/>
         <v>41</v>
@@ -7281,7 +7363,9 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="3"/>
+      <c r="N46" s="3">
+        <v>145.03771978021979</v>
+      </c>
       <c r="R46" s="6">
         <f t="shared" si="3"/>
         <v>42</v>
@@ -7332,7 +7416,9 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="3"/>
+      <c r="N47" s="3">
+        <v>145.27836080586081</v>
+      </c>
       <c r="R47" s="6">
         <f t="shared" si="3"/>
         <v>43</v>
@@ -7383,7 +7469,9 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="3"/>
+      <c r="N48" s="3">
+        <v>142.55758241758241</v>
+      </c>
       <c r="R48" s="6">
         <f t="shared" si="3"/>
         <v>44</v>
@@ -7434,7 +7522,9 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="3"/>
+      <c r="N49" s="3">
+        <v>150.63672161172161</v>
+      </c>
       <c r="R49" s="6">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -7485,7 +7575,9 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="3"/>
+      <c r="N50" s="3">
+        <v>151.16726190476189</v>
+      </c>
       <c r="R50" s="6">
         <f t="shared" si="3"/>
         <v>46</v>
@@ -7536,7 +7628,9 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="3"/>
+      <c r="N51" s="3">
+        <v>147.01094322344321</v>
+      </c>
       <c r="R51" s="6">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -7587,7 +7681,9 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="3"/>
+      <c r="N52" s="3">
+        <v>149.3844139194139</v>
+      </c>
       <c r="R52" s="6">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -7638,7 +7734,9 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="3"/>
+      <c r="N53" s="3">
+        <v>138.42366300366299</v>
+      </c>
       <c r="R53" s="6">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -7689,7 +7787,9 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="3"/>
+      <c r="N54" s="3">
+        <v>147.03862637362641</v>
+      </c>
       <c r="R54" s="6">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -7754,9 +7854,9 @@
       <c r="M56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N56" s="3" t="e">
+      <c r="N56" s="3">
         <f>AVERAGE(N5:N54)</f>
-        <v>#DIV/0!</v>
+        <v>149.31624835164834</v>
       </c>
       <c r="R56" s="6" t="s">
         <v>3</v>
@@ -7808,9 +7908,9 @@
       <c r="M57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N57" s="3" t="e">
+      <c r="N57" s="3">
         <f>_xlfn.STDEV.S(N5:N54)</f>
-        <v>#DIV/0!</v>
+        <v>4.5494683369505582</v>
       </c>
       <c r="R57" s="6" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
test-23: 3Ysum extrapol 2.0
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="19">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Hybrid model 2.0 (superdataset-24-f + 2Y.csv)</t>
+  </si>
+  <si>
+    <t>RF-100 (superdataset-24-f 2Y.csv + extrapol 2.0)</t>
+  </si>
+  <si>
+    <t>Hybrid3 model 2.0 (superdataset-24-f + 2Y + 3Y.csv)</t>
   </si>
 </sst>
 </file>
@@ -5098,7 +5104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AC57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
@@ -7947,27 +7953,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O56"/>
+  <dimension ref="C2:Z56"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="U2" s="5"/>
+      <c r="Y2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="Z2" s="5"/>
+    </row>
+    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>1</v>
@@ -7983,8 +7997,16 @@
       <c r="O3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="T3" s="6"/>
+      <c r="U3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -7998,16 +8020,26 @@
         <v>1</v>
       </c>
       <c r="J4" s="3">
-        <v>0.74759938062002673</v>
+        <v>0.57834400411422515</v>
       </c>
       <c r="N4" s="2">
         <v>1</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="3"/>
+      <c r="T4" s="6">
+        <v>1</v>
+      </c>
+      <c r="U4" s="7">
+        <v>0.74759938062002673</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="7">
         <v>0.78489980504236645</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <f>C4+1</f>
         <v>2</v>
@@ -8023,17 +8055,29 @@
         <v>2</v>
       </c>
       <c r="J5" s="3">
-        <v>0.75272216793297142</v>
+        <v>0.5172853331948799</v>
       </c>
       <c r="N5" s="2">
         <f>N4+1</f>
         <v>2</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="3"/>
+      <c r="T5" s="6">
+        <f>T4+1</f>
+        <v>2</v>
+      </c>
+      <c r="U5" s="7">
+        <v>0.75272216793297142</v>
+      </c>
+      <c r="Y5" s="6">
+        <f>Y4+1</f>
+        <v>2</v>
+      </c>
+      <c r="Z5" s="7">
         <v>0.76889713805937721</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f t="shared" ref="C6:C53" si="0">C5+1</f>
         <v>3</v>
@@ -8049,17 +8093,29 @@
         <v>3</v>
       </c>
       <c r="J6" s="3">
-        <v>0.81290062745285052</v>
+        <v>0.56135559361634901</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" ref="N6:N53" si="2">N5+1</f>
         <v>3</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="3"/>
+      <c r="T6" s="6">
+        <f t="shared" ref="T6:T53" si="3">T5+1</f>
+        <v>3</v>
+      </c>
+      <c r="U6" s="7">
+        <v>0.81290062745285052</v>
+      </c>
+      <c r="Y6" s="6">
+        <f t="shared" ref="Y6:Y53" si="4">Y5+1</f>
+        <v>3</v>
+      </c>
+      <c r="Z6" s="7">
         <v>0.80729775526569381</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8075,17 +8131,29 @@
         <v>4</v>
       </c>
       <c r="J7" s="3">
+        <v>0.56287075662473007</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="T7" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U7" s="7">
         <v>0.76359659281275505</v>
       </c>
-      <c r="N7" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y7" s="6">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="O7" s="3">
+      <c r="Z7" s="7">
         <v>0.77998675978926502</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8101,17 +8169,29 @@
         <v>5</v>
       </c>
       <c r="J8" s="3">
+        <v>0.5081679829283714</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="T8" s="6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="U8" s="7">
         <v>0.7545887963884832</v>
       </c>
-      <c r="N8" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y8" s="6">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="O8" s="3">
+      <c r="Z8" s="7">
         <v>0.74093244213597886</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8127,17 +8207,29 @@
         <v>6</v>
       </c>
       <c r="J9" s="3">
+        <v>0.56977280792018892</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="T9" s="6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="U9" s="7">
         <v>0.80385166737402391</v>
       </c>
-      <c r="N9" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y9" s="6">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="O9" s="3">
+      <c r="Z9" s="7">
         <v>0.78829967713958138</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8153,17 +8245,29 @@
         <v>7</v>
       </c>
       <c r="J10" s="3">
+        <v>0.52003827473417497</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="T10" s="6">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="U10" s="7">
         <v>0.81537059224632424</v>
       </c>
-      <c r="N10" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y10" s="6">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="O10" s="3">
+      <c r="Z10" s="7">
         <v>0.73867871133666696</v>
       </c>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8179,17 +8283,29 @@
         <v>8</v>
       </c>
       <c r="J11" s="3">
+        <v>0.46539564064000999</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="T11" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="U11" s="7">
         <v>0.80425470934478516</v>
       </c>
-      <c r="N11" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y11" s="6">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="O11" s="3">
+      <c r="Z11" s="7">
         <v>0.79989025541292258</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8205,17 +8321,29 @@
         <v>9</v>
       </c>
       <c r="J12" s="3">
+        <v>0.52738054435967174</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="T12" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="U12" s="7">
         <v>0.7576941490745841</v>
       </c>
-      <c r="N12" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y12" s="6">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="O12" s="3">
+      <c r="Z12" s="7">
         <v>0.80930455026279047</v>
       </c>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8231,17 +8359,29 @@
         <v>10</v>
       </c>
       <c r="J13" s="3">
+        <v>0.4888645545312692</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="T13" s="6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="U13" s="7">
         <v>0.74667295040812309</v>
       </c>
-      <c r="N13" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y13" s="6">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="O13" s="3">
+      <c r="Z13" s="7">
         <v>0.77140772157724169</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8257,17 +8397,29 @@
         <v>11</v>
       </c>
       <c r="J14" s="3">
+        <v>0.51058084555486583</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O14" s="3"/>
+      <c r="T14" s="6">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="U14" s="7">
         <v>0.78479006333818369</v>
       </c>
-      <c r="N14" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y14" s="6">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="O14" s="3">
+      <c r="Z14" s="7">
         <v>0.80790040470964197</v>
       </c>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -8283,17 +8435,29 @@
         <v>12</v>
       </c>
       <c r="J15" s="3">
+        <v>0.563488646066719</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O15" s="3"/>
+      <c r="T15" s="6">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="U15" s="7">
         <v>0.77498508287134604</v>
       </c>
-      <c r="N15" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y15" s="6">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="O15" s="3">
+      <c r="Z15" s="7">
         <v>0.75474996548915196</v>
       </c>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -8309,17 +8473,29 @@
         <v>13</v>
       </c>
       <c r="J16" s="3">
+        <v>0.51147828263257689</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="T16" s="6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="U16" s="7">
         <v>0.76680506361277445</v>
       </c>
-      <c r="N16" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y16" s="6">
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="O16" s="3">
+      <c r="Z16" s="7">
         <v>0.81167527136343665</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8335,17 +8511,29 @@
         <v>14</v>
       </c>
       <c r="J17" s="3">
+        <v>0.4834937046000386</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O17" s="3"/>
+      <c r="T17" s="6">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="U17" s="7">
         <v>0.79547860900348266</v>
       </c>
-      <c r="N17" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y17" s="6">
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="O17" s="3">
+      <c r="Z17" s="7">
         <v>0.80066366481058293</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8361,17 +8549,29 @@
         <v>15</v>
       </c>
       <c r="J18" s="3">
+        <v>0.54381787801258175</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O18" s="3"/>
+      <c r="T18" s="6">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="U18" s="7">
         <v>0.80253923797160254</v>
       </c>
-      <c r="N18" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y18" s="6">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="O18" s="3">
+      <c r="Z18" s="7">
         <v>0.79379990111229703</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -8387,17 +8587,29 @@
         <v>16</v>
       </c>
       <c r="J19" s="3">
+        <v>0.5761527509110238</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O19" s="3"/>
+      <c r="T19" s="6">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="U19" s="7">
         <v>0.75811037408550375</v>
       </c>
-      <c r="N19" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y19" s="6">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="O19" s="3">
+      <c r="Z19" s="7">
         <v>0.79330358700648618</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -8413,17 +8625,29 @@
         <v>17</v>
       </c>
       <c r="J20" s="3">
+        <v>0.6003089088774205</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O20" s="3"/>
+      <c r="T20" s="6">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="U20" s="7">
         <v>0.80959496508752071</v>
       </c>
-      <c r="N20" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y20" s="6">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="O20" s="3">
+      <c r="Z20" s="7">
         <v>0.80364508616800112</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -8439,17 +8663,29 @@
         <v>18</v>
       </c>
       <c r="J21" s="3">
+        <v>0.53130747434539705</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O21" s="3"/>
+      <c r="T21" s="6">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="U21" s="7">
         <v>0.78243223145681651</v>
       </c>
-      <c r="N21" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y21" s="6">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="O21" s="3">
+      <c r="Z21" s="7">
         <v>0.8358005987200301</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -8465,17 +8701,29 @@
         <v>19</v>
       </c>
       <c r="J22" s="3">
+        <v>0.43865025485995213</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O22" s="3"/>
+      <c r="T22" s="6">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="U22" s="7">
         <v>0.79065531295771696</v>
       </c>
-      <c r="N22" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y22" s="6">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="O22" s="3">
+      <c r="Z22" s="7">
         <v>0.79355445633115396</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -8491,17 +8739,29 @@
         <v>20</v>
       </c>
       <c r="J23" s="3">
+        <v>0.58465011076149842</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O23" s="3"/>
+      <c r="T23" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="U23" s="7">
         <v>0.75111177334431645</v>
       </c>
-      <c r="N23" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y23" s="6">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="O23" s="3">
+      <c r="Z23" s="7">
         <v>0.78853351229375457</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -8517,17 +8777,29 @@
         <v>21</v>
       </c>
       <c r="J24" s="3">
+        <v>0.57326671389181705</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O24" s="3"/>
+      <c r="T24" s="6">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="U24" s="7">
         <v>0.7933349338637159</v>
       </c>
-      <c r="N24" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y24" s="6">
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="O24" s="3">
+      <c r="Z24" s="7">
         <v>0.78748954623838974</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -8543,17 +8815,29 @@
         <v>22</v>
       </c>
       <c r="J25" s="3">
+        <v>0.49476677066589658</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O25" s="3"/>
+      <c r="T25" s="6">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="U25" s="7">
         <v>0.7431987341233699</v>
       </c>
-      <c r="N25" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y25" s="6">
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="O25" s="3">
+      <c r="Z25" s="7">
         <v>0.80992712180274473</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -8569,17 +8853,29 @@
         <v>23</v>
       </c>
       <c r="J26" s="3">
+        <v>0.5002916618770199</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O26" s="3"/>
+      <c r="T26" s="6">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="U26" s="7">
         <v>0.80481897041530459</v>
       </c>
-      <c r="N26" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y26" s="6">
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="O26" s="3">
+      <c r="Z26" s="7">
         <v>0.77620233911398839</v>
       </c>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -8595,17 +8891,29 @@
         <v>24</v>
       </c>
       <c r="J27" s="3">
+        <v>0.49019982541415219</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O27" s="3"/>
+      <c r="T27" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="U27" s="7">
         <v>0.77831347161363618</v>
       </c>
-      <c r="N27" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y27" s="6">
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="O27" s="3">
+      <c r="Z27" s="7">
         <v>0.80374149857995725</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -8621,17 +8929,29 @@
         <v>25</v>
       </c>
       <c r="J28" s="3">
+        <v>0.51516579421759845</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O28" s="3"/>
+      <c r="T28" s="6">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="U28" s="7">
         <v>0.73250447421016152</v>
       </c>
-      <c r="N28" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y28" s="6">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="O28" s="3">
+      <c r="Z28" s="7">
         <v>0.77311927125394853</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -8647,17 +8967,29 @@
         <v>26</v>
       </c>
       <c r="J29" s="3">
+        <v>0.56374703719391916</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O29" s="3"/>
+      <c r="T29" s="6">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="U29" s="7">
         <v>0.79928969776231029</v>
       </c>
-      <c r="N29" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y29" s="6">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="O29" s="3">
+      <c r="Z29" s="7">
         <v>0.79561855051336716</v>
       </c>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -8673,17 +9005,29 @@
         <v>27</v>
       </c>
       <c r="J30" s="3">
+        <v>0.52353799742386575</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O30" s="3"/>
+      <c r="T30" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="U30" s="7">
         <v>0.80145040301035131</v>
       </c>
-      <c r="N30" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y30" s="6">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="O30" s="3">
+      <c r="Z30" s="7">
         <v>0.81308835275443048</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -8699,17 +9043,29 @@
         <v>28</v>
       </c>
       <c r="J31" s="3">
+        <v>0.53240531571446525</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O31" s="3"/>
+      <c r="T31" s="6">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="U31" s="7">
         <v>0.79203197789581958</v>
       </c>
-      <c r="N31" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y31" s="6">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="O31" s="3">
+      <c r="Z31" s="7">
         <v>0.8111886017465374</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -8725,17 +9081,29 @@
         <v>29</v>
       </c>
       <c r="J32" s="3">
+        <v>0.50613099678628659</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O32" s="3"/>
+      <c r="T32" s="6">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="U32" s="7">
         <v>0.74549347792987275</v>
       </c>
-      <c r="N32" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y32" s="6">
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="O32" s="3">
+      <c r="Z32" s="7">
         <v>0.79891958026776666</v>
       </c>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -8751,17 +9119,29 @@
         <v>30</v>
       </c>
       <c r="J33" s="3">
+        <v>0.52438639008761223</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O33" s="3"/>
+      <c r="T33" s="6">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="U33" s="7">
         <v>0.78356932624316888</v>
       </c>
-      <c r="N33" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y33" s="6">
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="O33" s="3">
+      <c r="Z33" s="7">
         <v>0.79637222780511763</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -8777,17 +9157,29 @@
         <v>31</v>
       </c>
       <c r="J34" s="3">
+        <v>0.6169610482762905</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O34" s="3"/>
+      <c r="T34" s="6">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="U34" s="7">
         <v>0.78165766235738088</v>
       </c>
-      <c r="N34" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y34" s="6">
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="O34" s="3">
+      <c r="Z34" s="7">
         <v>0.80490616625728184</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -8803,17 +9195,29 @@
         <v>32</v>
       </c>
       <c r="J35" s="3">
+        <v>0.50156675152561681</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O35" s="3"/>
+      <c r="T35" s="6">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="U35" s="7">
         <v>0.8129048890288546</v>
       </c>
-      <c r="N35" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y35" s="6">
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="O35" s="3">
+      <c r="Z35" s="7">
         <v>0.79844802895196509</v>
       </c>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -8829,17 +9233,29 @@
         <v>33</v>
       </c>
       <c r="J36" s="3">
+        <v>0.52652791568615509</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O36" s="3"/>
+      <c r="T36" s="6">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="U36" s="7">
         <v>0.80361307339161958</v>
       </c>
-      <c r="N36" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y36" s="6">
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
-      <c r="O36" s="3">
+      <c r="Z36" s="7">
         <v>0.81164488617488939</v>
       </c>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -8855,17 +9271,29 @@
         <v>34</v>
       </c>
       <c r="J37" s="3">
+        <v>0.53958384752298505</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O37" s="3"/>
+      <c r="T37" s="6">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="U37" s="7">
         <v>0.77850151482103791</v>
       </c>
-      <c r="N37" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y37" s="6">
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
-      <c r="O37" s="3">
+      <c r="Z37" s="7">
         <v>0.78931160602477124</v>
       </c>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -8881,17 +9309,29 @@
         <v>35</v>
       </c>
       <c r="J38" s="3">
+        <v>0.57057254664261059</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O38" s="3"/>
+      <c r="T38" s="6">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="U38" s="7">
         <v>0.76357957335404536</v>
       </c>
-      <c r="N38" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y38" s="6">
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="O38" s="3">
+      <c r="Z38" s="7">
         <v>0.81606363231006518</v>
       </c>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -8907,17 +9347,29 @@
         <v>36</v>
       </c>
       <c r="J39" s="3">
+        <v>0.50221572484548593</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O39" s="3"/>
+      <c r="T39" s="6">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="U39" s="7">
         <v>0.82719591105098256</v>
       </c>
-      <c r="N39" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y39" s="6">
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="O39" s="3">
+      <c r="Z39" s="7">
         <v>0.81628912563866352</v>
       </c>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -8933,17 +9385,29 @@
         <v>37</v>
       </c>
       <c r="J40" s="3">
+        <v>0.54793609137779353</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O40" s="3"/>
+      <c r="T40" s="6">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="U40" s="7">
         <v>0.78768718630391255</v>
       </c>
-      <c r="N40" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y40" s="6">
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
-      <c r="O40" s="3">
+      <c r="Z40" s="7">
         <v>0.79620131781626413</v>
       </c>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -8959,17 +9423,29 @@
         <v>38</v>
       </c>
       <c r="J41" s="3">
+        <v>0.53644652056062414</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O41" s="3"/>
+      <c r="T41" s="6">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="U41" s="7">
         <v>0.80721891304325188</v>
       </c>
-      <c r="N41" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y41" s="6">
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="O41" s="3">
+      <c r="Z41" s="7">
         <v>0.79970030936830572</v>
       </c>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -8985,17 +9461,29 @@
         <v>39</v>
       </c>
       <c r="J42" s="3">
+        <v>0.52662293933756588</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O42" s="3"/>
+      <c r="T42" s="6">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="U42" s="7">
         <v>0.80684801694652231</v>
       </c>
-      <c r="N42" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y42" s="6">
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
-      <c r="O42" s="3">
+      <c r="Z42" s="7">
         <v>0.79815917870493136</v>
       </c>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -9011,17 +9499,29 @@
         <v>40</v>
       </c>
       <c r="J43" s="3">
+        <v>0.48051298933310949</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O43" s="3"/>
+      <c r="T43" s="6">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="U43" s="7">
         <v>0.77865927003954072</v>
       </c>
-      <c r="N43" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y43" s="6">
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="O43" s="3">
+      <c r="Z43" s="7">
         <v>0.79069923511435336</v>
       </c>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -9037,17 +9537,29 @@
         <v>41</v>
       </c>
       <c r="J44" s="3">
+        <v>0.51030224504723209</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O44" s="3"/>
+      <c r="T44" s="6">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="U44" s="7">
         <v>0.78440058195670237</v>
       </c>
-      <c r="N44" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y44" s="6">
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
-      <c r="O44" s="3">
+      <c r="Z44" s="7">
         <v>0.77816507524361822</v>
       </c>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9063,17 +9575,29 @@
         <v>42</v>
       </c>
       <c r="J45" s="3">
+        <v>0.51141837486401598</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O45" s="3"/>
+      <c r="T45" s="6">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="U45" s="7">
         <v>0.77517757569569157</v>
       </c>
-      <c r="N45" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y45" s="6">
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="O45" s="3">
+      <c r="Z45" s="7">
         <v>0.79559676665695334</v>
       </c>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -9089,17 +9613,29 @@
         <v>43</v>
       </c>
       <c r="J46" s="3">
+        <v>0.55159258801297328</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O46" s="3"/>
+      <c r="T46" s="6">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="U46" s="7">
         <v>0.73172178530723397</v>
       </c>
-      <c r="N46" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y46" s="6">
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="O46" s="3">
+      <c r="Z46" s="7">
         <v>0.81422631040683591</v>
       </c>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9115,17 +9651,29 @@
         <v>44</v>
       </c>
       <c r="J47" s="3">
+        <v>0.5393707805453487</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O47" s="3"/>
+      <c r="T47" s="6">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="U47" s="7">
         <v>0.78739711178736771</v>
       </c>
-      <c r="N47" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y47" s="6">
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="O47" s="3">
+      <c r="Z47" s="7">
         <v>0.83624260301461217</v>
       </c>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9141,17 +9689,29 @@
         <v>45</v>
       </c>
       <c r="J48" s="3">
+        <v>0.56574652514672397</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O48" s="3"/>
+      <c r="T48" s="6">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="U48" s="7">
         <v>0.76981245439444945</v>
       </c>
-      <c r="N48" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y48" s="6">
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="O48" s="3">
+      <c r="Z48" s="7">
         <v>0.77948556828586979</v>
       </c>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9167,17 +9727,29 @@
         <v>46</v>
       </c>
       <c r="J49" s="3">
+        <v>0.52092364561702587</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O49" s="3"/>
+      <c r="T49" s="6">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="U49" s="7">
         <v>0.74310584214061914</v>
       </c>
-      <c r="N49" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y49" s="6">
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="O49" s="3">
+      <c r="Z49" s="7">
         <v>0.77052783287717719</v>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9193,17 +9765,29 @@
         <v>47</v>
       </c>
       <c r="J50" s="3">
+        <v>0.57418724922542808</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O50" s="3"/>
+      <c r="T50" s="6">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="U50" s="7">
         <v>0.80322037948211167</v>
       </c>
-      <c r="N50" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y50" s="6">
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
-      <c r="O50" s="3">
+      <c r="Z50" s="7">
         <v>0.79610203589235684</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9219,17 +9803,29 @@
         <v>48</v>
       </c>
       <c r="J51" s="3">
+        <v>0.57927078295773371</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O51" s="3"/>
+      <c r="T51" s="6">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="U51" s="7">
         <v>0.78192280972213579</v>
       </c>
-      <c r="N51" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y51" s="6">
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="O51" s="3">
+      <c r="Z51" s="7">
         <v>0.75303614690770015</v>
       </c>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9245,17 +9841,29 @@
         <v>49</v>
       </c>
       <c r="J52" s="3">
+        <v>0.50372095038462072</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O52" s="3"/>
+      <c r="T52" s="6">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="U52" s="7">
         <v>0.74027177131612953</v>
       </c>
-      <c r="N52" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y52" s="6">
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="O52" s="3">
+      <c r="Z52" s="7">
         <v>0.8259339337042062</v>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9271,17 +9879,35 @@
         <v>50</v>
       </c>
       <c r="J53" s="3">
+        <v>0.5085555590799542</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O53" s="3"/>
+      <c r="T53" s="6">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="U53" s="7">
         <v>0.77066450762997896</v>
       </c>
-      <c r="N53" s="2">
-        <f t="shared" si="2"/>
+      <c r="Y53" s="6">
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="O53" s="3">
+      <c r="Z53" s="7">
         <v>0.78973831256011973</v>
       </c>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+    </row>
+    <row r="55" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C55" s="2" t="s">
         <v>3</v>
       </c>
@@ -9298,17 +9924,31 @@
       </c>
       <c r="J55" s="3">
         <f>AVERAGE(J4:J53)</f>
-        <v>0.77970641288442966</v>
+        <v>0.53162675857095731</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O55" s="3">
+      <c r="O55" s="3" t="e">
         <f>AVERAGE(O4:O53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U55" s="7">
+        <f>AVERAGE(U4:U53)</f>
+        <v>0.77970641288442966</v>
+      </c>
+      <c r="Y55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z55" s="7">
+        <f>AVERAGE(Z4:Z53)</f>
         <v>0.79398732852027254</v>
       </c>
     </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>4</v>
       </c>
@@ -9325,13 +9965,27 @@
       </c>
       <c r="J56" s="3">
         <f>_xlfn.STDEV.S(J4:J53)</f>
-        <v>2.4509800244337382E-2</v>
+        <v>3.6293783587861575E-2</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O56" s="3">
+      <c r="O56" s="3" t="e">
         <f>_xlfn.STDEV.S(O4:O53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U56" s="7">
+        <f>_xlfn.STDEV.S(U4:U53)</f>
+        <v>2.4509800244337382E-2</v>
+      </c>
+      <c r="Y56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z56" s="7">
+        <f>_xlfn.STDEV.S(Z4:Z53)</f>
         <v>2.0712879669264692E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test-23: hybrid3 model 2.0 (r2, 3Ysum)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="18">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24-f 3Ysum.csv)</t>
-  </si>
-  <si>
-    <t>Hybrid3 model (superdataset-24-f + 2Y + 3Y.csv)</t>
   </si>
   <si>
     <t>Hybrid3-model (superdataset-24-f + 2Y + 3Y.csv)</t>
@@ -140,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -155,6 +152,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -455,14 +460,14 @@
       </c>
       <c r="J3" s="5"/>
       <c r="N3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="T3" s="5"/>
       <c r="X3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="3:25" x14ac:dyDescent="0.25">
@@ -2599,10 +2604,10 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>6</v>
@@ -5120,11 +5125,11 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>6</v>
@@ -7956,7 +7961,7 @@
   <dimension ref="C2:Z56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7967,19 +7972,20 @@
       </c>
       <c r="E2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" s="5"/>
-      <c r="Y2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z2" s="5"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
@@ -7997,14 +8003,16 @@
       <c r="O3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6" t="s">
+      <c r="S3" s="2"/>
+      <c r="T3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="U3" s="10"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C4" s="2">
@@ -8019,25 +8027,25 @@
       <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="3">
-        <v>0.57834400411422515</v>
-      </c>
+      <c r="J4" s="3"/>
       <c r="N4" s="2">
         <v>1</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="T4" s="6">
+      <c r="O4" s="3">
+        <v>0.57834400411422515</v>
+      </c>
+      <c r="S4" s="2">
         <v>1</v>
       </c>
-      <c r="U4" s="7">
-        <v>0.74759938062002673</v>
-      </c>
-      <c r="Y4" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="7">
-        <v>0.78489980504236645</v>
-      </c>
+      <c r="T4" s="3">
+        <v>0.56982036045848528</v>
+      </c>
+      <c r="U4" s="11"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="11"/>
     </row>
     <row r="5" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
@@ -8054,28 +8062,27 @@
         <f>I4+1</f>
         <v>2</v>
       </c>
-      <c r="J5" s="3">
-        <v>0.5172853331948799</v>
-      </c>
+      <c r="J5" s="3"/>
       <c r="N5" s="2">
         <f>N4+1</f>
         <v>2</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="T5" s="6">
-        <f>T4+1</f>
+      <c r="O5" s="3">
+        <v>0.5172853331948799</v>
+      </c>
+      <c r="S5" s="2">
+        <f>S4+1</f>
         <v>2</v>
       </c>
-      <c r="U5" s="7">
-        <v>0.75272216793297142</v>
-      </c>
-      <c r="Y5" s="6">
-        <f>Y4+1</f>
-        <v>2</v>
-      </c>
-      <c r="Z5" s="7">
-        <v>0.76889713805937721</v>
-      </c>
+      <c r="T5" s="3">
+        <v>0.50672529465505234</v>
+      </c>
+      <c r="U5" s="11"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="11"/>
     </row>
     <row r="6" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
@@ -8092,28 +8099,27 @@
         <f t="shared" ref="I6:I53" si="1">I5+1</f>
         <v>3</v>
       </c>
-      <c r="J6" s="3">
-        <v>0.56135559361634901</v>
-      </c>
+      <c r="J6" s="3"/>
       <c r="N6" s="2">
         <f t="shared" ref="N6:N53" si="2">N5+1</f>
         <v>3</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="T6" s="6">
-        <f t="shared" ref="T6:T53" si="3">T5+1</f>
+      <c r="O6" s="3">
+        <v>0.56135559361634901</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" ref="S6:S53" si="3">S5+1</f>
         <v>3</v>
       </c>
-      <c r="U6" s="7">
-        <v>0.81290062745285052</v>
-      </c>
-      <c r="Y6" s="6">
-        <f t="shared" ref="Y6:Y53" si="4">Y5+1</f>
-        <v>3</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>0.80729775526569381</v>
-      </c>
+      <c r="T6" s="3">
+        <v>0.57613077610316288</v>
+      </c>
+      <c r="U6" s="11"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="11"/>
     </row>
     <row r="7" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -8130,28 +8136,27 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="3"/>
+      <c r="N7" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O7" s="3">
         <v>0.56287075662473007</v>
       </c>
-      <c r="N7" s="2">
-        <f t="shared" si="2"/>
+      <c r="S7" s="2">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="O7" s="3"/>
-      <c r="T7" s="6">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="U7" s="7">
-        <v>0.76359659281275505</v>
-      </c>
-      <c r="Y7" s="6">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="Z7" s="7">
-        <v>0.77998675978926502</v>
-      </c>
+      <c r="T7" s="3">
+        <v>0.56417736410670272</v>
+      </c>
+      <c r="U7" s="11"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="11"/>
     </row>
     <row r="8" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -8168,28 +8173,27 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="3"/>
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O8" s="3">
         <v>0.5081679829283714</v>
       </c>
-      <c r="N8" s="2">
-        <f t="shared" si="2"/>
+      <c r="S8" s="2">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="O8" s="3"/>
-      <c r="T8" s="6">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="U8" s="7">
-        <v>0.7545887963884832</v>
-      </c>
-      <c r="Y8" s="6">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="Z8" s="7">
-        <v>0.74093244213597886</v>
-      </c>
+      <c r="T8" s="3">
+        <v>0.5609967970187284</v>
+      </c>
+      <c r="U8" s="11"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="11"/>
     </row>
     <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -8206,28 +8210,27 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="3"/>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O9" s="3">
         <v>0.56977280792018892</v>
       </c>
-      <c r="N9" s="2">
-        <f t="shared" si="2"/>
+      <c r="S9" s="2">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="O9" s="3"/>
-      <c r="T9" s="6">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="U9" s="7">
-        <v>0.80385166737402391</v>
-      </c>
-      <c r="Y9" s="6">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="Z9" s="7">
-        <v>0.78829967713958138</v>
-      </c>
+      <c r="T9" s="3">
+        <v>0.4974589838323783</v>
+      </c>
+      <c r="U9" s="11"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="11"/>
     </row>
     <row r="10" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -8244,28 +8247,27 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="3"/>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O10" s="3">
         <v>0.52003827473417497</v>
       </c>
-      <c r="N10" s="2">
-        <f t="shared" si="2"/>
+      <c r="S10" s="2">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="O10" s="3"/>
-      <c r="T10" s="6">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="U10" s="7">
-        <v>0.81537059224632424</v>
-      </c>
-      <c r="Y10" s="6">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="Z10" s="7">
-        <v>0.73867871133666696</v>
-      </c>
+      <c r="T10" s="3">
+        <v>0.57176536329417393</v>
+      </c>
+      <c r="U10" s="11"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="11"/>
     </row>
     <row r="11" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -8282,28 +8284,27 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="3"/>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O11" s="3">
         <v>0.46539564064000999</v>
       </c>
-      <c r="N11" s="2">
-        <f t="shared" si="2"/>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="O11" s="3"/>
-      <c r="T11" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="U11" s="7">
-        <v>0.80425470934478516</v>
-      </c>
-      <c r="Y11" s="6">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="Z11" s="7">
-        <v>0.79989025541292258</v>
-      </c>
+      <c r="T11" s="3">
+        <v>0.57274363036149345</v>
+      </c>
+      <c r="U11" s="11"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="11"/>
     </row>
     <row r="12" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -8320,28 +8321,27 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="3"/>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O12" s="3">
         <v>0.52738054435967174</v>
       </c>
-      <c r="N12" s="2">
-        <f t="shared" si="2"/>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="O12" s="3"/>
-      <c r="T12" s="6">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="U12" s="7">
-        <v>0.7576941490745841</v>
-      </c>
-      <c r="Y12" s="6">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="Z12" s="7">
-        <v>0.80930455026279047</v>
-      </c>
+      <c r="T12" s="3">
+        <v>0.53158117665112259</v>
+      </c>
+      <c r="U12" s="11"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="11"/>
     </row>
     <row r="13" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -8358,28 +8358,27 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="3"/>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O13" s="3">
         <v>0.4888645545312692</v>
       </c>
-      <c r="N13" s="2">
-        <f t="shared" si="2"/>
+      <c r="S13" s="2">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="T13" s="6">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="U13" s="7">
-        <v>0.74667295040812309</v>
-      </c>
-      <c r="Y13" s="6">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="Z13" s="7">
-        <v>0.77140772157724169</v>
-      </c>
+      <c r="T13" s="3">
+        <v>0.58626620830813436</v>
+      </c>
+      <c r="U13" s="11"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="11"/>
     </row>
     <row r="14" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -8396,28 +8395,27 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="3"/>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O14" s="3">
         <v>0.51058084555486583</v>
       </c>
-      <c r="N14" s="2">
-        <f t="shared" si="2"/>
+      <c r="S14" s="2">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="O14" s="3"/>
-      <c r="T14" s="6">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="U14" s="7">
-        <v>0.78479006333818369</v>
-      </c>
-      <c r="Y14" s="6">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="Z14" s="7">
-        <v>0.80790040470964197</v>
-      </c>
+      <c r="T14" s="3">
+        <v>0.54553290276473554</v>
+      </c>
+      <c r="U14" s="11"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -8434,28 +8432,27 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="3"/>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O15" s="3">
         <v>0.563488646066719</v>
       </c>
-      <c r="N15" s="2">
-        <f t="shared" si="2"/>
+      <c r="S15" s="2">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="O15" s="3"/>
-      <c r="T15" s="6">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="U15" s="7">
-        <v>0.77498508287134604</v>
-      </c>
-      <c r="Y15" s="6">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="Z15" s="7">
-        <v>0.75474996548915196</v>
-      </c>
+      <c r="T15" s="3">
+        <v>0.56447468185661365</v>
+      </c>
+      <c r="U15" s="11"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="11"/>
     </row>
     <row r="16" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -8472,28 +8469,27 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="3"/>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O16" s="3">
         <v>0.51147828263257689</v>
       </c>
-      <c r="N16" s="2">
-        <f t="shared" si="2"/>
+      <c r="S16" s="2">
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="O16" s="3"/>
-      <c r="T16" s="6">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="U16" s="7">
-        <v>0.76680506361277445</v>
-      </c>
-      <c r="Y16" s="6">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="Z16" s="7">
-        <v>0.81167527136343665</v>
-      </c>
+      <c r="T16" s="3">
+        <v>0.59907866538529264</v>
+      </c>
+      <c r="U16" s="11"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -8510,28 +8506,27 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="3"/>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O17" s="3">
         <v>0.4834937046000386</v>
       </c>
-      <c r="N17" s="2">
-        <f t="shared" si="2"/>
+      <c r="S17" s="2">
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="O17" s="3"/>
-      <c r="T17" s="6">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="U17" s="7">
-        <v>0.79547860900348266</v>
-      </c>
-      <c r="Y17" s="6">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="Z17" s="7">
-        <v>0.80066366481058293</v>
-      </c>
+      <c r="T17" s="3">
+        <v>0.5660901383223842</v>
+      </c>
+      <c r="U17" s="11"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -8548,28 +8543,27 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="3"/>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O18" s="3">
         <v>0.54381787801258175</v>
       </c>
-      <c r="N18" s="2">
-        <f t="shared" si="2"/>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="O18" s="3"/>
-      <c r="T18" s="6">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="U18" s="7">
-        <v>0.80253923797160254</v>
-      </c>
-      <c r="Y18" s="6">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="Z18" s="7">
-        <v>0.79379990111229703</v>
-      </c>
+      <c r="T18" s="3">
+        <v>0.52580056159352639</v>
+      </c>
+      <c r="U18" s="11"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -8586,28 +8580,27 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="3"/>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O19" s="3">
         <v>0.5761527509110238</v>
       </c>
-      <c r="N19" s="2">
-        <f t="shared" si="2"/>
+      <c r="S19" s="2">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="O19" s="3"/>
-      <c r="T19" s="6">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="U19" s="7">
-        <v>0.75811037408550375</v>
-      </c>
-      <c r="Y19" s="6">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="Z19" s="7">
-        <v>0.79330358700648618</v>
-      </c>
+      <c r="T19" s="3">
+        <v>0.55290522283377541</v>
+      </c>
+      <c r="U19" s="11"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -8624,28 +8617,27 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="3"/>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O20" s="3">
         <v>0.6003089088774205</v>
       </c>
-      <c r="N20" s="2">
-        <f t="shared" si="2"/>
+      <c r="S20" s="2">
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="O20" s="3"/>
-      <c r="T20" s="6">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="U20" s="7">
-        <v>0.80959496508752071</v>
-      </c>
-      <c r="Y20" s="6">
-        <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="Z20" s="7">
-        <v>0.80364508616800112</v>
-      </c>
+      <c r="T20" s="3">
+        <v>0.58492600289221919</v>
+      </c>
+      <c r="U20" s="11"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -8662,28 +8654,27 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="3"/>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O21" s="3">
         <v>0.53130747434539705</v>
       </c>
-      <c r="N21" s="2">
-        <f t="shared" si="2"/>
+      <c r="S21" s="2">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="O21" s="3"/>
-      <c r="T21" s="6">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="U21" s="7">
-        <v>0.78243223145681651</v>
-      </c>
-      <c r="Y21" s="6">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="Z21" s="7">
-        <v>0.8358005987200301</v>
-      </c>
+      <c r="T21" s="3">
+        <v>0.55334096307414349</v>
+      </c>
+      <c r="U21" s="11"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -8700,28 +8691,27 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="3"/>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O22" s="3">
         <v>0.43865025485995213</v>
       </c>
-      <c r="N22" s="2">
-        <f t="shared" si="2"/>
+      <c r="S22" s="2">
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="O22" s="3"/>
-      <c r="T22" s="6">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="U22" s="7">
-        <v>0.79065531295771696</v>
-      </c>
-      <c r="Y22" s="6">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="Z22" s="7">
-        <v>0.79355445633115396</v>
-      </c>
+      <c r="T22" s="3">
+        <v>0.50476516824012774</v>
+      </c>
+      <c r="U22" s="11"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="11"/>
     </row>
     <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -8738,28 +8728,27 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="3"/>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O23" s="3">
         <v>0.58465011076149842</v>
       </c>
-      <c r="N23" s="2">
-        <f t="shared" si="2"/>
+      <c r="S23" s="2">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="O23" s="3"/>
-      <c r="T23" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="U23" s="7">
-        <v>0.75111177334431645</v>
-      </c>
-      <c r="Y23" s="6">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>0.78853351229375457</v>
-      </c>
+      <c r="T23" s="3">
+        <v>0.58140892034460334</v>
+      </c>
+      <c r="U23" s="11"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="11"/>
     </row>
     <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -8776,28 +8765,27 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="3"/>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O24" s="3">
         <v>0.57326671389181705</v>
       </c>
-      <c r="N24" s="2">
-        <f t="shared" si="2"/>
+      <c r="S24" s="2">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="O24" s="3"/>
-      <c r="T24" s="6">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="U24" s="7">
-        <v>0.7933349338637159</v>
-      </c>
-      <c r="Y24" s="6">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="Z24" s="7">
-        <v>0.78748954623838974</v>
-      </c>
+      <c r="T24" s="3">
+        <v>0.57157475164805338</v>
+      </c>
+      <c r="U24" s="11"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -8814,28 +8802,27 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="3"/>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O25" s="3">
         <v>0.49476677066589658</v>
       </c>
-      <c r="N25" s="2">
-        <f t="shared" si="2"/>
+      <c r="S25" s="2">
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="O25" s="3"/>
-      <c r="T25" s="6">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="U25" s="7">
-        <v>0.7431987341233699</v>
-      </c>
-      <c r="Y25" s="6">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-      <c r="Z25" s="7">
-        <v>0.80992712180274473</v>
-      </c>
+      <c r="T25" s="3">
+        <v>0.64031148120726189</v>
+      </c>
+      <c r="U25" s="11"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="11"/>
     </row>
     <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -8852,28 +8839,27 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="3"/>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O26" s="3">
         <v>0.5002916618770199</v>
       </c>
-      <c r="N26" s="2">
-        <f t="shared" si="2"/>
+      <c r="S26" s="2">
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="O26" s="3"/>
-      <c r="T26" s="6">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="U26" s="7">
-        <v>0.80481897041530459</v>
-      </c>
-      <c r="Y26" s="6">
-        <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-      <c r="Z26" s="7">
-        <v>0.77620233911398839</v>
-      </c>
+      <c r="T26" s="3">
+        <v>0.60395825977782502</v>
+      </c>
+      <c r="U26" s="11"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -8890,28 +8876,27 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="3"/>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O27" s="3">
         <v>0.49019982541415219</v>
       </c>
-      <c r="N27" s="2">
-        <f t="shared" si="2"/>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="O27" s="3"/>
-      <c r="T27" s="6">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="U27" s="7">
-        <v>0.77831347161363618</v>
-      </c>
-      <c r="Y27" s="6">
-        <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="Z27" s="7">
-        <v>0.80374149857995725</v>
-      </c>
+      <c r="T27" s="3">
+        <v>0.52894393121816186</v>
+      </c>
+      <c r="U27" s="11"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="11"/>
     </row>
     <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -8928,28 +8913,27 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="3"/>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O28" s="3">
         <v>0.51516579421759845</v>
       </c>
-      <c r="N28" s="2">
-        <f t="shared" si="2"/>
+      <c r="S28" s="2">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="O28" s="3"/>
-      <c r="T28" s="6">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="U28" s="7">
-        <v>0.73250447421016152</v>
-      </c>
-      <c r="Y28" s="6">
-        <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-      <c r="Z28" s="7">
-        <v>0.77311927125394853</v>
-      </c>
+      <c r="T28" s="3">
+        <v>0.57493541175350882</v>
+      </c>
+      <c r="U28" s="11"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
@@ -8966,28 +8950,27 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="3"/>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O29" s="3">
         <v>0.56374703719391916</v>
       </c>
-      <c r="N29" s="2">
-        <f t="shared" si="2"/>
+      <c r="S29" s="2">
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="O29" s="3"/>
-      <c r="T29" s="6">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="U29" s="7">
-        <v>0.79928969776231029</v>
-      </c>
-      <c r="Y29" s="6">
-        <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="Z29" s="7">
-        <v>0.79561855051336716</v>
-      </c>
+      <c r="T29" s="3">
+        <v>0.53675399722374384</v>
+      </c>
+      <c r="U29" s="11"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
@@ -9004,28 +8987,27 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="3"/>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O30" s="3">
         <v>0.52353799742386575</v>
       </c>
-      <c r="N30" s="2">
-        <f t="shared" si="2"/>
+      <c r="S30" s="2">
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="O30" s="3"/>
-      <c r="T30" s="6">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="U30" s="7">
-        <v>0.80145040301035131</v>
-      </c>
-      <c r="Y30" s="6">
-        <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
-      <c r="Z30" s="7">
-        <v>0.81308835275443048</v>
-      </c>
+      <c r="T30" s="3">
+        <v>0.58526121238325601</v>
+      </c>
+      <c r="U30" s="11"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
@@ -9042,28 +9024,27 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="3"/>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O31" s="3">
         <v>0.53240531571446525</v>
       </c>
-      <c r="N31" s="2">
-        <f t="shared" si="2"/>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="O31" s="3"/>
-      <c r="T31" s="6">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="U31" s="7">
-        <v>0.79203197789581958</v>
-      </c>
-      <c r="Y31" s="6">
-        <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="Z31" s="7">
-        <v>0.8111886017465374</v>
-      </c>
+      <c r="T31" s="3">
+        <v>0.50966394296965734</v>
+      </c>
+      <c r="U31" s="11"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="11"/>
     </row>
     <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
@@ -9080,28 +9061,27 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="3"/>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O32" s="3">
         <v>0.50613099678628659</v>
       </c>
-      <c r="N32" s="2">
-        <f t="shared" si="2"/>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="O32" s="3"/>
-      <c r="T32" s="6">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="U32" s="7">
-        <v>0.74549347792987275</v>
-      </c>
-      <c r="Y32" s="6">
-        <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-      <c r="Z32" s="7">
-        <v>0.79891958026776666</v>
-      </c>
+      <c r="T32" s="3">
+        <v>0.58559850960000603</v>
+      </c>
+      <c r="U32" s="11"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="11"/>
     </row>
     <row r="33" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
@@ -9118,28 +9098,27 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="3"/>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O33" s="3">
         <v>0.52438639008761223</v>
       </c>
-      <c r="N33" s="2">
-        <f t="shared" si="2"/>
+      <c r="S33" s="2">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="O33" s="3"/>
-      <c r="T33" s="6">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="U33" s="7">
-        <v>0.78356932624316888</v>
-      </c>
-      <c r="Y33" s="6">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="Z33" s="7">
-        <v>0.79637222780511763</v>
-      </c>
+      <c r="T33" s="3">
+        <v>0.56992766988844989</v>
+      </c>
+      <c r="U33" s="11"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="10"/>
+      <c r="Z33" s="11"/>
     </row>
     <row r="34" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
@@ -9156,28 +9135,27 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="3"/>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O34" s="3">
         <v>0.6169610482762905</v>
       </c>
-      <c r="N34" s="2">
-        <f t="shared" si="2"/>
+      <c r="S34" s="2">
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="O34" s="3"/>
-      <c r="T34" s="6">
-        <f t="shared" si="3"/>
-        <v>31</v>
-      </c>
-      <c r="U34" s="7">
-        <v>0.78165766235738088</v>
-      </c>
-      <c r="Y34" s="6">
-        <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="Z34" s="7">
-        <v>0.80490616625728184</v>
-      </c>
+      <c r="T34" s="3">
+        <v>0.53102074444680358</v>
+      </c>
+      <c r="U34" s="11"/>
+      <c r="V34" s="9"/>
+      <c r="W34" s="9"/>
+      <c r="X34" s="9"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="11"/>
     </row>
     <row r="35" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
@@ -9194,28 +9172,27 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="3"/>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O35" s="3">
         <v>0.50156675152561681</v>
       </c>
-      <c r="N35" s="2">
-        <f t="shared" si="2"/>
+      <c r="S35" s="2">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="O35" s="3"/>
-      <c r="T35" s="6">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="U35" s="7">
-        <v>0.8129048890288546</v>
-      </c>
-      <c r="Y35" s="6">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="Z35" s="7">
-        <v>0.79844802895196509</v>
-      </c>
+      <c r="T35" s="3">
+        <v>0.59787609125575847</v>
+      </c>
+      <c r="U35" s="11"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="11"/>
     </row>
     <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
@@ -9232,28 +9209,27 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="3"/>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O36" s="3">
         <v>0.52652791568615509</v>
       </c>
-      <c r="N36" s="2">
-        <f t="shared" si="2"/>
+      <c r="S36" s="2">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="O36" s="3"/>
-      <c r="T36" s="6">
-        <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="U36" s="7">
-        <v>0.80361307339161958</v>
-      </c>
-      <c r="Y36" s="6">
-        <f t="shared" si="4"/>
-        <v>33</v>
-      </c>
-      <c r="Z36" s="7">
-        <v>0.81164488617488939</v>
-      </c>
+      <c r="T36" s="3">
+        <v>0.49469226030304669</v>
+      </c>
+      <c r="U36" s="11"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="11"/>
     </row>
     <row r="37" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
@@ -9270,28 +9246,27 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="3"/>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O37" s="3">
         <v>0.53958384752298505</v>
       </c>
-      <c r="N37" s="2">
-        <f t="shared" si="2"/>
+      <c r="S37" s="2">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="O37" s="3"/>
-      <c r="T37" s="6">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="U37" s="7">
-        <v>0.77850151482103791</v>
-      </c>
-      <c r="Y37" s="6">
-        <f t="shared" si="4"/>
-        <v>34</v>
-      </c>
-      <c r="Z37" s="7">
-        <v>0.78931160602477124</v>
-      </c>
+      <c r="T37" s="3">
+        <v>0.54600643156294215</v>
+      </c>
+      <c r="U37" s="11"/>
+      <c r="V37" s="9"/>
+      <c r="W37" s="9"/>
+      <c r="X37" s="9"/>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="11"/>
     </row>
     <row r="38" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
@@ -9308,28 +9283,27 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="3"/>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O38" s="3">
         <v>0.57057254664261059</v>
       </c>
-      <c r="N38" s="2">
-        <f t="shared" si="2"/>
+      <c r="S38" s="2">
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="O38" s="3"/>
-      <c r="T38" s="6">
-        <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="U38" s="7">
-        <v>0.76357957335404536</v>
-      </c>
-      <c r="Y38" s="6">
-        <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="Z38" s="7">
-        <v>0.81606363231006518</v>
-      </c>
+      <c r="T38" s="3">
+        <v>0.57058183441394195</v>
+      </c>
+      <c r="U38" s="11"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="9"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="11"/>
     </row>
     <row r="39" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
@@ -9346,28 +9320,27 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="3"/>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O39" s="3">
         <v>0.50221572484548593</v>
       </c>
-      <c r="N39" s="2">
-        <f t="shared" si="2"/>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="O39" s="3"/>
-      <c r="T39" s="6">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="U39" s="7">
-        <v>0.82719591105098256</v>
-      </c>
-      <c r="Y39" s="6">
-        <f t="shared" si="4"/>
-        <v>36</v>
-      </c>
-      <c r="Z39" s="7">
-        <v>0.81628912563866352</v>
-      </c>
+      <c r="T39" s="3">
+        <v>0.56816604709976348</v>
+      </c>
+      <c r="U39" s="11"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="9"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="11"/>
     </row>
     <row r="40" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
@@ -9384,28 +9357,27 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="3"/>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O40" s="3">
         <v>0.54793609137779353</v>
       </c>
-      <c r="N40" s="2">
-        <f t="shared" si="2"/>
+      <c r="S40" s="2">
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="O40" s="3"/>
-      <c r="T40" s="6">
-        <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="U40" s="7">
-        <v>0.78768718630391255</v>
-      </c>
-      <c r="Y40" s="6">
-        <f t="shared" si="4"/>
-        <v>37</v>
-      </c>
-      <c r="Z40" s="7">
-        <v>0.79620131781626413</v>
-      </c>
+      <c r="T40" s="3">
+        <v>0.5089159538869853</v>
+      </c>
+      <c r="U40" s="11"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="9"/>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="11"/>
     </row>
     <row r="41" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
@@ -9422,28 +9394,27 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="3"/>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O41" s="3">
         <v>0.53644652056062414</v>
       </c>
-      <c r="N41" s="2">
-        <f t="shared" si="2"/>
+      <c r="S41" s="2">
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="O41" s="3"/>
-      <c r="T41" s="6">
-        <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="U41" s="7">
-        <v>0.80721891304325188</v>
-      </c>
-      <c r="Y41" s="6">
-        <f t="shared" si="4"/>
-        <v>38</v>
-      </c>
-      <c r="Z41" s="7">
-        <v>0.79970030936830572</v>
-      </c>
+      <c r="T41" s="3">
+        <v>0.55046632263679962</v>
+      </c>
+      <c r="U41" s="11"/>
+      <c r="V41" s="9"/>
+      <c r="W41" s="9"/>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="11"/>
     </row>
     <row r="42" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
@@ -9460,28 +9431,27 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="3"/>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O42" s="3">
         <v>0.52662293933756588</v>
       </c>
-      <c r="N42" s="2">
-        <f t="shared" si="2"/>
+      <c r="S42" s="2">
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="O42" s="3"/>
-      <c r="T42" s="6">
-        <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="U42" s="7">
-        <v>0.80684801694652231</v>
-      </c>
-      <c r="Y42" s="6">
-        <f t="shared" si="4"/>
-        <v>39</v>
-      </c>
-      <c r="Z42" s="7">
-        <v>0.79815917870493136</v>
-      </c>
+      <c r="T42" s="3">
+        <v>0.55520579759763766</v>
+      </c>
+      <c r="U42" s="11"/>
+      <c r="V42" s="9"/>
+      <c r="W42" s="9"/>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
@@ -9498,28 +9468,27 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="3"/>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O43" s="3">
         <v>0.48051298933310949</v>
       </c>
-      <c r="N43" s="2">
-        <f t="shared" si="2"/>
+      <c r="S43" s="2">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="O43" s="3"/>
-      <c r="T43" s="6">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="U43" s="7">
-        <v>0.77865927003954072</v>
-      </c>
-      <c r="Y43" s="6">
-        <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="Z43" s="7">
-        <v>0.79069923511435336</v>
-      </c>
+      <c r="T43" s="3">
+        <v>0.59396857214269372</v>
+      </c>
+      <c r="U43" s="11"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="11"/>
     </row>
     <row r="44" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
@@ -9536,28 +9505,27 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="3"/>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O44" s="3">
         <v>0.51030224504723209</v>
       </c>
-      <c r="N44" s="2">
-        <f t="shared" si="2"/>
+      <c r="S44" s="2">
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="O44" s="3"/>
-      <c r="T44" s="6">
-        <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="U44" s="7">
-        <v>0.78440058195670237</v>
-      </c>
-      <c r="Y44" s="6">
-        <f t="shared" si="4"/>
-        <v>41</v>
-      </c>
-      <c r="Z44" s="7">
-        <v>0.77816507524361822</v>
-      </c>
+      <c r="T44" s="3">
+        <v>0.54471931008658081</v>
+      </c>
+      <c r="U44" s="11"/>
+      <c r="V44" s="9"/>
+      <c r="W44" s="9"/>
+      <c r="X44" s="9"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="11"/>
     </row>
     <row r="45" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
@@ -9574,28 +9542,27 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="3"/>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O45" s="3">
         <v>0.51141837486401598</v>
       </c>
-      <c r="N45" s="2">
-        <f t="shared" si="2"/>
+      <c r="S45" s="2">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="O45" s="3"/>
-      <c r="T45" s="6">
-        <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="U45" s="7">
-        <v>0.77517757569569157</v>
-      </c>
-      <c r="Y45" s="6">
-        <f t="shared" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="Z45" s="7">
-        <v>0.79559676665695334</v>
-      </c>
+      <c r="T45" s="3">
+        <v>0.56271996981350592</v>
+      </c>
+      <c r="U45" s="11"/>
+      <c r="V45" s="9"/>
+      <c r="W45" s="9"/>
+      <c r="X45" s="9"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="11"/>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
@@ -9612,28 +9579,27 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="3"/>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O46" s="3">
         <v>0.55159258801297328</v>
       </c>
-      <c r="N46" s="2">
-        <f t="shared" si="2"/>
+      <c r="S46" s="2">
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="O46" s="3"/>
-      <c r="T46" s="6">
-        <f t="shared" si="3"/>
-        <v>43</v>
-      </c>
-      <c r="U46" s="7">
-        <v>0.73172178530723397</v>
-      </c>
-      <c r="Y46" s="6">
-        <f t="shared" si="4"/>
-        <v>43</v>
-      </c>
-      <c r="Z46" s="7">
-        <v>0.81422631040683591</v>
-      </c>
+      <c r="T46" s="3">
+        <v>0.56950738432921266</v>
+      </c>
+      <c r="U46" s="11"/>
+      <c r="V46" s="9"/>
+      <c r="W46" s="9"/>
+      <c r="X46" s="9"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="11"/>
     </row>
     <row r="47" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
@@ -9650,28 +9616,27 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="3"/>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O47" s="3">
         <v>0.5393707805453487</v>
       </c>
-      <c r="N47" s="2">
-        <f t="shared" si="2"/>
+      <c r="S47" s="2">
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="O47" s="3"/>
-      <c r="T47" s="6">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-      <c r="U47" s="7">
-        <v>0.78739711178736771</v>
-      </c>
-      <c r="Y47" s="6">
-        <f t="shared" si="4"/>
-        <v>44</v>
-      </c>
-      <c r="Z47" s="7">
-        <v>0.83624260301461217</v>
-      </c>
+      <c r="T47" s="3">
+        <v>0.53078208538106009</v>
+      </c>
+      <c r="U47" s="11"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="10"/>
+      <c r="Z47" s="11"/>
     </row>
     <row r="48" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
@@ -9688,28 +9653,27 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="3"/>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O48" s="3">
         <v>0.56574652514672397</v>
       </c>
-      <c r="N48" s="2">
-        <f t="shared" si="2"/>
+      <c r="S48" s="2">
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="O48" s="3"/>
-      <c r="T48" s="6">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="U48" s="7">
-        <v>0.76981245439444945</v>
-      </c>
-      <c r="Y48" s="6">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="Z48" s="7">
-        <v>0.77948556828586979</v>
-      </c>
+      <c r="T48" s="3">
+        <v>0.49050562807660869</v>
+      </c>
+      <c r="U48" s="11"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="9"/>
+      <c r="X48" s="9"/>
+      <c r="Y48" s="10"/>
+      <c r="Z48" s="11"/>
     </row>
     <row r="49" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
@@ -9726,28 +9690,27 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="3"/>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O49" s="3">
         <v>0.52092364561702587</v>
       </c>
-      <c r="N49" s="2">
-        <f t="shared" si="2"/>
+      <c r="S49" s="2">
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="O49" s="3"/>
-      <c r="T49" s="6">
-        <f t="shared" si="3"/>
-        <v>46</v>
-      </c>
-      <c r="U49" s="7">
-        <v>0.74310584214061914</v>
-      </c>
-      <c r="Y49" s="6">
-        <f t="shared" si="4"/>
-        <v>46</v>
-      </c>
-      <c r="Z49" s="7">
-        <v>0.77052783287717719</v>
-      </c>
+      <c r="T49" s="3">
+        <v>0.52685550582785523</v>
+      </c>
+      <c r="U49" s="11"/>
+      <c r="V49" s="9"/>
+      <c r="W49" s="9"/>
+      <c r="X49" s="9"/>
+      <c r="Y49" s="10"/>
+      <c r="Z49" s="11"/>
     </row>
     <row r="50" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
@@ -9764,28 +9727,27 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="3"/>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O50" s="3">
         <v>0.57418724922542808</v>
       </c>
-      <c r="N50" s="2">
-        <f t="shared" si="2"/>
+      <c r="S50" s="2">
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="O50" s="3"/>
-      <c r="T50" s="6">
-        <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-      <c r="U50" s="7">
-        <v>0.80322037948211167</v>
-      </c>
-      <c r="Y50" s="6">
-        <f t="shared" si="4"/>
-        <v>47</v>
-      </c>
-      <c r="Z50" s="7">
-        <v>0.79610203589235684</v>
-      </c>
+      <c r="T50" s="3">
+        <v>0.53255706766003796</v>
+      </c>
+      <c r="U50" s="11"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="9"/>
+      <c r="Y50" s="10"/>
+      <c r="Z50" s="11"/>
     </row>
     <row r="51" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
@@ -9802,28 +9764,27 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="3"/>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O51" s="3">
         <v>0.57927078295773371</v>
       </c>
-      <c r="N51" s="2">
-        <f t="shared" si="2"/>
+      <c r="S51" s="2">
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="O51" s="3"/>
-      <c r="T51" s="6">
-        <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="U51" s="7">
-        <v>0.78192280972213579</v>
-      </c>
-      <c r="Y51" s="6">
-        <f t="shared" si="4"/>
-        <v>48</v>
-      </c>
-      <c r="Z51" s="7">
-        <v>0.75303614690770015</v>
-      </c>
+      <c r="T51" s="3">
+        <v>0.52633498673066492</v>
+      </c>
+      <c r="U51" s="11"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="11"/>
     </row>
     <row r="52" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
@@ -9840,28 +9801,27 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="3"/>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O52" s="3">
         <v>0.50372095038462072</v>
       </c>
-      <c r="N52" s="2">
-        <f t="shared" si="2"/>
+      <c r="S52" s="2">
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="O52" s="3"/>
-      <c r="T52" s="6">
-        <f t="shared" si="3"/>
-        <v>49</v>
-      </c>
-      <c r="U52" s="7">
-        <v>0.74027177131612953</v>
-      </c>
-      <c r="Y52" s="6">
-        <f t="shared" si="4"/>
-        <v>49</v>
-      </c>
-      <c r="Z52" s="7">
-        <v>0.8259339337042062</v>
-      </c>
+      <c r="T52" s="3">
+        <v>0.52640933564695813</v>
+      </c>
+      <c r="U52" s="11"/>
+      <c r="V52" s="9"/>
+      <c r="W52" s="9"/>
+      <c r="X52" s="9"/>
+      <c r="Y52" s="10"/>
+      <c r="Z52" s="11"/>
     </row>
     <row r="53" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
@@ -9878,34 +9838,35 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="3"/>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O53" s="3">
         <v>0.5085555590799542</v>
       </c>
-      <c r="N53" s="2">
-        <f t="shared" si="2"/>
+      <c r="S53" s="2">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="O53" s="3"/>
-      <c r="T53" s="6">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="U53" s="7">
-        <v>0.77066450762997896</v>
-      </c>
-      <c r="Y53" s="6">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="Z53" s="7">
-        <v>0.78973831256011973</v>
-      </c>
+      <c r="T53" s="3">
+        <v>0.53696223287772549</v>
+      </c>
+      <c r="U53" s="11"/>
+      <c r="V53" s="9"/>
+      <c r="W53" s="9"/>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="10"/>
+      <c r="Z53" s="11"/>
     </row>
     <row r="54" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
-      <c r="Y54" s="5"/>
-      <c r="Z54" s="5"/>
+      <c r="U54" s="9"/>
+      <c r="V54" s="9"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="9"/>
+      <c r="Y54" s="9"/>
+      <c r="Z54" s="9"/>
     </row>
     <row r="55" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C55" s="2" t="s">
@@ -9922,31 +9883,30 @@
       <c r="I55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="3" t="e">
         <f>AVERAGE(J4:J53)</f>
-        <v>0.53162675857095731</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O55" s="3" t="e">
+      <c r="O55" s="3">
         <f>AVERAGE(O4:O53)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T55" s="6" t="s">
+        <v>0.53162675857095731</v>
+      </c>
+      <c r="S55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U55" s="7">
-        <f>AVERAGE(U4:U53)</f>
-        <v>0.77970641288442966</v>
-      </c>
-      <c r="Y55" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z55" s="7">
-        <f>AVERAGE(Z4:Z53)</f>
-        <v>0.79398732852027254</v>
-      </c>
+      <c r="T55" s="3">
+        <f>AVERAGE(T4:T53)</f>
+        <v>0.55374343823086725</v>
+      </c>
+      <c r="U55" s="11"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="10"/>
+      <c r="Z55" s="11"/>
     </row>
     <row r="56" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
@@ -9963,31 +9923,30 @@
       <c r="I56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="3" t="e">
         <f>_xlfn.STDEV.S(J4:J53)</f>
-        <v>3.6293783587861575E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O56" s="3" t="e">
+      <c r="O56" s="3">
         <f>_xlfn.STDEV.S(O4:O53)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T56" s="6" t="s">
+        <v>3.6293783587861575E-2</v>
+      </c>
+      <c r="S56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U56" s="7">
-        <f>_xlfn.STDEV.S(U4:U53)</f>
-        <v>2.4509800244337382E-2</v>
-      </c>
-      <c r="Y56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z56" s="7">
-        <f>_xlfn.STDEV.S(Z4:Z53)</f>
-        <v>2.0712879669264692E-2</v>
-      </c>
+      <c r="T56" s="3">
+        <f>_xlfn.STDEV.S(T4:T53)</f>
+        <v>3.1871497997395706E-2</v>
+      </c>
+      <c r="U56" s="11"/>
+      <c r="V56" s="9"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="10"/>
+      <c r="Z56" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10017,7 +9976,7 @@
         <v>7</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="4:17" x14ac:dyDescent="0.25">
@@ -11415,7 +11374,7 @@
         <v>7</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test-23: extrapol 2.0 (3Ysum, saldoone)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="19">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Hybrid3 model 2.0 (superdataset-24-f + 2Y + 3Y.csv)</t>
+  </si>
+  <si>
+    <t>Hybrid3-model 2.0 (superdataset-24-f + 2Y + 3Y.csv)</t>
   </si>
 </sst>
 </file>
@@ -7960,8 +7963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7972,7 +7975,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>16</v>
@@ -8027,7 +8030,9 @@
       <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3">
+        <v>0.46922838434286068</v>
+      </c>
       <c r="N4" s="2">
         <v>1</v>
       </c>
@@ -8062,7 +8067,9 @@
         <f>I4+1</f>
         <v>2</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3">
+        <v>0.46547302339289531</v>
+      </c>
       <c r="N5" s="2">
         <f>N4+1</f>
         <v>2</v>
@@ -8099,7 +8106,9 @@
         <f t="shared" ref="I6:I53" si="1">I5+1</f>
         <v>3</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3">
+        <v>0.39681496612747152</v>
+      </c>
       <c r="N6" s="2">
         <f t="shared" ref="N6:N53" si="2">N5+1</f>
         <v>3</v>
@@ -8136,7 +8145,9 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3">
+        <v>0.46630476747712207</v>
+      </c>
       <c r="N7" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -8173,7 +8184,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="3">
+        <v>0.445433832453483</v>
+      </c>
       <c r="N8" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -8210,7 +8223,9 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3">
+        <v>0.50548073729787268</v>
+      </c>
       <c r="N9" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -8247,7 +8262,9 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3">
+        <v>0.51527859126739473</v>
+      </c>
       <c r="N10" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -8284,7 +8301,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3">
+        <v>0.42795815654032687</v>
+      </c>
       <c r="N11" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -8321,7 +8340,9 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J12" s="3"/>
+      <c r="J12" s="3">
+        <v>0.50463043601468949</v>
+      </c>
       <c r="N12" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -8358,7 +8379,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J13" s="3"/>
+      <c r="J13" s="3">
+        <v>0.5200133185813931</v>
+      </c>
       <c r="N13" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -8395,7 +8418,9 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3">
+        <v>0.45635712482509228</v>
+      </c>
       <c r="N14" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -8432,7 +8457,9 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3">
+        <v>0.5606375426828849</v>
+      </c>
       <c r="N15" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -8469,7 +8496,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J16" s="3"/>
+      <c r="J16" s="3">
+        <v>0.4824804782706924</v>
+      </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -8506,7 +8535,9 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J17" s="3"/>
+      <c r="J17" s="3">
+        <v>0.50087203932964219</v>
+      </c>
       <c r="N17" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -8543,7 +8574,9 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J18" s="3"/>
+      <c r="J18" s="3">
+        <v>0.45929025664114542</v>
+      </c>
       <c r="N18" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -8580,7 +8613,9 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J19" s="3"/>
+      <c r="J19" s="3">
+        <v>0.47769239898625759</v>
+      </c>
       <c r="N19" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -8617,7 +8652,9 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J20" s="3"/>
+      <c r="J20" s="3">
+        <v>0.50947979755300032</v>
+      </c>
       <c r="N20" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -8654,7 +8691,9 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3">
+        <v>0.42416611857804798</v>
+      </c>
       <c r="N21" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -8691,7 +8730,9 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J22" s="3"/>
+      <c r="J22" s="3">
+        <v>0.47292918934920208</v>
+      </c>
       <c r="N22" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -8728,7 +8769,9 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J23" s="3"/>
+      <c r="J23" s="3">
+        <v>0.4330003726981364</v>
+      </c>
       <c r="N23" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -8765,7 +8808,9 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J24" s="3"/>
+      <c r="J24" s="3">
+        <v>0.45597270505445348</v>
+      </c>
       <c r="N24" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -8802,7 +8847,9 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J25" s="3"/>
+      <c r="J25" s="3">
+        <v>0.40048583988913611</v>
+      </c>
       <c r="N25" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -8839,7 +8886,9 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J26" s="3"/>
+      <c r="J26" s="3">
+        <v>0.39050308440404141</v>
+      </c>
       <c r="N26" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -8876,7 +8925,9 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J27" s="3"/>
+      <c r="J27" s="3">
+        <v>0.40122356415123028</v>
+      </c>
       <c r="N27" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -8913,7 +8964,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J28" s="3"/>
+      <c r="J28" s="3">
+        <v>0.43661211271150557</v>
+      </c>
       <c r="N28" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -8950,7 +9003,9 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J29" s="3"/>
+      <c r="J29" s="3">
+        <v>0.45366025275651373</v>
+      </c>
       <c r="N29" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -8987,7 +9042,9 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J30" s="3"/>
+      <c r="J30" s="3">
+        <v>0.45816568966241072</v>
+      </c>
       <c r="N30" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -9024,7 +9081,9 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J31" s="3"/>
+      <c r="J31" s="3">
+        <v>0.48127724345056899</v>
+      </c>
       <c r="N31" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -9061,7 +9120,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J32" s="3"/>
+      <c r="J32" s="3">
+        <v>0.52749286428987108</v>
+      </c>
       <c r="N32" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -9098,7 +9159,9 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J33" s="3"/>
+      <c r="J33" s="3">
+        <v>0.39466566320808572</v>
+      </c>
       <c r="N33" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -9135,7 +9198,9 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J34" s="3"/>
+      <c r="J34" s="3">
+        <v>0.47800670347500729</v>
+      </c>
       <c r="N34" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -9172,7 +9237,9 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J35" s="3"/>
+      <c r="J35" s="3">
+        <v>0.43328099280731358</v>
+      </c>
       <c r="N35" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -9209,7 +9276,9 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J36" s="3"/>
+      <c r="J36" s="3">
+        <v>0.4560033317230987</v>
+      </c>
       <c r="N36" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -9246,7 +9315,9 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J37" s="3"/>
+      <c r="J37" s="3">
+        <v>0.48895275485971929</v>
+      </c>
       <c r="N37" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -9283,7 +9354,9 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J38" s="3"/>
+      <c r="J38" s="3">
+        <v>0.52112425350214231</v>
+      </c>
       <c r="N38" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -9320,7 +9393,9 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J39" s="3"/>
+      <c r="J39" s="3">
+        <v>0.48060928466474029</v>
+      </c>
       <c r="N39" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -9357,7 +9432,9 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J40" s="3"/>
+      <c r="J40" s="3">
+        <v>0.4845793177748251</v>
+      </c>
       <c r="N40" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -9394,7 +9471,9 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J41" s="3"/>
+      <c r="J41" s="3">
+        <v>0.49273723542301417</v>
+      </c>
       <c r="N41" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -9431,7 +9510,9 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J42" s="3"/>
+      <c r="J42" s="3">
+        <v>0.43721252188626603</v>
+      </c>
       <c r="N42" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -9468,7 +9549,9 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J43" s="3"/>
+      <c r="J43" s="3">
+        <v>0.50685923671755306</v>
+      </c>
       <c r="N43" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -9505,7 +9588,9 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J44" s="3"/>
+      <c r="J44" s="3">
+        <v>0.52128673758164346</v>
+      </c>
       <c r="N44" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -9542,7 +9627,9 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J45" s="3"/>
+      <c r="J45" s="3">
+        <v>0.51201769662969987</v>
+      </c>
       <c r="N45" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -9579,7 +9666,9 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3">
+        <v>0.48673035336035397</v>
+      </c>
       <c r="N46" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -9616,7 +9705,9 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J47" s="3"/>
+      <c r="J47" s="3">
+        <v>0.5043141005455164</v>
+      </c>
       <c r="N47" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -9653,7 +9744,9 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J48" s="3"/>
+      <c r="J48" s="3">
+        <v>0.48371696359676741</v>
+      </c>
       <c r="N48" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -9690,7 +9783,9 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J49" s="3"/>
+      <c r="J49" s="3">
+        <v>0.48871337028589068</v>
+      </c>
       <c r="N49" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -9727,7 +9822,9 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J50" s="3"/>
+      <c r="J50" s="3">
+        <v>0.47151271182895532</v>
+      </c>
       <c r="N50" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -9764,7 +9861,9 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J51" s="3"/>
+      <c r="J51" s="3">
+        <v>0.49010386011949669</v>
+      </c>
       <c r="N51" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -9801,7 +9900,9 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J52" s="3"/>
+      <c r="J52" s="3">
+        <v>0.45256479629978652</v>
+      </c>
       <c r="N52" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -9838,7 +9939,9 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J53" s="3"/>
+      <c r="J53" s="3">
+        <v>0.549752036964267</v>
+      </c>
       <c r="N53" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -9883,9 +9986,9 @@
       <c r="I55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J55" s="3" t="e">
+      <c r="J55" s="3">
         <f>AVERAGE(J4:J53)</f>
-        <v>#DIV/0!</v>
+        <v>0.47267317624066968</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>3</v>
@@ -9923,9 +10026,9 @@
       <c r="I56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J56" s="3" t="e">
+      <c r="J56" s="3">
         <f>_xlfn.STDEV.S(J4:J53)</f>
-        <v>#DIV/0!</v>
+        <v>3.9683175963570169E-2</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>4</v>
@@ -9955,10 +10058,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:Q57"/>
+  <dimension ref="D3:P57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9967,19 +10070,19 @@
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="K3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>10</v>
@@ -9987,16 +10090,16 @@
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -10006,20 +10109,16 @@
       <c r="F5" s="3">
         <v>216.25894927536231</v>
       </c>
-      <c r="K5" s="2">
+      <c r="J5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="3">
-        <v>136.70759661835751</v>
-      </c>
-      <c r="P5" s="2">
+      <c r="K5" s="3"/>
+      <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="Q5" s="3">
-        <v>128.26578549403879</v>
-      </c>
-    </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
@@ -10030,22 +10129,18 @@
       <c r="F6" s="3">
         <v>208.92392512077291</v>
       </c>
-      <c r="K6" s="2">
-        <f>K5+1</f>
+      <c r="J6" s="2">
+        <f>J5+1</f>
         <v>2</v>
       </c>
-      <c r="L6" s="3">
-        <v>140.02938405797099</v>
-      </c>
-      <c r="P6" s="2">
-        <f>P5+1</f>
+      <c r="K6" s="3"/>
+      <c r="O6" s="2">
+        <f>O5+1</f>
         <v>2</v>
       </c>
-      <c r="Q6" s="3">
-        <v>133.62510106320829</v>
-      </c>
-    </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
@@ -10056,22 +10151,18 @@
       <c r="F7" s="3">
         <v>203.42491545893719</v>
       </c>
-      <c r="K7" s="2">
-        <f t="shared" ref="K7:K54" si="1">K6+1</f>
+      <c r="J7" s="2">
+        <f t="shared" ref="J7:J54" si="1">J6+1</f>
         <v>3</v>
       </c>
-      <c r="L7" s="3">
-        <v>142.045652173913</v>
-      </c>
-      <c r="P7" s="2">
-        <f t="shared" ref="P7:P54" si="2">P6+1</f>
+      <c r="K7" s="3"/>
+      <c r="O7" s="2">
+        <f t="shared" ref="O7:O54" si="2">O6+1</f>
         <v>3</v>
       </c>
-      <c r="Q7" s="3">
-        <v>129.6274868178424</v>
-      </c>
-    </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -10082,22 +10173,18 @@
       <c r="F8" s="3">
         <v>205.889347826087</v>
       </c>
-      <c r="K8" s="2">
+      <c r="J8" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L8" s="3">
-        <v>133.6248792270531</v>
-      </c>
-      <c r="P8" s="2">
+      <c r="K8" s="3"/>
+      <c r="O8" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Q8" s="3">
-        <v>127.0430453704974</v>
-      </c>
-    </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -10108,22 +10195,18 @@
       <c r="F9" s="3">
         <v>210.00800724637679</v>
       </c>
-      <c r="K9" s="2">
+      <c r="J9" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L9" s="3">
-        <v>133.76469806763279</v>
-      </c>
-      <c r="P9" s="2">
+      <c r="K9" s="3"/>
+      <c r="O9" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="Q9" s="3">
-        <v>131.5198761410567</v>
-      </c>
-    </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -10134,22 +10217,18 @@
       <c r="F10" s="3">
         <v>210.55535024154591</v>
       </c>
-      <c r="K10" s="2">
+      <c r="J10" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L10" s="3">
-        <v>147.3374033816425</v>
-      </c>
-      <c r="P10" s="2">
+      <c r="K10" s="3"/>
+      <c r="O10" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="Q10" s="3">
-        <v>129.9570566070802</v>
-      </c>
-    </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -10160,22 +10239,18 @@
       <c r="F11" s="3">
         <v>217.11873188405801</v>
       </c>
-      <c r="K11" s="2">
+      <c r="J11" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L11" s="3">
-        <v>139.13904589371981</v>
-      </c>
-      <c r="P11" s="2">
+      <c r="K11" s="3"/>
+      <c r="O11" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Q11" s="3">
-        <v>129.98991916721269</v>
-      </c>
-    </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -10186,22 +10261,18 @@
       <c r="F12" s="3">
         <v>216.93109903381651</v>
       </c>
-      <c r="K12" s="2">
+      <c r="J12" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="L12" s="3">
-        <v>139.21859903381639</v>
-      </c>
-      <c r="P12" s="2">
+      <c r="K12" s="3"/>
+      <c r="O12" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Q12" s="3">
-        <v>129.36490352133779</v>
-      </c>
-    </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -10212,22 +10283,18 @@
       <c r="F13" s="3">
         <v>212.62183574879231</v>
       </c>
-      <c r="K13" s="2">
+      <c r="J13" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L13" s="3">
-        <v>143.0381763285024</v>
-      </c>
-      <c r="P13" s="2">
+      <c r="K13" s="3"/>
+      <c r="O13" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="Q13" s="3">
-        <v>129.58422353535809</v>
-      </c>
-    </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -10238,22 +10305,18 @@
       <c r="F14" s="3">
         <v>202.3907729468599</v>
       </c>
-      <c r="K14" s="2">
+      <c r="J14" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L14" s="3">
-        <v>132.77280193236709</v>
-      </c>
-      <c r="P14" s="2">
+      <c r="K14" s="3"/>
+      <c r="O14" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="Q14" s="3">
-        <v>121.55001182330319</v>
-      </c>
-    </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -10264,22 +10327,18 @@
       <c r="F15" s="3">
         <v>203.79548309178739</v>
       </c>
-      <c r="K15" s="2">
+      <c r="J15" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="L15" s="3">
-        <v>136.1197101449275</v>
-      </c>
-      <c r="P15" s="2">
+      <c r="K15" s="3"/>
+      <c r="O15" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="Q15" s="3">
-        <v>134.26603925692251</v>
-      </c>
-    </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -10290,22 +10349,18 @@
       <c r="F16" s="3">
         <v>184.61871980676329</v>
       </c>
-      <c r="K16" s="2">
+      <c r="J16" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L16" s="3">
-        <v>140.01830917874389</v>
-      </c>
-      <c r="P16" s="2">
+      <c r="K16" s="3"/>
+      <c r="O16" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="Q16" s="3">
-        <v>133.82663780053539</v>
-      </c>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -10316,22 +10371,18 @@
       <c r="F17" s="3">
         <v>210.3666062801932</v>
       </c>
-      <c r="K17" s="2">
+      <c r="J17" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="L17" s="3">
-        <v>125.62954106280191</v>
-      </c>
-      <c r="P17" s="2">
+      <c r="K17" s="3"/>
+      <c r="O17" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="Q17" s="3">
-        <v>128.42998078554481</v>
-      </c>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -10342,22 +10393,18 @@
       <c r="F18" s="3">
         <v>205.06304347826091</v>
       </c>
-      <c r="K18" s="2">
+      <c r="J18" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="L18" s="3">
-        <v>136.0615458937198</v>
-      </c>
-      <c r="P18" s="2">
+      <c r="K18" s="3"/>
+      <c r="O18" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="Q18" s="3">
-        <v>127.01078078249689</v>
-      </c>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -10368,22 +10415,18 @@
       <c r="F19" s="3">
         <v>209.5690338164251</v>
       </c>
-      <c r="K19" s="2">
+      <c r="J19" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="L19" s="3">
-        <v>127.596497584541</v>
-      </c>
-      <c r="P19" s="2">
+      <c r="K19" s="3"/>
+      <c r="O19" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="Q19" s="3">
-        <v>130.095181108622</v>
-      </c>
-    </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -10394,22 +10437,18 @@
       <c r="F20" s="3">
         <v>200.81948067632851</v>
       </c>
-      <c r="K20" s="2">
+      <c r="J20" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="L20" s="3">
-        <v>132.5337198067632</v>
-      </c>
-      <c r="P20" s="2">
+      <c r="K20" s="3"/>
+      <c r="O20" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q20" s="3">
-        <v>126.8550053846193</v>
-      </c>
-    </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -10420,22 +10459,18 @@
       <c r="F21" s="3">
         <v>217.112077294686</v>
       </c>
-      <c r="K21" s="2">
+      <c r="J21" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L21" s="3">
-        <v>132.74778985507251</v>
-      </c>
-      <c r="P21" s="2">
+      <c r="K21" s="3"/>
+      <c r="O21" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="Q21" s="3">
-        <v>129.2379773261809</v>
-      </c>
-    </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -10446,22 +10481,18 @@
       <c r="F22" s="3">
         <v>199.72256038647339</v>
       </c>
-      <c r="K22" s="2">
+      <c r="J22" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="L22" s="3">
-        <v>143.7239855072464</v>
-      </c>
-      <c r="P22" s="2">
+      <c r="K22" s="3"/>
+      <c r="O22" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q22" s="3">
-        <v>131.68170694971479</v>
-      </c>
-    </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -10472,22 +10503,18 @@
       <c r="F23" s="3">
         <v>208.33532608695651</v>
       </c>
-      <c r="K23" s="2">
+      <c r="J23" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="L23" s="3">
-        <v>140.0293719806763</v>
-      </c>
-      <c r="P23" s="2">
+      <c r="K23" s="3"/>
+      <c r="O23" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="Q23" s="3">
-        <v>128.06853639951839</v>
-      </c>
-    </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -10498,22 +10525,18 @@
       <c r="F24" s="3">
         <v>197.21481884057971</v>
       </c>
-      <c r="K24" s="2">
+      <c r="J24" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="L24" s="3">
-        <v>138.0535628019324</v>
-      </c>
-      <c r="P24" s="2">
+      <c r="K24" s="3"/>
+      <c r="O24" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="Q24" s="3">
-        <v>124.88711724754521</v>
-      </c>
-    </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -10524,22 +10547,18 @@
       <c r="F25" s="3">
         <v>200.88818840579711</v>
       </c>
-      <c r="K25" s="2">
+      <c r="J25" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="L25" s="3">
-        <v>137.1313405797101</v>
-      </c>
-      <c r="P25" s="2">
+      <c r="K25" s="3"/>
+      <c r="O25" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="Q25" s="3">
-        <v>136.9638362364559</v>
-      </c>
-    </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -10550,22 +10569,18 @@
       <c r="F26" s="3">
         <v>215.2133816425121</v>
       </c>
-      <c r="K26" s="2">
+      <c r="J26" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="L26" s="3">
-        <v>143.0036111111111</v>
-      </c>
-      <c r="P26" s="2">
+      <c r="K26" s="3"/>
+      <c r="O26" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="Q26" s="3">
-        <v>123.8382186688814</v>
-      </c>
-    </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -10576,22 +10591,18 @@
       <c r="F27" s="3">
         <v>213.6066666666666</v>
       </c>
-      <c r="K27" s="2">
+      <c r="J27" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="L27" s="3">
-        <v>130.3520893719807</v>
-      </c>
-      <c r="P27" s="2">
+      <c r="K27" s="3"/>
+      <c r="O27" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="Q27" s="3">
-        <v>126.3511993477499</v>
-      </c>
-    </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -10602,22 +10613,18 @@
       <c r="F28" s="3">
         <v>206.40169082125601</v>
       </c>
-      <c r="K28" s="2">
+      <c r="J28" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L28" s="3">
-        <v>138.08850241545889</v>
-      </c>
-      <c r="P28" s="2">
+      <c r="K28" s="3"/>
+      <c r="O28" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="Q28" s="3">
-        <v>128.62619196929751</v>
-      </c>
-    </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -10628,22 +10635,18 @@
       <c r="F29" s="3">
         <v>211.1742391304347</v>
       </c>
-      <c r="K29" s="2">
+      <c r="J29" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="L29" s="3">
-        <v>137.84788647343001</v>
-      </c>
-      <c r="P29" s="2">
+      <c r="K29" s="3"/>
+      <c r="O29" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="Q29" s="3">
-        <v>135.8322929842474</v>
-      </c>
-    </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -10654,22 +10657,18 @@
       <c r="F30" s="3">
         <v>205.2859541062802</v>
       </c>
-      <c r="K30" s="2">
+      <c r="J30" s="2">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="L30" s="3">
-        <v>136.52646135265701</v>
-      </c>
-      <c r="P30" s="2">
+      <c r="K30" s="3"/>
+      <c r="O30" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="Q30" s="3">
-        <v>133.211285933444</v>
-      </c>
-    </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -10680,22 +10679,18 @@
       <c r="F31" s="3">
         <v>209.96460144927539</v>
       </c>
-      <c r="K31" s="2">
+      <c r="J31" s="2">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="L31" s="3">
-        <v>141.22724637681159</v>
-      </c>
-      <c r="P31" s="2">
+      <c r="K31" s="3"/>
+      <c r="O31" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="Q31" s="3">
-        <v>132.81840961967319</v>
-      </c>
-    </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -10706,22 +10701,18 @@
       <c r="F32" s="3">
         <v>206.06233091787439</v>
       </c>
-      <c r="K32" s="2">
+      <c r="J32" s="2">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="L32" s="3">
-        <v>135.13685990338161</v>
-      </c>
-      <c r="P32" s="2">
+      <c r="K32" s="3"/>
+      <c r="O32" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="Q32" s="3">
-        <v>137.04150591546141</v>
-      </c>
-    </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -10732,22 +10723,18 @@
       <c r="F33" s="3">
         <v>201.18555555555551</v>
       </c>
-      <c r="K33" s="2">
+      <c r="J33" s="2">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="L33" s="3">
-        <v>133.108115942029</v>
-      </c>
-      <c r="P33" s="2">
+      <c r="K33" s="3"/>
+      <c r="O33" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="Q33" s="3">
-        <v>132.20322075161161</v>
-      </c>
-    </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -10758,22 +10745,18 @@
       <c r="F34" s="3">
         <v>206.6653260869565</v>
       </c>
-      <c r="K34" s="2">
+      <c r="J34" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="L34" s="3">
-        <v>128.33978260869571</v>
-      </c>
-      <c r="P34" s="2">
+      <c r="K34" s="3"/>
+      <c r="O34" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="Q34" s="3">
-        <v>125.6606524533037</v>
-      </c>
-    </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -10784,22 +10767,18 @@
       <c r="F35" s="3">
         <v>210.65793478260861</v>
       </c>
-      <c r="K35" s="2">
+      <c r="J35" s="2">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="L35" s="3">
-        <v>135.25376811594199</v>
-      </c>
-      <c r="P35" s="2">
+      <c r="K35" s="3"/>
+      <c r="O35" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="Q35" s="3">
-        <v>132.000601070828</v>
-      </c>
-    </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -10810,22 +10789,18 @@
       <c r="F36" s="3">
         <v>207.55211352657</v>
       </c>
-      <c r="K36" s="2">
+      <c r="J36" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="L36" s="3">
-        <v>137.0328260869565</v>
-      </c>
-      <c r="P36" s="2">
+      <c r="K36" s="3"/>
+      <c r="O36" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="Q36" s="3">
-        <v>130.70111742279931</v>
-      </c>
-    </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -10836,22 +10811,18 @@
       <c r="F37" s="3">
         <v>211.44378019323671</v>
       </c>
-      <c r="K37" s="2">
+      <c r="J37" s="2">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="L37" s="3">
-        <v>136.23909420289851</v>
-      </c>
-      <c r="P37" s="2">
+      <c r="K37" s="3"/>
+      <c r="O37" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="Q37" s="3">
-        <v>130.49670548926369</v>
-      </c>
-    </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -10862,22 +10833,18 @@
       <c r="F38" s="3">
         <v>207.05544685990341</v>
       </c>
-      <c r="K38" s="2">
+      <c r="J38" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="L38" s="3">
-        <v>127.33426328502421</v>
-      </c>
-      <c r="P38" s="2">
+      <c r="K38" s="3"/>
+      <c r="O38" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="Q38" s="3">
-        <v>120.0395161335385</v>
-      </c>
-    </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -10888,22 +10855,18 @@
       <c r="F39" s="3">
         <v>198.01435990338169</v>
       </c>
-      <c r="K39" s="2">
+      <c r="J39" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="L39" s="3">
-        <v>133.75925120772951</v>
-      </c>
-      <c r="P39" s="2">
+      <c r="K39" s="3"/>
+      <c r="O39" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="Q39" s="3">
-        <v>122.8834256338357</v>
-      </c>
-    </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10914,22 +10877,18 @@
       <c r="F40" s="3">
         <v>214.56683574879219</v>
       </c>
-      <c r="K40" s="2">
+      <c r="J40" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="L40" s="3">
-        <v>134.3876690821256</v>
-      </c>
-      <c r="P40" s="2">
+      <c r="K40" s="3"/>
+      <c r="O40" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="Q40" s="3">
-        <v>126.88575873603681</v>
-      </c>
-    </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P40" s="3"/>
+    </row>
+    <row r="41" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10940,22 +10899,18 @@
       <c r="F41" s="3">
         <v>207.304577294686</v>
       </c>
-      <c r="K41" s="2">
+      <c r="J41" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="L41" s="3">
-        <v>147.03033816425119</v>
-      </c>
-      <c r="P41" s="2">
+      <c r="K41" s="3"/>
+      <c r="O41" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="Q41" s="3">
-        <v>139.64682838303941</v>
-      </c>
-    </row>
-    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P41" s="3"/>
+    </row>
+    <row r="42" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10966,22 +10921,18 @@
       <c r="F42" s="3">
         <v>212.26068840579711</v>
       </c>
-      <c r="K42" s="2">
+      <c r="J42" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="L42" s="3">
-        <v>130.38921497584539</v>
-      </c>
-      <c r="P42" s="2">
+      <c r="K42" s="3"/>
+      <c r="O42" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="Q42" s="3">
-        <v>132.92362707447541</v>
-      </c>
-    </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10992,22 +10943,18 @@
       <c r="F43" s="3">
         <v>192.08737922705311</v>
       </c>
-      <c r="K43" s="2">
+      <c r="J43" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="L43" s="3">
-        <v>134.8178260869565</v>
-      </c>
-      <c r="P43" s="2">
+      <c r="K43" s="3"/>
+      <c r="O43" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="Q43" s="3">
-        <v>124.34017943227821</v>
-      </c>
-    </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P43" s="3"/>
+    </row>
+    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -11018,22 +10965,18 @@
       <c r="F44" s="3">
         <v>204.32443236714971</v>
       </c>
-      <c r="K44" s="2">
+      <c r="J44" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L44" s="3">
-        <v>142.17863526570051</v>
-      </c>
-      <c r="P44" s="2">
+      <c r="K44" s="3"/>
+      <c r="O44" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="Q44" s="3">
-        <v>141.23971837425131</v>
-      </c>
-    </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P44" s="3"/>
+    </row>
+    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -11044,22 +10987,18 @@
       <c r="F45" s="3">
         <v>196.91400966183571</v>
       </c>
-      <c r="K45" s="2">
+      <c r="J45" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="L45" s="3">
-        <v>136.1986835748792</v>
-      </c>
-      <c r="P45" s="2">
+      <c r="K45" s="3"/>
+      <c r="O45" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="Q45" s="3">
-        <v>130.11608710891659</v>
-      </c>
-    </row>
-    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P45" s="3"/>
+    </row>
+    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -11070,22 +11009,18 @@
       <c r="F46" s="3">
         <v>216.0747342995169</v>
       </c>
-      <c r="K46" s="2">
+      <c r="J46" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="L46" s="3">
-        <v>132.6260144927536</v>
-      </c>
-      <c r="P46" s="2">
+      <c r="K46" s="3"/>
+      <c r="O46" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="Q46" s="3">
-        <v>125.51807460491619</v>
-      </c>
-    </row>
-    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P46" s="3"/>
+    </row>
+    <row r="47" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -11096,22 +11031,18 @@
       <c r="F47" s="3">
         <v>214.19390096618349</v>
       </c>
-      <c r="K47" s="2">
+      <c r="J47" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="L47" s="3">
-        <v>132.69594202898551</v>
-      </c>
-      <c r="P47" s="2">
+      <c r="K47" s="3"/>
+      <c r="O47" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="Q47" s="3">
-        <v>136.47943497056241</v>
-      </c>
-    </row>
-    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P47" s="3"/>
+    </row>
+    <row r="48" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -11122,22 +11053,18 @@
       <c r="F48" s="3">
         <v>201.84665458937201</v>
       </c>
-      <c r="K48" s="2">
+      <c r="J48" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="L48" s="3">
-        <v>137.0407729468599</v>
-      </c>
-      <c r="P48" s="2">
+      <c r="K48" s="3"/>
+      <c r="O48" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="Q48" s="3">
-        <v>126.73580691821979</v>
-      </c>
-    </row>
-    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P48" s="3"/>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -11148,22 +11075,18 @@
       <c r="F49" s="3">
         <v>215.09971014492751</v>
       </c>
-      <c r="K49" s="2">
+      <c r="J49" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="L49" s="3">
-        <v>140.53869565217391</v>
-      </c>
-      <c r="P49" s="2">
+      <c r="K49" s="3"/>
+      <c r="O49" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="Q49" s="3">
-        <v>141.23559237161999</v>
-      </c>
-    </row>
-    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P49" s="3"/>
+    </row>
+    <row r="50" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -11174,22 +11097,18 @@
       <c r="F50" s="3">
         <v>221.140652173913</v>
       </c>
-      <c r="K50" s="2">
+      <c r="J50" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="L50" s="3">
-        <v>145.40161835748791</v>
-      </c>
-      <c r="P50" s="2">
+      <c r="K50" s="3"/>
+      <c r="O50" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="Q50" s="3">
-        <v>136.73420574325519</v>
-      </c>
-    </row>
-    <row r="51" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P50" s="3"/>
+    </row>
+    <row r="51" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -11200,22 +11119,18 @@
       <c r="F51" s="3">
         <v>209.0242028985507</v>
       </c>
-      <c r="K51" s="2">
+      <c r="J51" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="L51" s="3">
-        <v>140.2756642512077</v>
-      </c>
-      <c r="P51" s="2">
+      <c r="K51" s="3"/>
+      <c r="O51" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="Q51" s="3">
-        <v>133.9830523298638</v>
-      </c>
-    </row>
-    <row r="52" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P51" s="3"/>
+    </row>
+    <row r="52" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -11226,22 +11141,18 @@
       <c r="F52" s="3">
         <v>197.6072946859903</v>
       </c>
-      <c r="K52" s="2">
+      <c r="J52" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="L52" s="3">
-        <v>140.66734299516909</v>
-      </c>
-      <c r="P52" s="2">
+      <c r="K52" s="3"/>
+      <c r="O52" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="Q52" s="3">
-        <v>131.2224712100662</v>
-      </c>
-    </row>
-    <row r="53" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P52" s="3"/>
+    </row>
+    <row r="53" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -11252,22 +11163,18 @@
       <c r="F53" s="3">
         <v>209.78096618357489</v>
       </c>
-      <c r="K53" s="2">
+      <c r="J53" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="L53" s="3">
-        <v>132.01683574879229</v>
-      </c>
-      <c r="P53" s="2">
+      <c r="K53" s="3"/>
+      <c r="O53" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="Q53" s="3">
-        <v>132.4690521927084</v>
-      </c>
-    </row>
-    <row r="54" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P53" s="3"/>
+    </row>
+    <row r="54" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -11278,22 +11185,18 @@
       <c r="F54" s="3">
         <v>194.1978260869565</v>
       </c>
-      <c r="K54" s="2">
+      <c r="J54" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="L54" s="3">
-        <v>140.04112318840581</v>
-      </c>
-      <c r="P54" s="2">
+      <c r="K54" s="3"/>
+      <c r="O54" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="Q54" s="3">
-        <v>126.631875892145</v>
-      </c>
-    </row>
-    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P54" s="3"/>
+    </row>
+    <row r="56" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>3</v>
       </c>
@@ -11305,22 +11208,22 @@
         <f>AVERAGE(F5:F54)</f>
         <v>207.1667103864734</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="J56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L56" s="3">
-        <f>AVERAGE(L5:L54)</f>
-        <v>136.73759492753624</v>
-      </c>
-      <c r="P56" s="2" t="s">
+      <c r="K56" s="3" t="e">
+        <f>AVERAGE(K5:K54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q56" s="3">
-        <f>AVERAGE(Q5:Q54)</f>
-        <v>130.39432635110768</v>
-      </c>
-    </row>
-    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="P56" s="3" t="e">
+        <f>AVERAGE(P5:P54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>4</v>
       </c>
@@ -11332,19 +11235,19 @@
         <f>_xlfn.STDEV.S(F5:F54)</f>
         <v>7.3329690189643877</v>
       </c>
-      <c r="K57" s="2" t="s">
+      <c r="J57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L57" s="3">
-        <f>_xlfn.STDEV.S(L5:L54)</f>
-        <v>4.9685652830725484</v>
-      </c>
-      <c r="P57" s="2" t="s">
+      <c r="K57" s="3" t="e">
+        <f>_xlfn.STDEV.S(K5:K54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q57" s="3">
-        <f>_xlfn.STDEV.S(Q5:Q54)</f>
-        <v>4.7585997477790096</v>
+      <c r="P57" s="3" t="e">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test-23: extrapol 2.0 & hybrid3 2.0 (mae)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="r2 (2Ysum)" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="18">
   <si>
     <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24-f 3Ysum.csv)</t>
-  </si>
-  <si>
-    <t>Hybrid3-model (superdataset-24-f + 2Y + 3Y.csv)</t>
   </si>
   <si>
     <t>RF-100 (superdataset-24-f.csv + extrapol 2.0)</t>
@@ -463,14 +460,14 @@
       </c>
       <c r="J3" s="5"/>
       <c r="N3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="T3" s="5"/>
       <c r="X3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="3:25" x14ac:dyDescent="0.25">
@@ -2607,10 +2604,10 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>6</v>
@@ -5128,11 +5125,11 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>6</v>
@@ -7975,13 +7972,13 @@
       </c>
       <c r="E2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
@@ -10060,8 +10057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10076,10 +10073,10 @@
       </c>
       <c r="F3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="4:16" x14ac:dyDescent="0.25">
@@ -10112,11 +10109,15 @@
       <c r="J5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>206.66380660954709</v>
+      </c>
       <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="3">
+        <v>201.90884944920441</v>
+      </c>
     </row>
     <row r="6" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
@@ -10133,12 +10134,16 @@
         <f>J5+1</f>
         <v>2</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3">
+        <v>212.8558629130967</v>
+      </c>
       <c r="O6" s="2">
         <f>O5+1</f>
         <v>2</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="3">
+        <v>208.26321909424721</v>
+      </c>
     </row>
     <row r="7" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
@@ -10155,12 +10160,16 @@
         <f t="shared" ref="J7:J54" si="1">J6+1</f>
         <v>3</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>214.32481028151781</v>
+      </c>
       <c r="O7" s="2">
         <f t="shared" ref="O7:O54" si="2">O6+1</f>
         <v>3</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="3">
+        <v>202.3569522643819</v>
+      </c>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
@@ -10177,12 +10186,16 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>201.02997552019579</v>
+      </c>
       <c r="O8" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="3">
+        <v>195.578029375765</v>
+      </c>
     </row>
     <row r="9" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
@@ -10199,12 +10212,16 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>197.1347735618115</v>
+      </c>
       <c r="O9" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="3">
+        <v>204.21499388004901</v>
+      </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
@@ -10221,12 +10238,16 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="3">
+        <v>195.36096695226439</v>
+      </c>
       <c r="O10" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P10" s="3"/>
+      <c r="P10" s="3">
+        <v>193.42537331701351</v>
+      </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
@@ -10243,12 +10264,16 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3">
+        <v>204.97538555691551</v>
+      </c>
       <c r="O11" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="P11" s="3"/>
+      <c r="P11" s="3">
+        <v>194.7519094247246</v>
+      </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
@@ -10265,12 +10290,16 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="3">
+        <v>204.89599755201959</v>
+      </c>
       <c r="O12" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="P12" s="3"/>
+      <c r="P12" s="3">
+        <v>209.19140758873931</v>
+      </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
@@ -10287,12 +10316,16 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3">
+        <v>195.98128518971851</v>
+      </c>
       <c r="O13" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="P13" s="3">
+        <v>189.51013463892289</v>
+      </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
@@ -10309,12 +10342,16 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="3">
+        <v>200.9626438188495</v>
+      </c>
       <c r="O14" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="P14" s="3"/>
+      <c r="P14" s="3">
+        <v>196.13413708690331</v>
+      </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
@@ -10331,12 +10368,16 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="K15" s="3"/>
+      <c r="K15" s="3">
+        <v>213.92667074663399</v>
+      </c>
       <c r="O15" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P15" s="3"/>
+      <c r="P15" s="3">
+        <v>199.1854957160343</v>
+      </c>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
@@ -10353,12 +10394,16 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3">
+        <v>206.2847246022032</v>
+      </c>
       <c r="O16" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="P16" s="3"/>
+      <c r="P16" s="3">
+        <v>195.36242350061201</v>
+      </c>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
@@ -10375,12 +10420,16 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3">
+        <v>206.01085679314559</v>
+      </c>
       <c r="O17" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="P17" s="3"/>
+      <c r="P17" s="3">
+        <v>199.86490820073439</v>
+      </c>
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
@@ -10397,12 +10446,16 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="K18" s="3"/>
+      <c r="K18" s="3">
+        <v>217.98350061199511</v>
+      </c>
       <c r="O18" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="P18" s="3"/>
+      <c r="P18" s="3">
+        <v>202.64277845777229</v>
+      </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
@@ -10419,12 +10472,16 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="K19" s="3"/>
+      <c r="K19" s="3">
+        <v>205.23118727050181</v>
+      </c>
       <c r="O19" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="P19" s="3"/>
+      <c r="P19" s="3">
+        <v>189.8554345165239</v>
+      </c>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
@@ -10441,12 +10498,16 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3">
+        <v>187.24915544675639</v>
+      </c>
       <c r="O20" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="P20" s="3"/>
+      <c r="P20" s="3">
+        <v>197.23663402692779</v>
+      </c>
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
@@ -10463,12 +10524,16 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="K21" s="3"/>
+      <c r="K21" s="3">
+        <v>196.88682986536111</v>
+      </c>
       <c r="O21" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="P21" s="3"/>
+      <c r="P21" s="3">
+        <v>203.65611995104041</v>
+      </c>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
@@ -10485,12 +10550,16 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3">
+        <v>214.93334149326799</v>
+      </c>
       <c r="O22" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="P22" s="3">
+        <v>198.8673561811506</v>
+      </c>
     </row>
     <row r="23" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
@@ -10507,12 +10576,16 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3">
+        <v>205.9227539779682</v>
+      </c>
       <c r="O23" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="P23" s="3"/>
+      <c r="P23" s="3">
+        <v>201.3649938800489</v>
+      </c>
     </row>
     <row r="24" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
@@ -10529,12 +10602,16 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <v>198.87408812729501</v>
+      </c>
       <c r="O24" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="P24" s="3"/>
+      <c r="P24" s="3">
+        <v>189.76112607099139</v>
+      </c>
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
@@ -10551,12 +10628,16 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="K25" s="3"/>
+      <c r="K25" s="3">
+        <v>197.95283965728271</v>
+      </c>
       <c r="O25" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P25" s="3"/>
+      <c r="P25" s="3">
+        <v>200.21166462668299</v>
+      </c>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
@@ -10573,12 +10654,16 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="K26" s="3"/>
+      <c r="K26" s="3">
+        <v>207.66452876376991</v>
+      </c>
       <c r="O26" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="P26" s="3">
+        <v>193.31332925336599</v>
+      </c>
     </row>
     <row r="27" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
@@ -10595,12 +10680,16 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="K27" s="3"/>
+      <c r="K27" s="3">
+        <v>197.90394124847001</v>
+      </c>
       <c r="O27" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="P27" s="3"/>
+      <c r="P27" s="3">
+        <v>186.67208078335369</v>
+      </c>
     </row>
     <row r="28" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
@@ -10617,12 +10706,16 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="K28" s="3"/>
+      <c r="K28" s="3">
+        <v>209.68507955936349</v>
+      </c>
       <c r="O28" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="P28" s="3"/>
+      <c r="P28" s="3">
+        <v>201.99212974296211</v>
+      </c>
     </row>
     <row r="29" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
@@ -10639,12 +10732,16 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="K29" s="3"/>
+      <c r="K29" s="3">
+        <v>202.95128518971839</v>
+      </c>
       <c r="O29" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="P29" s="3"/>
+      <c r="P29" s="3">
+        <v>186.95958384332931</v>
+      </c>
     </row>
     <row r="30" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
@@ -10661,12 +10758,16 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="K30" s="3"/>
+      <c r="K30" s="3">
+        <v>219.02046511627901</v>
+      </c>
       <c r="O30" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="P30" s="3"/>
+      <c r="P30" s="3">
+        <v>193.643341493268</v>
+      </c>
     </row>
     <row r="31" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
@@ -10683,12 +10784,16 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="K31" s="3"/>
+      <c r="K31" s="3">
+        <v>197.50045287637701</v>
+      </c>
       <c r="O31" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="P31" s="3"/>
+      <c r="P31" s="3">
+        <v>197.10949816401461</v>
+      </c>
     </row>
     <row r="32" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
@@ -10705,12 +10810,16 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="K32" s="3"/>
+      <c r="K32" s="3">
+        <v>194.2596205630355</v>
+      </c>
       <c r="O32" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="P32" s="3"/>
+      <c r="P32" s="3">
+        <v>203.89558139534881</v>
+      </c>
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
@@ -10727,12 +10836,16 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="K33" s="3"/>
+      <c r="K33" s="3">
+        <v>207.83381884944919</v>
+      </c>
       <c r="O33" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="P33" s="3"/>
+      <c r="P33" s="3">
+        <v>200.75492044063651</v>
+      </c>
     </row>
     <row r="34" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
@@ -10749,12 +10862,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="K34" s="3"/>
+      <c r="K34" s="3">
+        <v>205.1839167686658</v>
+      </c>
       <c r="O34" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="P34" s="3"/>
+      <c r="P34" s="3">
+        <v>182.58177478580171</v>
+      </c>
     </row>
     <row r="35" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
@@ -10771,12 +10888,16 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="K35" s="3"/>
+      <c r="K35" s="3">
+        <v>199.70571603427169</v>
+      </c>
       <c r="O35" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="P35" s="3"/>
+      <c r="P35" s="3">
+        <v>193.973476132191</v>
+      </c>
     </row>
     <row r="36" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
@@ -10793,12 +10914,16 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="K36" s="3"/>
+      <c r="K36" s="3">
+        <v>199.8348347613219</v>
+      </c>
       <c r="O36" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="P36" s="3"/>
+      <c r="P36" s="3">
+        <v>192.87325581395351</v>
+      </c>
     </row>
     <row r="37" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
@@ -10815,12 +10940,16 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="K37" s="3"/>
+      <c r="K37" s="3">
+        <v>201.90072215422271</v>
+      </c>
       <c r="O37" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="P37" s="3"/>
+      <c r="P37" s="3">
+        <v>201.4863892288862</v>
+      </c>
     </row>
     <row r="38" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
@@ -10837,12 +10966,16 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="K38" s="3"/>
+      <c r="K38" s="3">
+        <v>210.15872705018359</v>
+      </c>
       <c r="O38" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="P38" s="3"/>
+      <c r="P38" s="3">
+        <v>189.74165238678091</v>
+      </c>
     </row>
     <row r="39" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
@@ -10859,12 +10992,16 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="K39" s="3"/>
+      <c r="K39" s="3">
+        <v>197.1021787025704</v>
+      </c>
       <c r="O39" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="P39" s="3"/>
+      <c r="P39" s="3">
+        <v>198.32725826193391</v>
+      </c>
     </row>
     <row r="40" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
@@ -10881,12 +11018,16 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="K40" s="3"/>
+      <c r="K40" s="3">
+        <v>208.03127294981641</v>
+      </c>
       <c r="O40" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="P40" s="3"/>
+      <c r="P40" s="3">
+        <v>191.91577723378211</v>
+      </c>
     </row>
     <row r="41" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
@@ -10903,12 +11044,16 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="K41" s="3"/>
+      <c r="K41" s="3">
+        <v>210.57657282741741</v>
+      </c>
       <c r="O41" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="P41" s="3"/>
+      <c r="P41" s="3">
+        <v>202.66350061199509</v>
+      </c>
     </row>
     <row r="42" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
@@ -10925,12 +11070,16 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="K42" s="3"/>
+      <c r="K42" s="3">
+        <v>202.71604651162789</v>
+      </c>
       <c r="O42" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="P42" s="3"/>
+      <c r="P42" s="3">
+        <v>201.27548347613219</v>
+      </c>
     </row>
     <row r="43" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
@@ -10947,12 +11096,16 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="K43" s="3"/>
+      <c r="K43" s="3">
+        <v>198.43517747858019</v>
+      </c>
       <c r="O43" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="P43" s="3"/>
+      <c r="P43" s="3">
+        <v>202.94133414932679</v>
+      </c>
     </row>
     <row r="44" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
@@ -10969,12 +11122,16 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K44" s="3"/>
+      <c r="K44" s="3">
+        <v>203.32753977968181</v>
+      </c>
       <c r="O44" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P44" s="3"/>
+      <c r="P44" s="3">
+        <v>211.36705018359851</v>
+      </c>
     </row>
     <row r="45" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
@@ -10991,12 +11148,16 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="K45" s="3"/>
+      <c r="K45" s="3">
+        <v>212.9602447980416</v>
+      </c>
       <c r="O45" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="P45" s="3"/>
+      <c r="P45" s="3">
+        <v>209.0415544675642</v>
+      </c>
     </row>
     <row r="46" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
@@ -11013,12 +11174,16 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="K46" s="3"/>
+      <c r="K46" s="3">
+        <v>203.55583843329251</v>
+      </c>
       <c r="O46" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="P46" s="3"/>
+      <c r="P46" s="3">
+        <v>198.20809057527541</v>
+      </c>
     </row>
     <row r="47" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
@@ -11035,12 +11200,16 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="K47" s="3"/>
+      <c r="K47" s="3">
+        <v>204.4150305997552</v>
+      </c>
       <c r="O47" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="P47" s="3"/>
+      <c r="P47" s="3">
+        <v>196.59665850673201</v>
+      </c>
     </row>
     <row r="48" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
@@ -11057,12 +11226,16 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="K48" s="3"/>
+      <c r="K48" s="3">
+        <v>207.16824969400241</v>
+      </c>
       <c r="O48" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="P48" s="3"/>
+      <c r="P48" s="3">
+        <v>208.57662178702569</v>
+      </c>
     </row>
     <row r="49" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
@@ -11079,12 +11252,16 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="K49" s="3"/>
+      <c r="K49" s="3">
+        <v>195.307429620563</v>
+      </c>
       <c r="O49" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="P49" s="3"/>
+      <c r="P49" s="3">
+        <v>202.00973072215419</v>
+      </c>
     </row>
     <row r="50" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
@@ -11101,12 +11278,16 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="K50" s="3"/>
+      <c r="K50" s="3">
+        <v>198.4937576499388</v>
+      </c>
       <c r="O50" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="P50" s="3"/>
+      <c r="P50" s="3">
+        <v>192.64286413708689</v>
+      </c>
     </row>
     <row r="51" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
@@ -11123,12 +11304,16 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="K51" s="3"/>
+      <c r="K51" s="3">
+        <v>210.52051407588741</v>
+      </c>
       <c r="O51" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="P51" s="3"/>
+      <c r="P51" s="3">
+        <v>190.80787025703791</v>
+      </c>
     </row>
     <row r="52" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
@@ -11145,12 +11330,16 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="K52" s="3"/>
+      <c r="K52" s="3">
+        <v>195.04549571603431</v>
+      </c>
       <c r="O52" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="P52" s="3"/>
+      <c r="P52" s="3">
+        <v>197.01254589963281</v>
+      </c>
     </row>
     <row r="53" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
@@ -11167,12 +11356,16 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="K53" s="3"/>
+      <c r="K53" s="3">
+        <v>206.35179926560579</v>
+      </c>
       <c r="O53" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="P53" s="3"/>
+      <c r="P53" s="3">
+        <v>200.15489596083231</v>
+      </c>
     </row>
     <row r="54" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
@@ -11189,12 +11382,16 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K54" s="3"/>
+      <c r="K54" s="3">
+        <v>200.96567931456551</v>
+      </c>
       <c r="O54" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P54" s="3"/>
+      <c r="P54" s="3">
+        <v>194.21965728274171</v>
+      </c>
     </row>
     <row r="56" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
@@ -11211,16 +11408,16 @@
       <c r="J56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K56" s="3" t="e">
+      <c r="K56" s="3">
         <f>AVERAGE(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>203.88034785801716</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P56" s="3" t="e">
+      <c r="P56" s="3">
         <f>AVERAGE(P5:P54)</f>
-        <v>#DIV/0!</v>
+        <v>197.92203696450434</v>
       </c>
     </row>
     <row r="57" spans="4:16" x14ac:dyDescent="0.25">
@@ -11238,16 +11435,16 @@
       <c r="J57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K57" s="3" t="e">
+      <c r="K57" s="3">
         <f>_xlfn.STDEV.S(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>6.7529692742488869</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="3" t="e">
+      <c r="P57" s="3">
         <f>_xlfn.STDEV.S(P5:P54)</f>
-        <v>#DIV/0!</v>
+        <v>6.3389469523502964</v>
       </c>
     </row>
   </sheetData>
@@ -11259,8 +11456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11274,10 +11471,10 @@
       </c>
       <c r="E3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
@@ -11310,15 +11507,11 @@
       <c r="J5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="3">
-        <v>53910.977389492742</v>
-      </c>
+      <c r="K5" s="3"/>
       <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="P5" s="3">
-        <v>39006.772192397009</v>
-      </c>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
@@ -11335,16 +11528,12 @@
         <f>J5+1</f>
         <v>2</v>
       </c>
-      <c r="K6" s="3">
-        <v>50096.715575362308</v>
-      </c>
+      <c r="K6" s="3"/>
       <c r="O6" s="2">
         <f>O5+1</f>
         <v>2</v>
       </c>
-      <c r="P6" s="3">
-        <v>47733.867400683142</v>
-      </c>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -11361,16 +11550,12 @@
         <f t="shared" ref="J7:J54" si="1">J6+1</f>
         <v>3</v>
       </c>
-      <c r="K7" s="3">
-        <v>35222.748448067621</v>
-      </c>
+      <c r="K7" s="3"/>
       <c r="O7" s="2">
         <f t="shared" ref="O7:O54" si="2">O6+1</f>
         <v>3</v>
       </c>
-      <c r="P7" s="3">
-        <v>45164.441367669169</v>
-      </c>
+      <c r="P7" s="3"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -11387,16 +11572,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K8" s="3">
-        <v>47993.271027294657</v>
-      </c>
+      <c r="K8" s="3"/>
       <c r="O8" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="P8" s="3">
-        <v>45249.927797043427</v>
-      </c>
+      <c r="P8" s="3"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -11413,16 +11594,12 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K9" s="3">
-        <v>44127.120558454088</v>
-      </c>
+      <c r="K9" s="3"/>
       <c r="O9" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="P9" s="3">
-        <v>46666.908726800379</v>
-      </c>
+      <c r="P9" s="3"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -11439,16 +11616,12 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K10" s="3">
-        <v>46044.093117753611</v>
-      </c>
+      <c r="K10" s="3"/>
       <c r="O10" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P10" s="3">
-        <v>39610.820316505968</v>
-      </c>
+      <c r="P10" s="3"/>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -11465,16 +11638,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K11" s="3">
-        <v>44652.600970531377</v>
-      </c>
+      <c r="K11" s="3"/>
       <c r="O11" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="P11" s="3">
-        <v>41517.573482272317</v>
-      </c>
+      <c r="P11" s="3"/>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -11491,16 +11660,12 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K12" s="3">
-        <v>48462.159571618336</v>
-      </c>
+      <c r="K12" s="3"/>
       <c r="O12" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="P12" s="3">
-        <v>38511.678189972081</v>
-      </c>
+      <c r="P12" s="3"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -11517,16 +11682,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K13" s="3">
-        <v>53709.71522971012</v>
-      </c>
+      <c r="K13" s="3"/>
       <c r="O13" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="P13" s="3">
-        <v>37856.255232051291</v>
-      </c>
+      <c r="P13" s="3"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -11543,16 +11704,12 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K14" s="3">
-        <v>46608.68287463767</v>
-      </c>
+      <c r="K14" s="3"/>
       <c r="O14" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="P14" s="3">
-        <v>42811.744130845997</v>
-      </c>
+      <c r="P14" s="3"/>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -11569,16 +11726,12 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="K15" s="3">
-        <v>38590.6025874396</v>
-      </c>
+      <c r="K15" s="3"/>
       <c r="O15" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P15" s="3">
-        <v>42717.032815501218</v>
-      </c>
+      <c r="P15" s="3"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -11595,16 +11748,12 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="K16" s="3">
-        <v>45850.156096497572</v>
-      </c>
+      <c r="K16" s="3"/>
       <c r="O16" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="P16" s="3">
-        <v>49696.344082386589</v>
-      </c>
+      <c r="P16" s="3"/>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -11621,16 +11770,12 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="K17" s="3">
-        <v>45611.040309420277</v>
-      </c>
+      <c r="K17" s="3"/>
       <c r="O17" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="P17" s="3">
-        <v>40635.625035213758</v>
-      </c>
+      <c r="P17" s="3"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -11647,16 +11792,12 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="K18" s="3">
-        <v>42803.785097222208</v>
-      </c>
+      <c r="K18" s="3"/>
       <c r="O18" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="P18" s="3">
-        <v>38167.46125496718</v>
-      </c>
+      <c r="P18" s="3"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -11673,16 +11814,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="K19" s="3">
-        <v>47706.269455917864</v>
-      </c>
+      <c r="K19" s="3"/>
       <c r="O19" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="P19" s="3">
-        <v>55919.680124425278</v>
-      </c>
+      <c r="P19" s="3"/>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -11699,16 +11836,12 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="K20" s="3">
-        <v>55071.717099396141</v>
-      </c>
+      <c r="K20" s="3"/>
       <c r="O20" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="P20" s="3">
-        <v>35008.584443794243</v>
-      </c>
+      <c r="P20" s="3"/>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -11725,16 +11858,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="K21" s="3">
-        <v>42209.511441545903</v>
-      </c>
+      <c r="K21" s="3"/>
       <c r="O21" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="P21" s="3">
-        <v>43544.710408757492</v>
-      </c>
+      <c r="P21" s="3"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -11751,16 +11880,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="K22" s="3">
-        <v>49682.020270289853</v>
-      </c>
+      <c r="K22" s="3"/>
       <c r="O22" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="P22" s="3">
-        <v>48046.159090094123</v>
-      </c>
+      <c r="P22" s="3"/>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -11777,16 +11902,12 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="K23" s="3">
-        <v>49311.683922463752</v>
-      </c>
+      <c r="K23" s="3"/>
       <c r="O23" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="P23" s="3">
-        <v>48669.792198569798</v>
-      </c>
+      <c r="P23" s="3"/>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -11803,16 +11924,12 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="K24" s="3">
-        <v>39064.704778140083</v>
-      </c>
+      <c r="K24" s="3"/>
       <c r="O24" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="P24" s="3">
-        <v>50289.550007839753</v>
-      </c>
+      <c r="P24" s="3"/>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -11829,16 +11946,12 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="K25" s="3">
-        <v>41983.070560990323</v>
-      </c>
+      <c r="K25" s="3"/>
       <c r="O25" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P25" s="3">
-        <v>60817.454827383262</v>
-      </c>
+      <c r="P25" s="3"/>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -11855,16 +11968,12 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="K26" s="3">
-        <v>56149.619405072437</v>
-      </c>
+      <c r="K26" s="3"/>
       <c r="O26" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="P26" s="3">
-        <v>42204.776910945322</v>
-      </c>
+      <c r="P26" s="3"/>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -11881,16 +11990,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="K27" s="3">
-        <v>43317.098553502386</v>
-      </c>
+      <c r="K27" s="3"/>
       <c r="O27" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="P27" s="3">
-        <v>46342.243827842372</v>
-      </c>
+      <c r="P27" s="3"/>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -11907,16 +12012,12 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="K28" s="3">
-        <v>47764.68925603864</v>
-      </c>
+      <c r="K28" s="3"/>
       <c r="O28" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="P28" s="3">
-        <v>47142.793646105951</v>
-      </c>
+      <c r="P28" s="3"/>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
@@ -11933,16 +12034,12 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="K29" s="3">
-        <v>47005.041559057943</v>
-      </c>
+      <c r="K29" s="3"/>
       <c r="O29" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="P29" s="3">
-        <v>50337.450980638983</v>
-      </c>
+      <c r="P29" s="3"/>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
@@ -11959,16 +12056,12 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="K30" s="3">
-        <v>51930.882647584527</v>
-      </c>
+      <c r="K30" s="3"/>
       <c r="O30" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="P30" s="3">
-        <v>40127.910379273548</v>
-      </c>
+      <c r="P30" s="3"/>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
@@ -11985,16 +12078,12 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="K31" s="3">
-        <v>54694.252778985508</v>
-      </c>
+      <c r="K31" s="3"/>
       <c r="O31" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="P31" s="3">
-        <v>48037.636582938037</v>
-      </c>
+      <c r="P31" s="3"/>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
@@ -12011,16 +12100,12 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="K32" s="3">
-        <v>44476.25490277775</v>
-      </c>
+      <c r="K32" s="3"/>
       <c r="O32" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="P32" s="3">
-        <v>40658.443962036399</v>
-      </c>
+      <c r="P32" s="3"/>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
@@ -12037,16 +12122,12 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="K33" s="3">
-        <v>45825.90305362318</v>
-      </c>
+      <c r="K33" s="3"/>
       <c r="O33" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="P33" s="3">
-        <v>48095.118633339021</v>
-      </c>
+      <c r="P33" s="3"/>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
@@ -12063,16 +12144,12 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="K34" s="3">
-        <v>40826.333127173893</v>
-      </c>
+      <c r="K34" s="3"/>
       <c r="O34" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="P34" s="3">
-        <v>43738.795843558997</v>
-      </c>
+      <c r="P34" s="3"/>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
@@ -12089,16 +12166,12 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="K35" s="3">
-        <v>43269.059705555548</v>
-      </c>
+      <c r="K35" s="3"/>
       <c r="O35" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="P35" s="3">
-        <v>38232.851050016987</v>
-      </c>
+      <c r="P35" s="3"/>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
@@ -12115,16 +12188,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="K36" s="3">
-        <v>48590.220545289849</v>
-      </c>
+      <c r="K36" s="3"/>
       <c r="O36" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="P36" s="3">
-        <v>43530.890776404507</v>
-      </c>
+      <c r="P36" s="3"/>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
@@ -12141,16 +12210,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="K37" s="3">
-        <v>50665.984278019299</v>
-      </c>
+      <c r="K37" s="3"/>
       <c r="O37" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="P37" s="3">
-        <v>41049.915703464721</v>
-      </c>
+      <c r="P37" s="3"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
@@ -12167,16 +12232,12 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="K38" s="3">
-        <v>43188.038527777768</v>
-      </c>
+      <c r="K38" s="3"/>
       <c r="O38" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="P38" s="3">
-        <v>42807.43649225837</v>
-      </c>
+      <c r="P38" s="3"/>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
@@ -12193,16 +12254,12 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="K39" s="3">
-        <v>46723.236136352643</v>
-      </c>
+      <c r="K39" s="3"/>
       <c r="O39" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="P39" s="3">
-        <v>37022.076416313917</v>
-      </c>
+      <c r="P39" s="3"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
@@ -12219,16 +12276,12 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="K40" s="3">
-        <v>41983.045774879211</v>
-      </c>
+      <c r="K40" s="3"/>
       <c r="O40" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="P40" s="3">
-        <v>46372.431892333218</v>
-      </c>
+      <c r="P40" s="3"/>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
@@ -12245,16 +12298,12 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="K41" s="3">
-        <v>44475.251282367128</v>
-      </c>
+      <c r="K41" s="3"/>
       <c r="O41" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="P41" s="3">
-        <v>37394.644561750858</v>
-      </c>
+      <c r="P41" s="3"/>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
@@ -12271,16 +12320,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="K42" s="3">
-        <v>43919.014241908197</v>
-      </c>
+      <c r="K42" s="3"/>
       <c r="O42" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="P42" s="3">
-        <v>42989.305727892373</v>
-      </c>
+      <c r="P42" s="3"/>
     </row>
     <row r="43" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
@@ -12297,16 +12342,12 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="K43" s="3">
-        <v>49965.224176690812</v>
-      </c>
+      <c r="K43" s="3"/>
       <c r="O43" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="P43" s="3">
-        <v>59114.40698198069</v>
-      </c>
+      <c r="P43" s="3"/>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
@@ -12323,16 +12364,12 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K44" s="3">
-        <v>45448.302644082098</v>
-      </c>
+      <c r="K44" s="3"/>
       <c r="O44" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P44" s="3">
-        <v>42599.521412786933</v>
-      </c>
+      <c r="P44" s="3"/>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
@@ -12349,16 +12386,12 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="K45" s="3">
-        <v>57046.581365096623</v>
-      </c>
+      <c r="K45" s="3"/>
       <c r="O45" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="P45" s="3">
-        <v>44165.999187277339</v>
-      </c>
+      <c r="P45" s="3"/>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
@@ -12375,16 +12408,12 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="K46" s="3">
-        <v>51849.101043236718</v>
-      </c>
+      <c r="K46" s="3"/>
       <c r="O46" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="P46" s="3">
-        <v>43993.52235304963</v>
-      </c>
+      <c r="P46" s="3"/>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
@@ -12401,16 +12430,12 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="K47" s="3">
-        <v>47776.05933115942</v>
-      </c>
+      <c r="K47" s="3"/>
       <c r="O47" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="P47" s="3">
-        <v>38780.100139815353</v>
-      </c>
+      <c r="P47" s="3"/>
     </row>
     <row r="48" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
@@ -12427,16 +12452,12 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="K48" s="3">
-        <v>63866.519510024162</v>
-      </c>
+      <c r="K48" s="3"/>
       <c r="O48" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="P48" s="3">
-        <v>54017.109314865571</v>
-      </c>
+      <c r="P48" s="3"/>
     </row>
     <row r="49" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
@@ -12453,16 +12474,12 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="K49" s="3">
-        <v>50267.479442874377</v>
-      </c>
+      <c r="K49" s="3"/>
       <c r="O49" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="P49" s="3">
-        <v>47912.575040021628</v>
-      </c>
+      <c r="P49" s="3"/>
     </row>
     <row r="50" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
@@ -12479,16 +12496,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="K50" s="3">
-        <v>48853.398831521707</v>
-      </c>
+      <c r="K50" s="3"/>
       <c r="O50" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="P50" s="3">
-        <v>43434.446787438843</v>
-      </c>
+      <c r="P50" s="3"/>
     </row>
     <row r="51" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
@@ -12505,16 +12518,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="K51" s="3">
-        <v>53105.532463888892</v>
-      </c>
+      <c r="K51" s="3"/>
       <c r="O51" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="P51" s="3">
-        <v>40703.061288956553</v>
-      </c>
+      <c r="P51" s="3"/>
     </row>
     <row r="52" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
@@ -12531,16 +12540,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="K52" s="3">
-        <v>40680.08984927534</v>
-      </c>
+      <c r="K52" s="3"/>
       <c r="O52" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="P52" s="3">
-        <v>55575.226855439301</v>
-      </c>
+      <c r="P52" s="3"/>
     </row>
     <row r="53" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
@@ -12557,16 +12562,12 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="K53" s="3">
-        <v>38670.934781763273</v>
-      </c>
+      <c r="K53" s="3"/>
       <c r="O53" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="P53" s="3">
-        <v>42928.353085234281</v>
-      </c>
+      <c r="P53" s="3"/>
     </row>
     <row r="54" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
@@ -12583,16 +12584,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K54" s="3">
-        <v>42767.607619927519</v>
-      </c>
+      <c r="K54" s="3"/>
       <c r="O54" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P54" s="3">
-        <v>47179.19244073861</v>
-      </c>
+      <c r="P54" s="3"/>
     </row>
     <row r="56" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
@@ -12609,16 +12606,16 @@
       <c r="J56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K56" s="3" t="e">
         <f>AVERAGE(K5:K54)</f>
-        <v>47076.26806435507</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P56" s="3">
+      <c r="P56" s="3" t="e">
         <f>AVERAGE(P5:P54)</f>
-        <v>44682.612427997839</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="57" spans="3:16" x14ac:dyDescent="0.25">
@@ -12636,16 +12633,16 @@
       <c r="J57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K57" s="3">
+      <c r="K57" s="3" t="e">
         <f>_xlfn.STDEV.S(K5:K54)</f>
-        <v>5443.0499555306624</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="3">
+      <c r="P57" s="3" t="e">
         <f>_xlfn.STDEV.S(P5:P54)</f>
-        <v>5667.3617182787521</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test-23: extrapol 2.0 & hybrid3 2.0 (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-23.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-23.xlsx
@@ -11456,13 +11456,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="V45" sqref="V45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
@@ -11507,11 +11509,15 @@
       <c r="J5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>97505.714762790682</v>
+      </c>
       <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="3">
+        <v>97249.526480905741</v>
+      </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
@@ -11528,12 +11534,16 @@
         <f>J5+1</f>
         <v>2</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3">
+        <v>97391.868350061181</v>
+      </c>
       <c r="O6" s="2">
         <f>O5+1</f>
         <v>2</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="3">
+        <v>78548.746614810269</v>
+      </c>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -11550,12 +11560,16 @@
         <f t="shared" ref="J7:J54" si="1">J6+1</f>
         <v>3</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>107150.3802609547</v>
+      </c>
       <c r="O7" s="2">
         <f t="shared" ref="O7:O54" si="2">O6+1</f>
         <v>3</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="3">
+        <v>81115.498075887386</v>
+      </c>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -11572,12 +11586,16 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>82607.412100734407</v>
+      </c>
       <c r="O8" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="3">
+        <v>80880.733705140752</v>
+      </c>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -11594,12 +11612,16 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>92551.962875152996</v>
+      </c>
       <c r="O9" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="3">
+        <v>88387.025123255822</v>
+      </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -11616,12 +11638,16 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="3">
+        <v>82721.72344369645</v>
+      </c>
       <c r="O10" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P10" s="3"/>
+      <c r="P10" s="3">
+        <v>83042.990164871473</v>
+      </c>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -11638,12 +11664,16 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3">
+        <v>102206.4837348837</v>
+      </c>
       <c r="O11" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="P11" s="3"/>
+      <c r="P11" s="3">
+        <v>82050.116771970614</v>
+      </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -11660,12 +11690,16 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="3">
+        <v>87344.492795348822</v>
+      </c>
       <c r="O12" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="P12" s="3"/>
+      <c r="P12" s="3">
+        <v>84624.566461444309</v>
+      </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -11682,12 +11716,16 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3">
+        <v>83742.228321664603</v>
+      </c>
       <c r="O13" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="P13" s="3">
+        <v>104300.0243080783</v>
+      </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -11704,12 +11742,16 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="3">
+        <v>104475.83710134641</v>
+      </c>
       <c r="O14" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="P14" s="3"/>
+      <c r="P14" s="3">
+        <v>80667.723119339047</v>
+      </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -11726,12 +11768,16 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="K15" s="3"/>
+      <c r="K15" s="3">
+        <v>87194.811403304775</v>
+      </c>
       <c r="O15" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P15" s="3"/>
+      <c r="P15" s="3">
+        <v>96237.263360709898</v>
+      </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -11748,12 +11794,16 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3">
+        <v>89286.856252509169</v>
+      </c>
       <c r="O16" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="P16" s="3"/>
+      <c r="P16" s="3">
+        <v>86121.93094039167</v>
+      </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -11770,12 +11820,16 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3">
+        <v>89107.413994981631</v>
+      </c>
       <c r="O17" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="P17" s="3"/>
+      <c r="P17" s="3">
+        <v>83874.836241248457</v>
+      </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -11792,12 +11846,16 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="K18" s="3"/>
+      <c r="K18" s="3">
+        <v>91393.715976744177</v>
+      </c>
       <c r="O18" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="P18" s="3"/>
+      <c r="P18" s="3">
+        <v>85578.378965850672</v>
+      </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -11814,12 +11872,16 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="K19" s="3"/>
+      <c r="K19" s="3">
+        <v>103321.5476397797</v>
+      </c>
       <c r="O19" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="P19" s="3"/>
+      <c r="P19" s="3">
+        <v>87821.554435618105</v>
+      </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -11836,12 +11898,16 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3">
+        <v>80308.809951529984</v>
+      </c>
       <c r="O20" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="P20" s="3"/>
+      <c r="P20" s="3">
+        <v>89165.804376621774</v>
+      </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -11858,12 +11924,16 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="K21" s="3"/>
+      <c r="K21" s="3">
+        <v>72118.470334761325</v>
+      </c>
       <c r="O21" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="P21" s="3"/>
+      <c r="P21" s="3">
+        <v>94742.860203304779</v>
+      </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -11880,12 +11950,16 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3">
+        <v>103609.1791730722</v>
+      </c>
       <c r="O22" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="P22" s="3">
+        <v>72041.439153733168</v>
+      </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -11902,12 +11976,16 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3">
+        <v>92727.942221664634</v>
+      </c>
       <c r="O23" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="P23" s="3"/>
+      <c r="P23" s="3">
+        <v>78759.266331334133</v>
+      </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -11924,12 +12002,16 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <v>87004.955337821273</v>
+      </c>
       <c r="O24" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="P24" s="3"/>
+      <c r="P24" s="3">
+        <v>95574.872751897172</v>
+      </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -11946,12 +12028,16 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="K25" s="3"/>
+      <c r="K25" s="3">
+        <v>84090.501052264372</v>
+      </c>
       <c r="O25" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P25" s="3"/>
+      <c r="P25" s="3">
+        <v>77014.386386291299</v>
+      </c>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -11968,12 +12054,16 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="K26" s="3"/>
+      <c r="K26" s="3">
+        <v>84970.028297184806</v>
+      </c>
       <c r="O26" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="P26" s="3">
+        <v>93054.168052631576</v>
+      </c>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -11990,12 +12080,16 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="K27" s="3"/>
+      <c r="K27" s="3">
+        <v>93954.534851652366</v>
+      </c>
       <c r="O27" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="P27" s="3"/>
+      <c r="P27" s="3">
+        <v>94663.463553121182</v>
+      </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -12012,12 +12106,16 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="K28" s="3"/>
+      <c r="K28" s="3">
+        <v>88213.385052753962</v>
+      </c>
       <c r="O28" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="P28" s="3"/>
+      <c r="P28" s="3">
+        <v>80138.179235006115</v>
+      </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
@@ -12034,12 +12132,16 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="K29" s="3"/>
+      <c r="K29" s="3">
+        <v>97544.262790697685</v>
+      </c>
       <c r="O29" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="P29" s="3"/>
+      <c r="P29" s="3">
+        <v>89454.138774785781</v>
+      </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
@@ -12056,12 +12158,16 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="K30" s="3"/>
+      <c r="K30" s="3">
+        <v>87958.745657282736</v>
+      </c>
       <c r="O30" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="P30" s="3"/>
+      <c r="P30" s="3">
+        <v>72150.426653610775</v>
+      </c>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
@@ -12078,12 +12184,16 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="K31" s="3"/>
+      <c r="K31" s="3">
+        <v>96007.633729498164</v>
+      </c>
       <c r="O31" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="P31" s="3"/>
+      <c r="P31" s="3">
+        <v>90690.874816768643</v>
+      </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
@@ -12100,12 +12210,16 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="K32" s="3"/>
+      <c r="K32" s="3">
+        <v>74649.246682496916</v>
+      </c>
       <c r="O32" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="P32" s="3"/>
+      <c r="P32" s="3">
+        <v>85887.11223341494</v>
+      </c>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
@@ -12122,12 +12236,16 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="K33" s="3"/>
+      <c r="K33" s="3">
+        <v>90396.302598408802</v>
+      </c>
       <c r="O33" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="P33" s="3"/>
+      <c r="P33" s="3">
+        <v>68118.509080905758</v>
+      </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
@@ -12144,12 +12262,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="K34" s="3"/>
+      <c r="K34" s="3">
+        <v>84908.145806609522</v>
+      </c>
       <c r="O34" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="P34" s="3"/>
+      <c r="P34" s="3">
+        <v>98749.744679559371</v>
+      </c>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
@@ -12166,12 +12288,16 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="K35" s="3"/>
+      <c r="K35" s="3">
+        <v>117772.2593356181</v>
+      </c>
       <c r="O35" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="P35" s="3"/>
+      <c r="P35" s="3">
+        <v>95859.72477123623</v>
+      </c>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
@@ -12188,12 +12314,16 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="K36" s="3"/>
+      <c r="K36" s="3">
+        <v>78622.491770624227</v>
+      </c>
       <c r="O36" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="P36" s="3"/>
+      <c r="P36" s="3">
+        <v>71606.475465728276</v>
+      </c>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
@@ -12210,12 +12340,16 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="K37" s="3"/>
+      <c r="K37" s="3">
+        <v>106037.3946949816</v>
+      </c>
       <c r="O37" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="P37" s="3"/>
+      <c r="P37" s="3">
+        <v>89715.730296572816</v>
+      </c>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
@@ -12232,12 +12366,16 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="K38" s="3"/>
+      <c r="K38" s="3">
+        <v>84587.503971113823</v>
+      </c>
       <c r="O38" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="P38" s="3"/>
+      <c r="P38" s="3">
+        <v>90647.304252019589</v>
+      </c>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
@@ -12254,12 +12392,16 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="K39" s="3"/>
+      <c r="K39" s="3">
+        <v>91582.478769033012</v>
+      </c>
       <c r="O39" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="P39" s="3"/>
+      <c r="P39" s="3">
+        <v>67584.314030477341</v>
+      </c>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
@@ -12276,12 +12418,16 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="K40" s="3"/>
+      <c r="K40" s="3">
+        <v>84789.030697552022</v>
+      </c>
       <c r="O40" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="P40" s="3"/>
+      <c r="P40" s="3">
+        <v>81921.458703182361</v>
+      </c>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
@@ -12298,12 +12444,16 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="K41" s="3"/>
+      <c r="K41" s="3">
+        <v>86562.352121664619</v>
+      </c>
       <c r="O41" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="P41" s="3"/>
+      <c r="P41" s="3">
+        <v>89700.619584577697</v>
+      </c>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
@@ -12320,12 +12470,16 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="K42" s="3"/>
+      <c r="K42" s="3">
+        <v>100049.0954356181</v>
+      </c>
       <c r="O42" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="P42" s="3"/>
+      <c r="P42" s="3">
+        <v>88660.380602203179</v>
+      </c>
     </row>
     <row r="43" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
@@ -12342,12 +12496,16 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="K43" s="3"/>
+      <c r="K43" s="3">
+        <v>106457.3437903305</v>
+      </c>
       <c r="O43" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="P43" s="3"/>
+      <c r="P43" s="3">
+        <v>85589.857345165234</v>
+      </c>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
@@ -12364,12 +12522,16 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K44" s="3"/>
+      <c r="K44" s="3">
+        <v>91419.526717625457</v>
+      </c>
       <c r="O44" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P44" s="3"/>
+      <c r="P44" s="3">
+        <v>77261.478046389224</v>
+      </c>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
@@ -12386,12 +12548,16 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="K45" s="3"/>
+      <c r="K45" s="3">
+        <v>91011.98656646267</v>
+      </c>
       <c r="O45" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="P45" s="3"/>
+      <c r="P45" s="3">
+        <v>93607.082694369645</v>
+      </c>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
@@ -12408,12 +12574,16 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="K46" s="3"/>
+      <c r="K46" s="3">
+        <v>106835.6968168911</v>
+      </c>
       <c r="O46" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="P46" s="3"/>
+      <c r="P46" s="3">
+        <v>87619.254756303533</v>
+      </c>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
@@ -12430,12 +12600,16 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="K47" s="3"/>
+      <c r="K47" s="3">
+        <v>90217.921144430831</v>
+      </c>
       <c r="O47" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="P47" s="3"/>
+      <c r="P47" s="3">
+        <v>101372.9401408813</v>
+      </c>
     </row>
     <row r="48" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
@@ -12452,12 +12626,16 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="K48" s="3"/>
+      <c r="K48" s="3">
+        <v>87243.938466095467</v>
+      </c>
       <c r="O48" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="P48" s="3"/>
+      <c r="P48" s="3">
+        <v>94505.361277845761</v>
+      </c>
     </row>
     <row r="49" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
@@ -12474,12 +12652,16 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="K49" s="3"/>
+      <c r="K49" s="3">
+        <v>94457.17440697673</v>
+      </c>
       <c r="O49" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="P49" s="3"/>
+      <c r="P49" s="3">
+        <v>84143.758284088122</v>
+      </c>
     </row>
     <row r="50" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
@@ -12496,12 +12678,16 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="K50" s="3"/>
+      <c r="K50" s="3">
+        <v>91582.329269767433</v>
+      </c>
       <c r="O50" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="P50" s="3"/>
+      <c r="P50" s="3">
+        <v>96352.754174296191</v>
+      </c>
     </row>
     <row r="51" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
@@ -12518,12 +12704,16 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="K51" s="3"/>
+      <c r="K51" s="3">
+        <v>87569.278293023235</v>
+      </c>
       <c r="O51" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="P51" s="3"/>
+      <c r="P51" s="3">
+        <v>88124.540556058739</v>
+      </c>
     </row>
     <row r="52" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
@@ -12540,12 +12730,16 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="K52" s="3"/>
+      <c r="K52" s="3">
+        <v>84722.701322154215</v>
+      </c>
       <c r="O52" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="P52" s="3"/>
+      <c r="P52" s="3">
+        <v>81590.952621664619</v>
+      </c>
     </row>
     <row r="53" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
@@ -12562,12 +12756,16 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="K53" s="3"/>
+      <c r="K53" s="3">
+        <v>78730.575311015898</v>
+      </c>
       <c r="O53" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="P53" s="3"/>
+      <c r="P53" s="3">
+        <v>98547.61101664626</v>
+      </c>
     </row>
     <row r="54" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
@@ -12584,12 +12782,16 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K54" s="3"/>
+      <c r="K54" s="3">
+        <v>101609.2402314565</v>
+      </c>
       <c r="O54" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P54" s="3"/>
+      <c r="P54" s="3">
+        <v>86863.704526560585</v>
+      </c>
     </row>
     <row r="56" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
@@ -12606,16 +12808,16 @@
       <c r="J56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K56" s="3" t="e">
+      <c r="K56" s="3">
         <f>AVERAGE(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>91566.498233681748</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P56" s="3" t="e">
+      <c r="P56" s="3">
         <f>AVERAGE(P5:P54)</f>
-        <v>#DIV/0!</v>
+        <v>86639.629283975519</v>
       </c>
     </row>
     <row r="57" spans="3:16" x14ac:dyDescent="0.25">
@@ -12633,16 +12835,16 @@
       <c r="J57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K57" s="3" t="e">
+      <c r="K57" s="3">
         <f>_xlfn.STDEV.S(K5:K54)</f>
-        <v>#DIV/0!</v>
+        <v>9319.3982926204935</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="3" t="e">
+      <c r="P57" s="3">
         <f>_xlfn.STDEV.S(P5:P54)</f>
-        <v>#DIV/0!</v>
+        <v>8509.2391157804832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>